<commit_message>
Achievements for the first visit to Port Royal added
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="265">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -590,6 +590,72 @@
     <t xml:space="preserve">Waterway</t>
   </si>
   <si>
+    <t xml:space="preserve">PortRockFace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isla de Muerta: Rock Face</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortCaveMouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isla de Muerta: Cave Mouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortHarbor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harbor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortRampart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rampart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortInterceptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Interceptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortInterceptorHold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Interceptor: Ship’s Hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortInterceptorBattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortInterceptorDualBattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortPowderStore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isla de Muerta: Powder Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortNook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isla de Muerta: Moonlight Nook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortHeap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isla de Muerta: Treasure Heap</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -636,6 +702,12 @@
   </si>
   <si>
     <t xml:space="preserve">Hydra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbossa</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -869,7 +941,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -1163,13 +1235,13 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I60" activeCellId="0" sqref="I60"/>
+      <selection pane="bottomLeft" activeCell="F83" activeCellId="0" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.76"/>
@@ -1205,7 +1277,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 0, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3526,11 +3598,11 @@
         <v>91</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""worldId"": ",C94,", ""name"": """,D94,""", ""display"": """,E94,""", ""areaId"": ",B94,", ""hideWorld"": ",F94,", },")</f>
-        <v>3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 0, },</v>
+        <v>3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,30 +3658,366 @@
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <f aca="false">B97+C97*256</f>
-        <v>0</v>
+        <v>4104</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A97,": { ""worldId"": ",C97,", ""name"": """,D97,""", ""display"": """,E97,""", ""areaId"": ",B97,", ""hideWorld"": ",F97,", },")</f>
+        <v>4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <f aca="false">B98+C98*256</f>
-        <v>0</v>
+        <v>4105</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A98,": { ""worldId"": ",C98,", ""name"": """,D98,""", ""display"": """,E98,""", ""areaId"": ",B98,", ""hideWorld"": ",F98,", },")</f>
+        <v>4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <f aca="false">B99+C99*256</f>
-        <v>0</v>
+        <v>4097</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A99,": { ""worldId"": ",C99,", ""name"": """,D99,""", ""display"": """,E99,""", ""areaId"": ",B99,", ""hideWorld"": ",F99,", },")</f>
+        <v>4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <f aca="false">B100+C100*256</f>
-        <v>0</v>
+        <v>4098</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A100,": { ""worldId"": ",C100,", ""name"": """,D100,""", ""display"": """,E100,""", ""areaId"": ",B100,", ""hideWorld"": ",F100,", },")</f>
+        <v>4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
         <f aca="false">B101+C101*256</f>
+        <v>4096</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A101,": { ""worldId"": ",C101,", ""name"": """,D101,""", ""display"": """,E101,""", ""areaId"": ",B101,", ""hideWorld"": ",F101,", },")</f>
+        <v>4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <f aca="false">B102+C102*256</f>
+        <v>4099</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A102,": { ""worldId"": ",C102,", ""name"": """,D102,""", ""display"": """,E102,""", ""areaId"": ",B102,", ""hideWorld"": ",F102,", },")</f>
+        <v>4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <f aca="false">B103+C103*256</f>
+        <v>4100</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A103,": { ""worldId"": ",C103,", ""name"": """,D103,""", ""display"": """,E103,""", ""areaId"": ",B103,", ""hideWorld"": ",F103,", },")</f>
+        <v>4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <f aca="false">B104+C104*256</f>
+        <v>4117</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A104,": { ""worldId"": ",C104,", ""name"": """,D104,""", ""display"": """,E104,""", ""areaId"": ",B104,", ""hideWorld"": ",F104,", },")</f>
+        <v>4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <f aca="false">B105+C105*256</f>
+        <v>4103</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A105,": { ""worldId"": ",C105,", ""name"": """,D105,""", ""display"": """,E105,""", ""areaId"": ",B105,", ""hideWorld"": ",F105,", },")</f>
+        <v>4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <f aca="false">B106+C106*256</f>
+        <v>4108</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A106,": { ""worldId"": ",C106,", ""name"": """,D106,""", ""display"": """,E106,""", ""areaId"": ",B106,", ""hideWorld"": ",F106,", },")</f>
+        <v>4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <f aca="false">B107+C107*256</f>
+        <v>4109</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A107,": { ""worldId"": ",C107,", ""name"": """,D107,""", ""display"": """,E107,""", ""areaId"": ",B107,", ""hideWorld"": ",F107,", },")</f>
+        <v>4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <f aca="false">B108+C108*256</f>
+        <v>4106</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A108,": { ""worldId"": ",C108,", ""name"": """,D108,""", ""display"": """,E108,""", ""areaId"": ",B108,", ""hideWorld"": ",F108,", },")</f>
+        <v>4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <f aca="false">B109+C109*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <f aca="false">B110+C110*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <f aca="false">B111+C111*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <f aca="false">B112+C112*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <f aca="false">B113+C113*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <f aca="false">B114+C114*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <f aca="false">B115+C115*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <f aca="false">B116+C116*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <f aca="false">B117+C117*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <f aca="false">B118+C118*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <f aca="false">B119+C119*256</f>
         <v>0</v>
       </c>
     </row>
@@ -3634,13 +4042,13 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3650,13 +4058,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -3666,18 +4074,18 @@
       </c>
       <c r="F1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },</v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", },")</f>
@@ -3692,7 +4100,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", },")</f>
@@ -3701,13 +4109,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", },")</f>
@@ -3722,7 +4130,7 @@
         <v>123</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", },")</f>
@@ -3731,13 +4139,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>131</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", },")</f>
@@ -3752,7 +4160,7 @@
         <v>146</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", },")</f>
@@ -3767,7 +4175,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="D8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", },")</f>
@@ -3782,7 +4190,7 @@
         <v>184</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="D9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", },")</f>
@@ -3791,17 +4199,32 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>163</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="D10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", },")</f>
         <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", },")</f>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3829,14 +4252,14 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3860,10 +4283,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -3872,10 +4295,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -3884,10 +4307,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -3896,10 +4319,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -3908,10 +4331,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -3920,10 +4343,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -3932,10 +4355,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -3944,10 +4367,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -3956,10 +4379,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -3968,10 +4391,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -3980,10 +4403,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -4054,7 +4477,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
@@ -4068,25 +4491,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,13 +4563,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4203,16 +4626,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4271,7 +4694,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added locations, registered bosses, and created achievements for the first visit to Halloween Town
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="286">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -701,6 +701,18 @@
     <t xml:space="preserve">Christmas Town: Santa’s House</t>
   </si>
   <si>
+    <t xml:space="preserve">HalloweenHill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curly Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HalloweenFactory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas Town: Toy Factory: Shipping and Receiving</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -753,6 +765,12 @@
   </si>
   <si>
     <t xml:space="preserve">Barbossa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Keeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oogie Boogie</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -982,11 +1000,11 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -1286,10 +1304,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G115" activeCellId="0" sqref="G115"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.76"/>
@@ -1325,7 +1343,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4181,13 +4199,51 @@
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <f aca="false">B116+C116*256</f>
-        <v>0</v>
+        <v>3587</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A116,": { ""worldId"": ",C116,", ""name"": """,D116,""", ""display"": """,E116,""", ""areaId"": ",B116,", ""hideWorld"": ",F116,", },")</f>
+        <v>3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <f aca="false">B117+C117*256</f>
-        <v>0</v>
+        <v>3593</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A117,": { ""worldId"": ",C117,", ""name"": """,D117,""", ""display"": """,E117,""", ""areaId"": ",B117,", ""hideWorld"": ",F117,", },")</f>
+        <v>3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4223,13 +4279,13 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -4239,13 +4295,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4255,18 +4311,18 @@
       </c>
       <c r="F1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },</v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", },")</f>
@@ -4281,7 +4337,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", },")</f>
@@ -4290,13 +4346,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", },")</f>
@@ -4311,7 +4367,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", },")</f>
@@ -4320,13 +4376,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", },")</f>
@@ -4341,7 +4397,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", },")</f>
@@ -4356,7 +4412,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", },")</f>
@@ -4371,7 +4427,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", },")</f>
@@ -4380,13 +4436,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", },")</f>
@@ -4395,17 +4451,47 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", },")</f>
         <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", },")</f>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", },")</f>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,14 +4519,14 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -4464,10 +4550,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -4476,10 +4562,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -4488,10 +4574,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -4500,10 +4586,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -4512,10 +4598,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -4524,10 +4610,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -4536,10 +4622,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -4548,10 +4634,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -4560,10 +4646,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -4572,10 +4658,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -4584,10 +4670,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -4658,7 +4744,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
@@ -4672,25 +4758,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4744,13 +4830,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4807,16 +4893,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,7 +4961,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added all achievements up to the end of Agrabah I
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="306">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -713,6 +713,60 @@
     <t xml:space="preserve">Christmas Town: Toy Factory: Shipping and Receiving</t>
   </si>
   <si>
+    <t xml:space="preserve">AgrabahShop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Peddler’s Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahBazaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bazaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahWalls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palace Walls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveEntrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cave of Wonders: Entrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveValley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cave of Wonders: Valley of Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveGuardians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cave of Wonders: Stone Guardians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveChasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cave of Wonders: Chasm of Challenges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveTreasure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cave of Wonders: Treasure Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahPalace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Palace</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -771,6 +825,12 @@
   </si>
   <si>
     <t xml:space="preserve">Oogie Boogie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volcano and Blizzard</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1004,7 +1064,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -1299,15 +1359,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="E140" activeCellId="0" sqref="E140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.76"/>
@@ -1343,7 +1403,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,17 +4309,415 @@
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <f aca="false">B118+C118*256</f>
-        <v>0</v>
+        <v>1794</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G118" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A118,": { ""worldId"": ",C118,", ""name"": """,D118,""", ""display"": """,E118,""", ""areaId"": ",B118,", ""hideWorld"": ",F118,", },")</f>
+        <v>1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <f aca="false">B119+C119*256</f>
+        <v>1792</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G119" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A119,": { ""worldId"": ",C119,", ""name"": """,D119,""", ""display"": """,E119,""", ""areaId"": ",B119,", ""hideWorld"": ",F119,", },")</f>
+        <v>1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <f aca="false">B120+C120*256</f>
+        <v>1793</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A120,": { ""worldId"": ",C120,", ""name"": """,D120,""", ""display"": """,E120,""", ""areaId"": ",B120,", ""hideWorld"": ",F120,", },")</f>
+        <v>1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <f aca="false">B121+C121*256</f>
+        <v>1798</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A121,": { ""worldId"": ",C121,", ""name"": """,D121,""", ""display"": """,E121,""", ""areaId"": ",B121,", ""hideWorld"": ",F121,", },")</f>
+        <v>1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <f aca="false">B122+C122*256</f>
+        <v>1799</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A122,": { ""worldId"": ",C122,", ""name"": """,D122,""", ""display"": """,E122,""", ""areaId"": ",B122,", ""hideWorld"": ",F122,", },")</f>
+        <v>1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <f aca="false">B123+C123*256</f>
+        <v>1804</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G123" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A123,": { ""worldId"": ",C123,", ""name"": """,D123,""", ""display"": """,E123,""", ""areaId"": ",B123,", ""hideWorld"": ",F123,", },")</f>
+        <v>1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <f aca="false">B124+C124*256</f>
+        <v>1801</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A124,": { ""worldId"": ",C124,", ""name"": """,D124,""", ""display"": """,E124,""", ""areaId"": ",B124,", ""hideWorld"": ",F124,", },")</f>
+        <v>1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <f aca="false">B125+C125*256</f>
+        <v>1805</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A125,": { ""worldId"": ",C125,", ""name"": """,D125,""", ""display"": """,E125,""", ""areaId"": ",B125,", ""hideWorld"": ",F125,", },")</f>
+        <v>1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <f aca="false">B126+C126*256</f>
+        <v>1802</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A126,": { ""worldId"": ",C126,", ""name"": """,D126,""", ""display"": """,E126,""", ""areaId"": ",B126,", ""hideWorld"": ",F126,", },")</f>
+        <v>1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <f aca="false">B127+C127*256</f>
+        <v>1795</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="F127" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A127,": { ""worldId"": ",C127,", ""name"": """,D127,""", ""display"": """,E127,""", ""areaId"": ",B127,", ""hideWorld"": ",F127,", },")</f>
+        <v>1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <f aca="false">B128+C128*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <f aca="false">B129+C129*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <f aca="false">B130+C130*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <f aca="false">B131+C131*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <f aca="false">B132+C132*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <f aca="false">B133+C133*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <f aca="false">B134+C134*256</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <f aca="false">B135+C135*256</f>
+        <v>0</v>
+      </c>
       <c r="D135" s="2"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <f aca="false">B136+C136*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <f aca="false">B137+C137*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <f aca="false">B138+C138*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <f aca="false">B139+C139*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <f aca="false">B140+C140*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <f aca="false">B141+C141*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <f aca="false">B142+C142*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <f aca="false">B143+C143*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <f aca="false">B144+C144*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <f aca="false">B145+C145*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="n">
+        <f aca="false">B146+C146*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="n">
+        <f aca="false">B147+C147*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="n">
+        <f aca="false">B148+C148*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="n">
+        <f aca="false">B149+C149*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="n">
+        <f aca="false">B150+C150*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="n">
+        <f aca="false">B151+C151*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="n">
+        <f aca="false">B152+C152*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="n">
+        <f aca="false">B153+C153*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="n">
+        <f aca="false">B154+C154*256</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4279,13 +4737,13 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -4295,13 +4753,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4311,18 +4769,18 @@
       </c>
       <c r="F1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },</v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", },")</f>
@@ -4337,7 +4795,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", },")</f>
@@ -4346,13 +4804,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", },")</f>
@@ -4367,7 +4825,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", },")</f>
@@ -4376,13 +4834,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", },")</f>
@@ -4397,7 +4855,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", },")</f>
@@ -4412,7 +4870,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="D8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", },")</f>
@@ -4427,7 +4885,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="D9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", },")</f>
@@ -4436,13 +4894,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="D10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", },")</f>
@@ -4451,13 +4909,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="D11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", },")</f>
@@ -4472,7 +4930,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="D12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", },")</f>
@@ -4487,11 +4945,26 @@
         <v>227</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", },")</f>
         <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", },")</f>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, },</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4519,14 +4992,14 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -4550,10 +5023,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -4562,10 +5035,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -4574,10 +5047,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -4586,10 +5059,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -4598,10 +5071,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -4610,10 +5083,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -4622,10 +5095,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -4634,10 +5107,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -4646,10 +5119,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -4658,10 +5131,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -4670,10 +5143,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -4744,7 +5217,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
@@ -4758,25 +5231,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,13 +5303,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,16 +5366,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4961,7 +5434,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Slightly refactored "Dull Claws" to use a boss registration
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="332">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -834,6 +834,12 @@
   </si>
   <si>
     <t xml:space="preserve">PridePeakBattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ColiseumTourney1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Underdrome</t>
   </si>
   <si>
     <t xml:space="preserve">Event ID</t>
@@ -1437,10 +1443,10 @@
   </sheetPr>
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
+      <selection pane="bottomLeft" activeCell="G140" activeCellId="0" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1479,7 +1485,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,7 +4941,26 @@
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
         <f aca="false">B140+C140*256</f>
-        <v>0</v>
+        <v>1545</v>
+      </c>
+      <c r="B140" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C140" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F140" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A140,": { ""worldId"": ",C140,", ""name"": """,D140,""", ""display"": """,E140,""", ""areaId"": ",B140,", ""hideWorld"": ",F140,", },")</f>
+        <v>1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5040,7 +5065,7 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
@@ -5056,13 +5081,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5077,13 +5102,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", },")</f>
@@ -5098,7 +5123,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", },")</f>
@@ -5107,13 +5132,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", },")</f>
@@ -5128,7 +5153,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", },")</f>
@@ -5137,13 +5162,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", },")</f>
@@ -5158,7 +5183,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", },")</f>
@@ -5173,7 +5198,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", },")</f>
@@ -5188,7 +5213,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", },")</f>
@@ -5197,13 +5222,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", },")</f>
@@ -5212,13 +5237,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", },")</f>
@@ -5233,7 +5258,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", },")</f>
@@ -5248,7 +5273,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", },")</f>
@@ -5257,13 +5282,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", },")</f>
@@ -5278,7 +5303,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", },")</f>
@@ -5317,7 +5342,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5341,10 +5366,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -5353,10 +5378,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -5365,10 +5390,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -5377,10 +5402,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -5389,10 +5414,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -5401,10 +5426,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -5413,10 +5438,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -5425,10 +5450,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -5437,10 +5462,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -5449,10 +5474,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -5461,10 +5486,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -5549,25 +5574,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5621,13 +5646,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5684,16 +5709,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5752,7 +5777,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Improved robustness of the event register
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Bosses" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Events" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Animations" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Stats - Terra" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="334">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -848,7 +848,13 @@
     <t xml:space="preserve">Location Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Boss ID</t>
+    <t xml:space="preserve">Event Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Boss?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score</t>
   </si>
   <si>
     <t xml:space="preserve">9d</t>
@@ -1102,7 +1108,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1116,6 +1122,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1443,7 +1457,7 @@
   </sheetPr>
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G140" activeCellId="0" sqref="G140"/>
@@ -5063,12 +5077,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5089,30 +5103,44 @@
       <c r="C1" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="0"/>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(D2:D1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, },</v>
+      <c r="I1" s="5" t="str">
+        <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", },")</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, },</v>
+        <v>278</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2," }, ")</f>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5 }, </v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5123,26 +5151,40 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", },")</f>
-        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, },</v>
+        <v>279</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0"/>
+      <c r="G3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3," }, ")</f>
+        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5 }, </v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", },")</f>
-        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, },</v>
+        <v>281</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0"/>
+      <c r="G4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4," }, ")</f>
+        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10 }, </v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5153,26 +5195,40 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", },")</f>
-        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, },</v>
+        <v>282</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0"/>
+      <c r="G5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5," }, ")</f>
+        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10 }, </v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", },")</f>
-        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, },</v>
+        <v>284</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0"/>
+      <c r="G6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6," }, ")</f>
+        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10 }, </v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5183,11 +5239,18 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", },")</f>
-        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, },</v>
+        <v>285</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0"/>
+      <c r="G7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7," }, ")</f>
+        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10 }, </v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5198,11 +5261,18 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", },")</f>
-        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, },</v>
+        <v>286</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="0"/>
+      <c r="G8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8," }, ")</f>
+        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5 }, </v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5213,41 +5283,62 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", },")</f>
-        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, },</v>
+        <v>287</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0"/>
+      <c r="G9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9," }, ")</f>
+        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10 }, </v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", },")</f>
-        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, },</v>
+        <v>289</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0"/>
+      <c r="G10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10," }, ")</f>
+        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10 }, </v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", },")</f>
-        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, },</v>
+        <v>291</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F11" s="0"/>
+      <c r="G11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11," }, ")</f>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25 }, </v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5258,11 +5349,18 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", },")</f>
-        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, },</v>
+        <v>292</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0"/>
+      <c r="G12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12," }, ")</f>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10 }, </v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5273,26 +5371,40 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", },")</f>
-        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, },</v>
+        <v>293</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0"/>
+      <c r="G13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13," }, ")</f>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10 }, </v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", },")</f>
-        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, },</v>
+        <v>295</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" s="0"/>
+      <c r="G14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14," }, ")</f>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5 }, </v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5303,11 +5415,18 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", },")</f>
-        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, },</v>
+        <v>296</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F15" s="0"/>
+      <c r="G15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15," }, ")</f>
+        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5342,7 +5461,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5366,10 +5485,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -5378,10 +5497,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -5390,10 +5509,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -5402,10 +5521,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -5414,10 +5533,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -5426,10 +5545,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -5438,10 +5557,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -5450,10 +5569,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -5462,10 +5581,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -5474,10 +5593,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -5486,10 +5605,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -5574,25 +5693,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5646,13 +5765,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5668,15 +5787,15 @@
       <c r="D5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="6" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
         <v>29</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="6" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
         <v>25</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="6" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
         <v>24</v>
       </c>
@@ -5709,16 +5828,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5777,7 +5896,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Further improved the robustness of the event registry
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="336">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -915,6 +915,12 @@
   </si>
   <si>
     <t xml:space="preserve">Scar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain and Panic Cup</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1460,7 +1466,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G140" activeCellId="0" sqref="G140"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5082,7 +5088,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5118,7 +5124,7 @@
       </c>
       <c r="I1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1 }, "Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,8 +5145,8 @@
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2," }, ")</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2," }, ")</f>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5161,8 +5167,8 @@
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3," }, ")</f>
-        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3," }, ")</f>
+        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5183,8 +5189,8 @@
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4," }, ")</f>
-        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4," }, ")</f>
+        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5205,8 +5211,8 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5," }, ")</f>
-        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5," }, ")</f>
+        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5227,8 +5233,8 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6," }, ")</f>
-        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6," }, ")</f>
+        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5249,8 +5255,8 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7," }, ")</f>
-        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7," }, ")</f>
+        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5271,8 +5277,8 @@
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8," }, ")</f>
-        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8," }, ")</f>
+        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,8 +5299,8 @@
       </c>
       <c r="F9" s="0"/>
       <c r="G9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9," }, ")</f>
-        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9," }, ")</f>
+        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5315,8 +5321,8 @@
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10," }, ")</f>
-        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10," }, ")</f>
+        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5337,8 +5343,8 @@
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11," }, ")</f>
-        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11," }, ")</f>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5359,8 +5365,8 @@
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12," }, ")</f>
-        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12," }, ")</f>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5381,8 +5387,8 @@
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13," }, ")</f>
-        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13," }, ")</f>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5403,8 +5409,8 @@
       </c>
       <c r="F14" s="0"/>
       <c r="G14" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14," }, ")</f>
-        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14," }, ")</f>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1 }, </v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5425,8 +5431,29 @@
       </c>
       <c r="F15" s="0"/>
       <c r="G15" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15," }, ")</f>
-        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15," }, ")</f>
+        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1 }, </v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C16,""": { ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16," }, ")</f>
+        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5461,7 +5488,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5485,10 +5512,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -5497,10 +5524,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -5509,10 +5536,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -5521,10 +5548,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -5533,10 +5560,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -5545,10 +5572,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -5557,10 +5584,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -5569,10 +5596,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -5581,10 +5608,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -5593,10 +5620,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -5605,10 +5632,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -5693,25 +5720,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5765,13 +5792,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5828,16 +5855,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5896,7 +5923,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements up to the end of Hollow Bastion II
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Events" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Animations" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Stats - Terra" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Abilities" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Stats - Terra" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="420">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -842,6 +843,114 @@
     <t xml:space="preserve">The Underdrome</t>
   </si>
   <si>
+    <t xml:space="preserve">ColiseumVictory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortRockFace2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bailey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RestorationSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restoration Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corridors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnsemStudy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ansem’s Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceCell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pit Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceCanyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceGrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceDataspace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataspace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceIOTowerHallway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Tower: Hallway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceIOCommunications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Tower: Communications Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RestorationSiteCutscene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CorridorsBattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CavernDepths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cavern of Remembrance: Depths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RestorationSiteCutscene2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleGate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RavineTrail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravine Trail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrystalFissure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal Fissure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreatMawCutscene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Great Maw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnsemStudyCutscene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreatMaw</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -857,6 +966,9 @@
     <t xml:space="preserve">Score</t>
   </si>
   <si>
+    <t xml:space="preserve">LV 1?</t>
+  </si>
+  <si>
     <t xml:space="preserve">9d</t>
   </si>
   <si>
@@ -923,6 +1035,18 @@
     <t xml:space="preserve">Pain and Panic Cup</t>
   </si>
   <si>
+    <t xml:space="preserve">Monitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hostile Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demyx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battle of 1000 Heartless</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -987,6 +1111,135 @@
   </si>
   <si>
     <t xml:space="preserve">Grabbed by Twilight Thorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Jump LV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Jump LV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Jump LV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Jump MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Run LV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Run LV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Run LV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Run MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Dodge LV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Dodge LV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Dodge LV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Dodge MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glide LV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glide LV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glide LV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glide MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge Roll LV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge Roll LV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge Roll LV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge Roll MAX</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -1114,7 +1367,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1128,14 +1381,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1461,10 +1706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
@@ -1505,7 +1750,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,84 +5231,677 @@
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
         <f aca="false">B141+C141*256</f>
-        <v>0</v>
+        <v>1549</v>
+      </c>
+      <c r="B141" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C141" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F141" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A141,": { ""worldId"": ",C141,", ""name"": """,D141,""", ""display"": """,E141,""", ""areaId"": ",B141,", ""hideWorld"": ",F141,", },")</f>
+        <v>1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
         <f aca="false">B142+C142*256</f>
-        <v>0</v>
+        <v>4112</v>
+      </c>
+      <c r="B142" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C142" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F142" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A142,": { ""worldId"": ",C142,", ""name"": """,D142,""", ""display"": """,E142,""", ""areaId"": ",B142,", ""hideWorld"": ",F142,", },")</f>
+        <v>4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
         <f aca="false">B143+C143*256</f>
-        <v>0</v>
+        <v>1032</v>
+      </c>
+      <c r="B143" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C143" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F143" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A143,": { ""worldId"": ",C143,", ""name"": """,D143,""", ""display"": """,E143,""", ""areaId"": ",B143,", ""hideWorld"": ",F143,", },")</f>
+        <v>1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
         <f aca="false">B144+C144*256</f>
-        <v>0</v>
+        <v>1031</v>
+      </c>
+      <c r="B144" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C144" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A144,": { ""worldId"": ",C144,", ""name"": """,D144,""", ""display"": """,E144,""", ""areaId"": ",B144,", ""hideWorld"": ",F144,", },")</f>
+        <v>1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
         <f aca="false">B145+C145*256</f>
-        <v>0</v>
+        <v>1030</v>
+      </c>
+      <c r="B145" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C145" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F145" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G145" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A145,": { ""worldId"": ",C145,", ""name"": """,D145,""", ""display"": """,E145,""", ""areaId"": ",B145,", ""hideWorld"": ",F145,", },")</f>
+        <v>1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
         <f aca="false">B146+C146*256</f>
-        <v>0</v>
+        <v>1035</v>
+      </c>
+      <c r="B146" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F146" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A146,": { ""worldId"": ",C146,", ""name"": """,D146,""", ""display"": """,E146,""", ""areaId"": ",B146,", ""hideWorld"": ",F146,", },")</f>
+        <v>1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
         <f aca="false">B147+C147*256</f>
-        <v>0</v>
+        <v>1029</v>
+      </c>
+      <c r="B147" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C147" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F147" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A147,": { ""worldId"": ",C147,", ""name"": """,D147,""", ""display"": """,E147,""", ""areaId"": ",B147,", ""hideWorld"": ",F147,", },")</f>
+        <v>1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="n">
         <f aca="false">B148+C148*256</f>
-        <v>0</v>
+        <v>4352</v>
+      </c>
+      <c r="B148" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F148" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A148,": { ""worldId"": ",C148,", ""name"": """,D148,""", ""display"": """,E148,""", ""areaId"": ",B148,", ""hideWorld"": ",F148,", },")</f>
+        <v>4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="n">
         <f aca="false">B149+C149*256</f>
-        <v>0</v>
+        <v>4353</v>
+      </c>
+      <c r="B149" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C149" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F149" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A149,": { ""worldId"": ",C149,", ""name"": """,D149,""", ""display"": """,E149,""", ""areaId"": ",B149,", ""hideWorld"": ",F149,", },")</f>
+        <v>4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
         <f aca="false">B150+C150*256</f>
-        <v>0</v>
+        <v>4354</v>
+      </c>
+      <c r="B150" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A150,": { ""worldId"": ",C150,", ""name"": """,D150,""", ""display"": """,E150,""", ""areaId"": ",B150,", ""hideWorld"": ",F150,", },")</f>
+        <v>4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="n">
         <f aca="false">B151+C151*256</f>
-        <v>0</v>
+        <v>4355</v>
+      </c>
+      <c r="B151" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A151,": { ""worldId"": ",C151,", ""name"": """,D151,""", ""display"": """,E151,""", ""areaId"": ",B151,", ""hideWorld"": ",F151,", },")</f>
+        <v>4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
         <f aca="false">B152+C152*256</f>
-        <v>0</v>
+        <v>4356</v>
+      </c>
+      <c r="B152" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C152" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A152,": { ""worldId"": ",C152,", ""name"": """,D152,""", ""display"": """,E152,""", ""areaId"": ",B152,", ""hideWorld"": ",F152,", },")</f>
+        <v>4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
         <f aca="false">B153+C153*256</f>
-        <v>0</v>
+        <v>4357</v>
+      </c>
+      <c r="B153" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C153" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F153" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G153" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A153,": { ""worldId"": ",C153,", ""name"": """,D153,""", ""display"": """,E153,""", ""areaId"": ",B153,", ""hideWorld"": ",F153,", },")</f>
+        <v>4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
         <f aca="false">B154+C154*256</f>
+        <v>1043</v>
+      </c>
+      <c r="B154" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C154" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F154" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A154,": { ""worldId"": ",C154,", ""name"": """,D154,""", ""display"": """,E154,""", ""areaId"": ",B154,", ""hideWorld"": ",F154,", },")</f>
+        <v>1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="n">
+        <f aca="false">B155+C155*256</f>
+        <v>1044</v>
+      </c>
+      <c r="B155" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C155" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F155" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G155" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A155,": { ""worldId"": ",C155,", ""name"": """,D155,""", ""display"": """,E155,""", ""areaId"": ",B155,", ""hideWorld"": ",F155,", },")</f>
+        <v>1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="n">
+        <f aca="false">B156+C156*256</f>
+        <v>1045</v>
+      </c>
+      <c r="B156" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="C156" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F156" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G156" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A156,": { ""worldId"": ",C156,", ""name"": """,D156,""", ""display"": """,E156,""", ""areaId"": ",B156,", ""hideWorld"": ",F156,", },")</f>
+        <v>1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="n">
+        <f aca="false">B157+C157*256</f>
+        <v>1042</v>
+      </c>
+      <c r="B157" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C157" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F157" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A157,": { ""worldId"": ",C157,", ""name"": """,D157,""", ""display"": """,E157,""", ""areaId"": ",B157,", ""hideWorld"": ",F157,", },")</f>
+        <v>1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="n">
+        <f aca="false">B158+C158*256</f>
+        <v>1028</v>
+      </c>
+      <c r="B158" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C158" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F158" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A158,": { ""worldId"": ",C158,", ""name"": """,D158,""", ""display"": """,E158,""", ""areaId"": ",B158,", ""hideWorld"": ",F158,", },")</f>
+        <v>1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="n">
+        <f aca="false">B159+C159*256</f>
+        <v>1040</v>
+      </c>
+      <c r="B159" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C159" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F159" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G159" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A159,": { ""worldId"": ",C159,", ""name"": """,D159,""", ""display"": """,E159,""", ""areaId"": ",B159,", ""hideWorld"": ",F159,", },")</f>
+        <v>1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="n">
+        <f aca="false">B160+C160*256</f>
+        <v>1027</v>
+      </c>
+      <c r="B160" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F160" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A160,": { ""worldId"": ",C160,", ""name"": """,D160,""", ""display"": """,E160,""", ""areaId"": ",B160,", ""hideWorld"": ",F160,", },")</f>
+        <v>1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="n">
+        <f aca="false">B161+C161*256</f>
+        <v>1026</v>
+      </c>
+      <c r="B161" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C161" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F161" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A161,": { ""worldId"": ",C161,", ""name"": """,D161,""", ""display"": """,E161,""", ""areaId"": ",B161,", ""hideWorld"": ",F161,", },")</f>
+        <v>1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="n">
+        <f aca="false">B162+C162*256</f>
+        <v>1039</v>
+      </c>
+      <c r="B162" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C162" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F162" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A162,": { ""worldId"": ",C162,", ""name"": """,D162,""", ""display"": """,E162,""", ""areaId"": ",B162,", ""hideWorld"": ",F162,", },")</f>
+        <v>1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="n">
+        <f aca="false">B163+C163*256</f>
+        <v>1041</v>
+      </c>
+      <c r="B163" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C163" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F163" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A163,": { ""worldId"": ",C163,", ""name"": """,D163,""", ""display"": """,E163,""", ""areaId"": ",B163,", ""hideWorld"": ",F163,", },")</f>
+        <v>1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="n">
+        <f aca="false">B164+C164*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="n">
+        <f aca="false">B165+C165*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="n">
+        <f aca="false">B166+C166*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="n">
+        <f aca="false">B167+C167*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="n">
+        <f aca="false">B168+C168*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="n">
+        <f aca="false">B169+C169*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <f aca="false">B170+C170*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="n">
+        <f aca="false">B171+C171*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="n">
+        <f aca="false">B172+C172*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="n">
+        <f aca="false">B173+C173*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="n">
+        <f aca="false">B174+C174*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="n">
+        <f aca="false">B175+C175*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="n">
+        <f aca="false">B176+C176*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="n">
+        <f aca="false">B177+C177*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="n">
+        <f aca="false">B178+C178*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="n">
+        <f aca="false">B179+C179*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="n">
+        <f aca="false">B180+C180*256</f>
         <v>0</v>
       </c>
     </row>
@@ -5085,68 +5923,73 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="4" style="1" width="12.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F1" s="0"/>
+        <v>310</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="str">
+      <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1 }, "Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>314</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="0"/>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2," }, ")</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2,", ""lv1"": ",F2," }, ")</f>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,40 +6000,44 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="0"/>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3," }, ")</f>
-        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3,", ""lv1"": ",F3," }, ")</f>
+        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="0"/>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4," }, ")</f>
-        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4,", ""lv1"": ",F4," }, ")</f>
+        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5201,40 +6048,44 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="0"/>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5," }, ")</f>
-        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5,", ""lv1"": ",F5," }, ")</f>
+        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>283</v>
+        <v>320</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="0"/>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6," }, ")</f>
-        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6,", ""lv1"": ",F6," }, ")</f>
+        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,18 +6096,20 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F7" s="0"/>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7," }, ")</f>
-        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7,", ""lv1"": ",F7," }, ")</f>
+        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,18 +6120,20 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D8" s="0" t="n">
+        <v>323</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="0"/>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8," }, ")</f>
-        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8,", ""lv1"": ",F8," }, ")</f>
+        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,62 +6144,68 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D9" s="0" t="n">
+        <v>324</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="0"/>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9," }, ")</f>
-        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9,", ""lv1"": ",F9," }, ")</f>
+        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>326</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F10" s="0"/>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10," }, ")</f>
-        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10,", ""lv1"": ",F10," }, ")</f>
+        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D11" s="0" t="n">
+        <v>328</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="F11" s="0"/>
+      <c r="F11" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G11" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11," }, ")</f>
-        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11,", ""lv1"": ",F11," }, ")</f>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,18 +6216,20 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D12" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="0"/>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G12" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12," }, ")</f>
-        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12,", ""lv1"": ",F12," }, ")</f>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5377,40 +6240,44 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F13" s="0"/>
+      <c r="F13" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G13" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13," }, ")</f>
-        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13,", ""lv1"": ",F13," }, ")</f>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>332</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="0"/>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G14" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14," }, ")</f>
-        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14,", ""lv1"": ",F14," }, ")</f>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5421,29 +6288,31 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="F15" s="0"/>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G15" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15," }, ")</f>
-        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15,", ""lv1"": ",F15," }, ")</f>
+        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>297</v>
+        <v>334</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -5451,9 +6320,108 @@
       <c r="E16" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT("""",C16,""": { ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16," }, ")</f>
-        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0 }, </v>
+        <f aca="false">_xlfn.CONCAT("""",C16,""": { ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16,", ""lv1"": ",F16," }, ")</f>
+        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C17,""": { ""locationCode"": """,B17,""", ""eventId"": 0x",A17,", ""score"": ",E17,", ""isBoss"": ",D17,", ""lv1"": ",F17," }, ")</f>
+        <v>"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C18,""": { ""locationCode"": """,B18,""", ""eventId"": 0x",A18,", ""score"": ",E18,", ""isBoss"": ",D18,", ""lv1"": ",F18," }, ")</f>
+        <v>"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C19,""": { ""locationCode"": """,B19,""", ""eventId"": 0x",A19,", ""score"": ",E19,", ""isBoss"": ",D19,", ""lv1"": ",F19," }, ")</f>
+        <v>"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C20,""": { ""locationCode"": """,B20,""", ""eventId"": 0x",A20,", ""score"": ",E20,", ""isBoss"": ",D20,", ""lv1"": ",F20," }, ")</f>
+        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5478,7 +6446,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5488,7 +6456,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>299</v>
+        <v>340</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5512,10 +6480,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>300</v>
+        <v>341</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>301</v>
+        <v>342</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -5524,10 +6492,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>302</v>
+        <v>343</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -5536,10 +6504,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -5548,10 +6516,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -5560,10 +6528,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>307</v>
+        <v>348</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>308</v>
+        <v>349</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -5572,10 +6540,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>309</v>
+        <v>350</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>310</v>
+        <v>351</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -5584,10 +6552,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>311</v>
+        <v>352</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>312</v>
+        <v>353</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -5596,10 +6564,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>313</v>
+        <v>354</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>314</v>
+        <v>355</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -5608,10 +6576,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>315</v>
+        <v>356</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>316</v>
+        <v>357</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -5620,10 +6588,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>317</v>
+        <v>358</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>318</v>
+        <v>359</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -5632,10 +6600,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>319</v>
+        <v>360</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>320</v>
+        <v>361</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -5696,6 +6664,421 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(E2:E1045)</f>
+        <v>0x5e: { "name": "High Jump LV1", "type": "Growth", "ap": 2, "id": 0x5e },0x5f: { "name": "High Jump LV2", "type": "Growth", "ap": 2, "id": 0x5f },0x60: { "name": "High Jump LV3", "type": "Growth", "ap": 2, "id": 0x60 },0x61: { "name": "High Jump MAX", "type": "Growth", "ap": 2, "id": 0x61 },0x62: { "name": "Quick Run LV1", "type": "Growth", "ap": 2, "id": 0x62 },0x63: { "name": "Quick Run LV2", "type": "Growth", "ap": 2, "id": 0x63 },0x64: { "name": "Quick Run LV3", "type": "Growth", "ap": 2, "id": 0x64 },0x65: { "name": "Quick Run MAX", "type": "Growth", "ap": 2, "id": 0x65 },0x66: { "name": "Aerial Dodge LV1", "type": "Growth", "ap": 3, "id": 0x66 },0x67: { "name": "Aerial Dodge LV2", "type": "Growth", "ap": 3, "id": 0x67 },0x68: { "name": "Aerial Dodge LV3", "type": "Growth", "ap": 3, "id": 0x68 },0x69: { "name": "Aerial Dodge MAX", "type": "Growth", "ap": 3, "id": 0x69 },0x6a: { "name": "Glide LV1", "type": "Growth", "ap": 3, "id": 0x6a },0x6b: { "name": "Glide LV2", "type": "Growth", "ap": 3, "id": 0x6b },0x6c: { "name": "Glide LV3", "type": "Growth", "ap": 3, "id": 0x6c },0x6d: { "name": "Glide MAX", "type": "Growth", "ap": 3, "id": 0x6d },0x234: { "name": "Dodge Roll LV1", "type": "Growth", "ap": 3, "id": 0x234 },0x235: { "name": "Dodge Roll LV2", "type": "Growth", "ap": 3, "id": 0x235 },0x236: { "name": "Dodge Roll LV3", "type": "Growth", "ap": 3, "id": 0x236 },0x237: { "name": "Dodge Roll MAX", "type": "Growth", "ap": 3, "id": 0x237 },</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A2,": { ""name"": """,B2,""", ""type"": """,C2,""", ""ap"": ",D2,", ""id"": ",A2," },")</f>
+        <v>0x5e: { "name": "High Jump LV1", "type": "Growth", "ap": 2, "id": 0x5e },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A3,": { ""name"": """,B3,""", ""type"": """,C3,""", ""ap"": ",D3,", ""id"": ",A3," },")</f>
+        <v>0x5f: { "name": "High Jump LV2", "type": "Growth", "ap": 2, "id": 0x5f },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A4,": { ""name"": """,B4,""", ""type"": """,C4,""", ""ap"": ",D4,", ""id"": ",A4," },")</f>
+        <v>0x60: { "name": "High Jump LV3", "type": "Growth", "ap": 2, "id": 0x60 },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A5,": { ""name"": """,B5,""", ""type"": """,C5,""", ""ap"": ",D5,", ""id"": ",A5," },")</f>
+        <v>0x61: { "name": "High Jump MAX", "type": "Growth", "ap": 2, "id": 0x61 },</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A6,": { ""name"": """,B6,""", ""type"": """,C6,""", ""ap"": ",D6,", ""id"": ",A6," },")</f>
+        <v>0x62: { "name": "Quick Run LV1", "type": "Growth", "ap": 2, "id": 0x62 },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A7,": { ""name"": """,B7,""", ""type"": """,C7,""", ""ap"": ",D7,", ""id"": ",A7," },")</f>
+        <v>0x63: { "name": "Quick Run LV2", "type": "Growth", "ap": 2, "id": 0x63 },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A8,": { ""name"": """,B8,""", ""type"": """,C8,""", ""ap"": ",D8,", ""id"": ",A8," },")</f>
+        <v>0x64: { "name": "Quick Run LV3", "type": "Growth", "ap": 2, "id": 0x64 },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A9,": { ""name"": """,B9,""", ""type"": """,C9,""", ""ap"": ",D9,", ""id"": ",A9," },")</f>
+        <v>0x65: { "name": "Quick Run MAX", "type": "Growth", "ap": 2, "id": 0x65 },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A10,": { ""name"": """,B10,""", ""type"": """,C10,""", ""ap"": ",D10,", ""id"": ",A10," },")</f>
+        <v>0x66: { "name": "Aerial Dodge LV1", "type": "Growth", "ap": 3, "id": 0x66 },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A11,": { ""name"": """,B11,""", ""type"": """,C11,""", ""ap"": ",D11,", ""id"": ",A11," },")</f>
+        <v>0x67: { "name": "Aerial Dodge LV2", "type": "Growth", "ap": 3, "id": 0x67 },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A12,": { ""name"": """,B12,""", ""type"": """,C12,""", ""ap"": ",D12,", ""id"": ",A12," },")</f>
+        <v>0x68: { "name": "Aerial Dodge LV3", "type": "Growth", "ap": 3, "id": 0x68 },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A13,": { ""name"": """,B13,""", ""type"": """,C13,""", ""ap"": ",D13,", ""id"": ",A13," },")</f>
+        <v>0x69: { "name": "Aerial Dodge MAX", "type": "Growth", "ap": 3, "id": 0x69 },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A14,": { ""name"": """,B14,""", ""type"": """,C14,""", ""ap"": ",D14,", ""id"": ",A14," },")</f>
+        <v>0x6a: { "name": "Glide LV1", "type": "Growth", "ap": 3, "id": 0x6a },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A15,": { ""name"": """,B15,""", ""type"": """,C15,""", ""ap"": ",D15,", ""id"": ",A15," },")</f>
+        <v>0x6b: { "name": "Glide LV2", "type": "Growth", "ap": 3, "id": 0x6b },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A16,": { ""name"": """,B16,""", ""type"": """,C16,""", ""ap"": ",D16,", ""id"": ",A16," },")</f>
+        <v>0x6c: { "name": "Glide LV3", "type": "Growth", "ap": 3, "id": 0x6c },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A17,": { ""name"": """,B17,""", ""type"": """,C17,""", ""ap"": ",D17,", ""id"": ",A17," },")</f>
+        <v>0x6d: { "name": "Glide MAX", "type": "Growth", "ap": 3, "id": 0x6d },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A18,": { ""name"": """,B18,""", ""type"": """,C18,""", ""ap"": ",D18,", ""id"": ",A18," },")</f>
+        <v>0x234: { "name": "Dodge Roll LV1", "type": "Growth", "ap": 3, "id": 0x234 },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A19,": { ""name"": """,B19,""", ""type"": """,C19,""", ""ap"": ",D19,", ""id"": ",A19," },")</f>
+        <v>0x235: { "name": "Dodge Roll LV2", "type": "Growth", "ap": 3, "id": 0x235 },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A20,": { ""name"": """,B20,""", ""type"": """,C20,""", ""ap"": ",D20,", ""id"": ",A20," },")</f>
+        <v>0x236: { "name": "Dodge Roll LV3", "type": "Growth", "ap": 3, "id": 0x236 },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A21,": { ""name"": """,B21,""", ""type"": """,C21,""", ""ap"": ",D21,", ""id"": ",A21," },")</f>
+        <v>0x237: { "name": "Dodge Roll MAX", "type": "Growth", "ap": 3, "id": 0x237 },</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5720,25 +7103,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>321</v>
+        <v>405</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>322</v>
+        <v>406</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>323</v>
+        <v>407</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>324</v>
+        <v>408</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>325</v>
+        <v>409</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>326</v>
+        <v>410</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>327</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,13 +7175,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>328</v>
+        <v>412</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>329</v>
+        <v>413</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,15 +7197,15 @@
       <c r="D5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
         <v>29</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="4" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
         <v>25</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="4" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
         <v>24</v>
       </c>
@@ -5855,16 +7238,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>331</v>
+        <v>415</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>332</v>
+        <v>416</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>333</v>
+        <v>417</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>334</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5923,7 +7306,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>335</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements for the second visit of the Land of Dragons
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="425">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -951,6 +951,18 @@
     <t xml:space="preserve">GreatMaw</t>
   </si>
   <si>
+    <t xml:space="preserve">DragonAntechamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antechamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DragonThrone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throne Room</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -1045,6 +1057,9 @@
   </si>
   <si>
     <t xml:space="preserve">Battle of 1000 Heartless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storm Rider</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1708,10 +1723,10 @@
   </sheetPr>
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="G165" activeCellId="0" sqref="G165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1750,7 +1765,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5806,13 +5821,51 @@
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
         <f aca="false">B164+C164*256</f>
-        <v>0</v>
+        <v>2058</v>
+      </c>
+      <c r="B164" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C164" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F164" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A164,": { ""worldId"": ",C164,", ""name"": """,D164,""", ""display"": """,E164,""", ""areaId"": ",B164,", ""hideWorld"": ",F164,", },")</f>
+        <v>2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
         <f aca="false">B165+C165*256</f>
-        <v>0</v>
+        <v>2059</v>
+      </c>
+      <c r="B165" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C165" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F165" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A165,": { ""worldId"": ",C165,", ""name"": """,D165,""", ""display"": """,E165,""", ""areaId"": ",B165,", ""hideWorld"": ",F165,", },")</f>
+        <v>2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5923,10 +5976,10 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5940,22 +5993,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -5965,18 +6018,18 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -6000,7 +6053,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -6018,13 +6071,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -6048,7 +6101,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -6066,13 +6119,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -6096,7 +6149,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
@@ -6120,7 +6173,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -6144,7 +6197,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
@@ -6162,13 +6215,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -6186,13 +6239,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
@@ -6216,7 +6269,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -6240,7 +6293,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
@@ -6258,13 +6311,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -6288,7 +6341,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -6306,13 +6359,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -6336,7 +6389,7 @@
         <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -6360,7 +6413,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -6384,7 +6437,7 @@
         <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -6408,7 +6461,7 @@
         <v>307</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -6421,7 +6474,31 @@
       </c>
       <c r="G20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C20,""": { ""locationCode"": """,B20,""", ""eventId"": 0x",A20,", ""score"": ",E20,", ""isBoss"": ",D20,", ""lv1"": ",F20," }, ")</f>
-        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
+        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C21,""": { ""locationCode"": """,B21,""", ""eventId"": 0x",A21,", ""score"": ",E21,", ""isBoss"": ",D21,", ""lv1"": ",F21," }, ")</f>
+        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6456,7 +6533,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6480,10 +6557,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -6492,10 +6569,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -6504,10 +6581,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -6516,10 +6593,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -6528,10 +6605,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -6540,10 +6617,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -6552,10 +6629,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -6564,10 +6641,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -6576,10 +6653,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -6588,10 +6665,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -6600,10 +6677,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -6685,16 +6762,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -6709,13 +6786,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -6727,13 +6804,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -6745,13 +6822,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -6763,13 +6840,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -6781,13 +6858,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -6799,13 +6876,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -6817,13 +6894,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -6835,13 +6912,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -6853,13 +6930,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
@@ -6871,13 +6948,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>3</v>
@@ -6889,13 +6966,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
@@ -6907,13 +6984,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>3</v>
@@ -6925,13 +7002,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>3</v>
@@ -6943,13 +7020,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>3</v>
@@ -6961,13 +7038,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>3</v>
@@ -6979,13 +7056,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3</v>
@@ -6997,13 +7074,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>3</v>
@@ -7015,13 +7092,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
@@ -7033,13 +7110,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>3</v>
@@ -7051,13 +7128,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
@@ -7103,25 +7180,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7175,13 +7252,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,16 +7315,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7306,7 +7383,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added the achievements for the second visit to Beast's Castle
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="428">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -963,6 +963,12 @@
     <t xml:space="preserve">Throne Room</t>
   </si>
   <si>
+    <t xml:space="preserve">BeastBridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -1060,6 +1066,9 @@
   </si>
   <si>
     <t xml:space="preserve">Storm Rider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xaldin</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1723,10 +1732,10 @@
   </sheetPr>
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G165" activeCellId="0" sqref="G165"/>
+      <selection pane="bottomLeft" activeCell="G166" activeCellId="0" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1765,7 +1774,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5871,7 +5880,26 @@
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
         <f aca="false">B166+C166*256</f>
-        <v>0</v>
+        <v>1295</v>
+      </c>
+      <c r="B166" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C166" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F166" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A166,": { ""worldId"": ",C166,", ""name"": """,D166,""", ""display"": """,E166,""", ""areaId"": ",B166,", ""hideWorld"": ",F166,", },")</f>
+        <v>1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5976,10 +6004,10 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5993,22 +6021,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -6018,18 +6046,18 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -6053,7 +6081,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -6071,13 +6099,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -6101,7 +6129,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -6119,13 +6147,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -6149,7 +6177,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
@@ -6173,7 +6201,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -6197,7 +6225,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
@@ -6215,13 +6243,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -6239,13 +6267,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
@@ -6269,7 +6297,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -6293,7 +6321,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
@@ -6311,13 +6339,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -6341,7 +6369,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -6359,13 +6387,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -6389,7 +6417,7 @@
         <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -6413,7 +6441,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -6437,7 +6465,7 @@
         <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -6461,7 +6489,7 @@
         <v>307</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -6479,13 +6507,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -6498,7 +6526,31 @@
       </c>
       <c r="G21" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C21,""": { ""locationCode"": """,B21,""", ""eventId"": 0x",A21,", ""score"": ",E21,", ""isBoss"": ",D21,", ""lv1"": ",F21," }, ")</f>
-        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C22,""": { ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22," }, ")</f>
+        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6533,7 +6585,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6557,10 +6609,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -6569,10 +6621,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -6581,10 +6633,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -6593,10 +6645,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -6605,10 +6657,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -6617,10 +6669,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -6629,10 +6681,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -6641,10 +6693,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -6653,10 +6705,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -6665,10 +6717,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -6677,10 +6729,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -6762,16 +6814,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -6786,13 +6838,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -6804,13 +6856,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -6822,13 +6874,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -6840,13 +6892,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -6858,13 +6910,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -6876,13 +6928,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -6894,13 +6946,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -6912,13 +6964,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -6930,13 +6982,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
@@ -6948,13 +7000,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>3</v>
@@ -6966,13 +7018,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
@@ -6984,13 +7036,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>3</v>
@@ -7002,13 +7054,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>3</v>
@@ -7020,13 +7072,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>3</v>
@@ -7038,13 +7090,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>3</v>
@@ -7056,13 +7108,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3</v>
@@ -7074,13 +7126,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>3</v>
@@ -7092,13 +7144,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
@@ -7110,13 +7162,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>3</v>
@@ -7128,13 +7180,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
@@ -7180,25 +7232,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7252,13 +7304,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7315,16 +7367,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7383,7 +7435,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements up to the end of the second visit of Olympus Coliseum
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="431">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -969,6 +969,9 @@
     <t xml:space="preserve">Bridge</t>
   </si>
   <si>
+    <t xml:space="preserve">ColiseumTourneyHades</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -1069,6 +1072,12 @@
   </si>
   <si>
     <t xml:space="preserve">Xaldin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hades</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1732,10 +1741,10 @@
   </sheetPr>
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G166" activeCellId="0" sqref="G166"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1774,7 +1783,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5914,26 @@
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
         <f aca="false">B167+C167*256</f>
-        <v>0</v>
+        <v>1555</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C167" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F167" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A167,": { ""worldId"": ",C167,", ""name"": """,D167,""", ""display"": """,E167,""", ""areaId"": ",B167,", ""hideWorld"": ",F167,", },")</f>
+        <v>1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6004,10 +6032,10 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6021,22 +6049,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -6046,18 +6074,18 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, "Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -6081,7 +6109,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -6099,13 +6127,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -6129,7 +6157,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -6147,13 +6175,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -6177,7 +6205,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
@@ -6201,7 +6229,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -6225,7 +6253,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
@@ -6243,13 +6271,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -6267,13 +6295,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
@@ -6297,7 +6325,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -6321,7 +6349,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
@@ -6339,13 +6367,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -6369,7 +6397,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -6387,13 +6415,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -6417,7 +6445,7 @@
         <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -6441,7 +6469,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -6465,7 +6493,7 @@
         <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -6489,7 +6517,7 @@
         <v>307</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -6507,13 +6535,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -6537,7 +6565,7 @@
         <v>312</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -6551,6 +6579,30 @@
       <c r="G22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C22,""": { ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22," }, ")</f>
         <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C23,""": { ""locationCode"": """,B23,""", ""eventId"": 0x",A23,", ""score"": ",E23,", ""isBoss"": ",D23,", ""lv1"": ",F23," }, ")</f>
+        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6585,7 +6637,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6609,10 +6661,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -6621,10 +6673,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -6633,10 +6685,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -6645,10 +6697,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -6657,10 +6709,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -6669,10 +6721,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -6681,10 +6733,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -6693,10 +6745,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -6705,10 +6757,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -6717,10 +6769,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -6729,10 +6781,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -6814,16 +6866,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -6838,13 +6890,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -6856,13 +6908,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -6874,13 +6926,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>374</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -6892,13 +6944,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -6910,13 +6962,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -6928,13 +6980,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -6946,13 +6998,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -6964,13 +7016,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -6982,13 +7034,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
@@ -7000,13 +7052,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>3</v>
@@ -7018,13 +7070,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
@@ -7036,13 +7088,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>3</v>
@@ -7054,13 +7106,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>3</v>
@@ -7072,13 +7124,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>3</v>
@@ -7090,13 +7142,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>3</v>
@@ -7108,13 +7160,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3</v>
@@ -7126,13 +7178,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>3</v>
@@ -7144,13 +7196,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
@@ -7162,13 +7214,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>3</v>
@@ -7180,13 +7232,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
@@ -7232,25 +7284,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7304,13 +7356,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7367,16 +7419,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7435,7 +7487,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements for the second visit to Port Royal
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="444">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -972,6 +972,42 @@
     <t xml:space="preserve">ColiseumTourneyHades</t>
   </si>
   <si>
+    <t xml:space="preserve">PortPearl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Black Pearl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortPearlCaptain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Black Pearl: Captain’s Stateroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortPearlBattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortGraveyardInterceptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship Graveyard: The Interceptor’s Hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortGraveyardRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship Graveyard: Seadrift Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortGraveyardKeep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship Graveyard: Seadrift Keep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PortHarborCutscene</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -1078,6 +1114,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grim Reaper II</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1741,10 +1780,10 @@
   </sheetPr>
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C178" activeCellId="0" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1783,7 +1822,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },4101: { "worldId": 16, "name": "PortPearl", "display": "The Black Pearl", "areaId": 5, "hideWorld": 0, },4102: { "worldId": 16, "name": "PortPearlCaptain", "display": "The Black Pearl: Captain’s Stateroom", "areaId": 6, "hideWorld": 0, },4115: { "worldId": 16, "name": "PortPearlBattle", "display": "The Black Pearl", "areaId": 19, "hideWorld": 0, },4107: { "worldId": 16, "name": "PortGraveyardInterceptor", "display": "Ship Graveyard: The Interceptor’s Hold", "areaId": 11, "hideWorld": 0, },4111: { "worldId": 16, "name": "PortGraveyardRow", "display": "Ship Graveyard: Seadrift Row", "areaId": 15, "hideWorld": 0, },4110: { "worldId": 16, "name": "PortGraveyardKeep", "display": "Ship Graveyard: Seadrift Keep", "areaId": 14, "hideWorld": 0, },4120: { "worldId": 16, "name": "PortHarborCutscene", "display": "Harbor", "areaId": 24, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5939,43 +5978,176 @@
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
         <f aca="false">B168+C168*256</f>
-        <v>0</v>
+        <v>4101</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C168" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G168" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A168,": { ""worldId"": ",C168,", ""name"": """,D168,""", ""display"": """,E168,""", ""areaId"": ",B168,", ""hideWorld"": ",F168,", },")</f>
+        <v>4101: { "worldId": 16, "name": "PortPearl", "display": "The Black Pearl", "areaId": 5, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
         <f aca="false">B169+C169*256</f>
-        <v>0</v>
+        <v>4102</v>
+      </c>
+      <c r="B169" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C169" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F169" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G169" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A169,": { ""worldId"": ",C169,", ""name"": """,D169,""", ""display"": """,E169,""", ""areaId"": ",B169,", ""hideWorld"": ",F169,", },")</f>
+        <v>4102: { "worldId": 16, "name": "PortPearlCaptain", "display": "The Black Pearl: Captain’s Stateroom", "areaId": 6, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
         <f aca="false">B170+C170*256</f>
-        <v>0</v>
+        <v>4115</v>
+      </c>
+      <c r="B170" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C170" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F170" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G170" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A170,": { ""worldId"": ",C170,", ""name"": """,D170,""", ""display"": """,E170,""", ""areaId"": ",B170,", ""hideWorld"": ",F170,", },")</f>
+        <v>4115: { "worldId": 16, "name": "PortPearlBattle", "display": "The Black Pearl", "areaId": 19, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
         <f aca="false">B171+C171*256</f>
-        <v>0</v>
+        <v>4107</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C171" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F171" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G171" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A171,": { ""worldId"": ",C171,", ""name"": """,D171,""", ""display"": """,E171,""", ""areaId"": ",B171,", ""hideWorld"": ",F171,", },")</f>
+        <v>4107: { "worldId": 16, "name": "PortGraveyardInterceptor", "display": "Ship Graveyard: The Interceptor’s Hold", "areaId": 11, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
         <f aca="false">B172+C172*256</f>
-        <v>0</v>
+        <v>4111</v>
+      </c>
+      <c r="B172" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C172" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F172" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A172,": { ""worldId"": ",C172,", ""name"": """,D172,""", ""display"": """,E172,""", ""areaId"": ",B172,", ""hideWorld"": ",F172,", },")</f>
+        <v>4111: { "worldId": 16, "name": "PortGraveyardRow", "display": "Ship Graveyard: Seadrift Row", "areaId": 15, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
         <f aca="false">B173+C173*256</f>
-        <v>0</v>
+        <v>4110</v>
+      </c>
+      <c r="B173" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C173" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F173" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G173" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A173,": { ""worldId"": ",C173,", ""name"": """,D173,""", ""display"": """,E173,""", ""areaId"": ",B173,", ""hideWorld"": ",F173,", },")</f>
+        <v>4110: { "worldId": 16, "name": "PortGraveyardKeep", "display": "Ship Graveyard: Seadrift Keep", "areaId": 14, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
         <f aca="false">B174+C174*256</f>
-        <v>0</v>
+        <v>4120</v>
+      </c>
+      <c r="B174" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G174" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A174,": { ""worldId"": ",C174,", ""name"": """,D174,""", ""display"": """,E174,""", ""areaId"": ",B174,", ""hideWorld"": ",F174,", },")</f>
+        <v>4120: { "worldId": 16, "name": "PortHarborCutscene", "display": "Harbor", "areaId": 24, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6032,10 +6204,10 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6049,22 +6221,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -6074,18 +6246,18 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, "Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -6109,7 +6281,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -6127,13 +6299,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -6157,7 +6329,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -6175,13 +6347,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -6205,7 +6377,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
@@ -6229,7 +6401,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -6253,7 +6425,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
@@ -6271,13 +6443,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -6295,13 +6467,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
@@ -6325,7 +6497,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -6349,7 +6521,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
@@ -6367,13 +6539,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -6397,7 +6569,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -6415,13 +6587,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -6445,7 +6617,7 @@
         <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -6469,7 +6641,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -6493,7 +6665,7 @@
         <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -6517,7 +6689,7 @@
         <v>307</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -6535,13 +6707,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -6565,7 +6737,7 @@
         <v>312</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -6578,18 +6750,18 @@
       </c>
       <c r="G22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C22,""": { ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22," }, ")</f>
-        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
@@ -6602,7 +6774,31 @@
       </c>
       <c r="G23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C23,""": { ""locationCode"": """,B23,""", ""eventId"": 0x",A23,", ""score"": ",E23,", ""isBoss"": ",D23,", ""lv1"": ",F23," }, ")</f>
-        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C24,""": { ""locationCode"": """,B24,""", ""eventId"": 0x",A24,", ""score"": ",E24,", ""isBoss"": ",D24,", ""lv1"": ",F24," }, ")</f>
+        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6637,7 +6833,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6661,10 +6857,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -6673,10 +6869,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -6685,10 +6881,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -6697,10 +6893,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -6709,10 +6905,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -6721,10 +6917,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -6733,10 +6929,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -6745,10 +6941,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -6757,10 +6953,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -6769,10 +6965,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -6781,10 +6977,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -6866,16 +7062,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -6890,13 +7086,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -6908,13 +7104,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -6926,13 +7122,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -6944,13 +7140,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -6962,13 +7158,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -6980,13 +7176,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -6998,13 +7194,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -7016,13 +7212,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -7034,13 +7230,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
@@ -7052,13 +7248,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>3</v>
@@ -7070,13 +7266,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
@@ -7088,13 +7284,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>3</v>
@@ -7106,13 +7302,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>3</v>
@@ -7124,13 +7320,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>3</v>
@@ -7142,13 +7338,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>3</v>
@@ -7160,13 +7356,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3</v>
@@ -7178,13 +7374,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>3</v>
@@ -7196,13 +7392,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
@@ -7214,13 +7410,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>3</v>
@@ -7232,13 +7428,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
@@ -7284,25 +7480,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7356,13 +7552,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7419,16 +7615,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7487,7 +7683,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements up to the end of Agrabah II
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="461">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -1008,6 +1008,42 @@
     <t xml:space="preserve">PortHarborCutscene</t>
   </si>
   <si>
+    <t xml:space="preserve">HalloweenWrapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas Town: The Wrapping Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HalloweenPlaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas Town: Christmas Tree Plaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahShop2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahSand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandswept Ruins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahRuin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruined Chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahAbove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Above the City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrideSavannahBattle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event ID</t>
   </si>
   <si>
@@ -1117,6 +1153,21 @@
   </si>
   <si>
     <t xml:space="preserve">Grim Reaper II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandswept Ruins Escape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jafar</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1778,12 +1829,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I180"/>
+  <dimension ref="A1:I197"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C178" activeCellId="0" sqref="C178"/>
+      <selection pane="bottomLeft" activeCell="F184" activeCellId="0" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1822,7 +1873,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },4101: { "worldId": 16, "name": "PortPearl", "display": "The Black Pearl", "areaId": 5, "hideWorld": 0, },4102: { "worldId": 16, "name": "PortPearlCaptain", "display": "The Black Pearl: Captain’s Stateroom", "areaId": 6, "hideWorld": 0, },4115: { "worldId": 16, "name": "PortPearlBattle", "display": "The Black Pearl", "areaId": 19, "hideWorld": 0, },4107: { "worldId": 16, "name": "PortGraveyardInterceptor", "display": "Ship Graveyard: The Interceptor’s Hold", "areaId": 11, "hideWorld": 0, },4111: { "worldId": 16, "name": "PortGraveyardRow", "display": "Ship Graveyard: Seadrift Row", "areaId": 15, "hideWorld": 0, },4110: { "worldId": 16, "name": "PortGraveyardKeep", "display": "Ship Graveyard: Seadrift Keep", "areaId": 14, "hideWorld": 0, },4120: { "worldId": 16, "name": "PortHarborCutscene", "display": "Harbor", "areaId": 24, "hideWorld": 0, },</v>
+        <v>65535: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },523: { "worldId": 2, "name": "SunsetStation", "display": "Sunset Station", "areaId": 11, "hideWorld": 0, },522: { "worldId": 2, "name": "SunsetTerrace", "display": "Sunset Terrace", "areaId": 10, "hideWorld": 0, },548: { "worldId": 2, "name": "Tunnelway", "display": "Tunnelway", "areaId": 36, "hideWorld": 0, },524: { "worldId": 2, "name": "SunsetHill", "display": "Sunset Hill", "areaId": 12, "hideWorld": 0, },520: { "worldId": 2, "name": "StationPlaza", "display": "Station Plaza", "areaId": 8, "hideWorld": 0, },518: { "worldId": 2, "name": "StationHeights", "display": "Market Street: Station Heights", "areaId": 6, "hideWorld": 0, },515: { "worldId": 2, "name": "BackAlley", "display": "Back Alley", "areaId": 3, "hideWorld": 0, },514: { "worldId": 2, "name": "UsualSpot", "display": "The Usual Spot", "areaId": 2, "hideWorld": 0, },516: { "worldId": 2, "name": "Sandlot", "display": "Sandlot", "areaId": 4, "hideWorld": 0, },519: { "worldId": 2, "name": "TramCommon", "display": "Market Street: Tram Common", "areaId": 7, "hideWorld": 0, },525: { "worldId": 2, "name": "Woods", "display": "The Woods", "areaId": 13, "hideWorld": 0, },513: { "worldId": 2, "name": "RoxasRoom", "display": "Roxas’s Room", "areaId": 1, "hideWorld": 0, },526: { "worldId": 2, "name": "Courtyard", "display": "Mansion: Courtyard", "areaId": 14, "hideWorld": 0, },527: { "worldId": 2, "name": "Foyer", "display": "Mansion: Foyer", "areaId": 15, "hideWorld": 0, },530: { "worldId": 2, "name": "WhiteRoom", "display": "Mansion: The White Room", "areaId": 18, "hideWorld": 0, },529: { "worldId": 2, "name": "Library", "display": "Mansion: Library", "areaId": 17, "hideWorld": 0, },533: { "worldId": 2, "name": "ComputerRoom", "display": "Mansion: Computer Room", "areaId": 21, "hideWorld": 0, },531: { "worldId": 2, "name": "BasementHall", "display": "Mansion: Basement Hall", "areaId": 19, "hideWorld": 0, },532: { "worldId": 2, "name": "BasementHallAxel", "display": "Mansion: Basement Hall", "areaId": 20, "hideWorld": 0, },534: { "worldId": 2, "name": "BasementCorridor", "display": "Mansion: Basement Corridor", "areaId": 22, "hideWorld": 0, },535: { "worldId": 2, "name": "PodRoom", "display": "Mansion: Pod Room", "areaId": 23, "hideWorld": 0, },544: { "worldId": 2, "name": "StationOfSerenity", "display": "Station of Serenity", "areaId": 32, "hideWorld": 1, },545: { "worldId": 2, "name": "StationOfCalling", "display": "Station of Calling", "areaId": 33, "hideWorld": 1, },546: { "worldId": 2, "name": "StationOfAwakening", "display": "Station of Awakening", "areaId": 34, "hideWorld": 1, },517: { "worldId": 2, "name": "SandlotBattlefield", "display": "Sandlot", "areaId": 5, "hideWorld": 0, },521: { "worldId": 2, "name": "CentralStation", "display": "Central Station", "areaId": 9, "hideWorld": 0, },537: { "worldId": 2, "name": "Tower", "display": "The Tower", "areaId": 25, "hideWorld": 1, },541: { "worldId": 2, "name": "StarChamber", "display": "Tower: Star Chamber", "areaId": 29, "hideWorld": 1, },543: { "worldId": 2, "name": "WaywardStairs", "display": "Tower: Wayward Stairs", "areaId": 31, "hideWorld": 1, },550: { "worldId": 2, "name": "WaywardStairs2", "display": "Tower: Wayward Stairs", "areaId": 38, "hideWorld": 1, },542: { "worldId": 2, "name": "MoonChamber", "display": "Tower: Moon Chamber", "areaId": 30, "hideWorld": 1, },551: { "worldId": 2, "name": "WaywardStairs3", "display": "Tower: Wayward Stairs", "areaId": 39, "hideWorld": 1, },539: { "worldId": 2, "name": "SorcererLoft", "display": "Tower: Sorcerer’s Loft", "areaId": 27, "hideWorld": 1, },540: { "worldId": 2, "name": "Wardrobe", "display": "Tower: Wardrobe", "areaId": 28, "hideWorld": 1, },3840: { "worldId": 15, "name": "WorldMap", "display": "World Map", "areaId": 0, "hideWorld": 1, },1024: { "worldId": 4, "name": "VillainVale", "display": "Villain’s Vale", "areaId": 0, "hideWorld": 0, },1034: { "worldId": 4, "name": "Marketplace", "display": "Marketplace", "areaId": 10, "hideWorld": 0, },1033: { "worldId": 4, "name": "Borough", "display": "Borough", "areaId": 9, "hideWorld": 0, },1037: { "worldId": 4, "name": "Merlin", "display": "Merlin’s House", "areaId": 13, "hideWorld": 0, },2048: { "worldId": 8, "name": "BambooGrove", "display": "Bamboo Grove", "areaId": 0, "hideWorld": 0, },2049: { "worldId": 8, "name": "Encampment", "display": "Encampment", "areaId": 1, "hideWorld": 0, },2050: { "worldId": 8, "name": "Checkpoint", "display": "Checkpoint", "areaId": 2, "hideWorld": 0, },2052: { "worldId": 8, "name": "Village", "display": "Village", "areaId": 4, "hideWorld": 0, },2051: { "worldId": 8, "name": "MountainTrail", "display": "Mountain Trail", "areaId": 3, "hideWorld": 0, },2053: { "worldId": 8, "name": "VillageCave", "display": "Village Cave", "areaId": 5, "hideWorld": 0, },2060: { "worldId": 8, "name": "RuinedVillage", "display": "Village", "areaId": 12, "hideWorld": 0, },2054: { "worldId": 8, "name": "Ridge", "display": "Ridge", "areaId": 6, "hideWorld": 0, },2055: { "worldId": 8, "name": "Summit", "display": "Summit", "areaId": 7, "hideWorld": 0, },2056: { "worldId": 8, "name": "ImperialSquare", "display": "Imperial Square", "areaId": 8, "hideWorld": 0, },2057: { "worldId": 8, "name": "PalaceGate", "display": "Palace Gate", "areaId": 9, "hideWorld": 0, },1280: { "worldId": 5, "name": "EntranceHall", "display": "Entrance Hall", "areaId": 0, "hideWorld": 0, },1281: { "worldId": 5, "name": "Parlor", "display": "Parlor", "areaId": 1, "hideWorld": 0, },1286: { "worldId": 5, "name": "BeastCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },1282: { "worldId": 5, "name": "BelleRoom", "display": "Belle’s Room", "areaId": 2, "hideWorld": 0, },1287: { "worldId": 5, "name": "EastWing", "display": "The East Wing", "areaId": 7, "hideWorld": 0, },1284: { "worldId": 5, "name": "Ballroom", "display": "Ballroom", "areaId": 4, "hideWorld": 0, },1288: { "worldId": 5, "name": "WestHall", "display": "The West Hall", "areaId": 8, "hideWorld": 0, },1291: { "worldId": 5, "name": "Undercroft", "display": "Undercroft", "areaId": 11, "hideWorld": 0, },1290: { "worldId": 5, "name": "Dungeon", "display": "Dungeon", "areaId": 10, "hideWorld": 0, },1292: { "worldId": 5, "name": "SecretPassage", "display": "Secret Passage", "areaId": 12, "hideWorld": 0, },1289: { "worldId": 5, "name": "WestWing", "display": "The West Wing", "areaId": 9, "hideWorld": 0, },1283: { "worldId": 5, "name": "BeastRoom", "display": "The Beast’s Room", "areaId": 3, "hideWorld": 0, },1285: { "worldId": 5, "name": "BallroomBattle", "display": "Ballroom", "areaId": 5, "hideWorld": 0, },2304: { "worldId": 9, "name": "Book", "display": "The Hundred Acre Wood", "areaId": 0, "hideWorld": 1, },2306: { "worldId": 9, "name": "PoohHouse", "display": "Pooh Bear’s House", "areaId": 2, "hideWorld": 0, },1542: { "worldId": 6, "name": "HadesChamber", "display": "Hades’ Chamber", "areaId": 6, "hideWorld": 0, },1541: { "worldId": 6, "name": "ValleyOfTheDead", "display": "Valley of the Dead", "areaId": 5, "hideWorld": 0, },1546: { "worldId": 6, "name": "CaveOfTheDeadInnerChamber", "display": "Cave of the Dead: Inner Chamber", "areaId": 10, "hideWorld": 0, },1551: { "worldId": 6, "name": "CaveOfTheDeadPassage", "display": "Cave of the Dead: Passage", "areaId": 15, "hideWorld": 0, },1539: { "worldId": 6, "name": "UnderworldEntrance", "display": "Underworld Entrance", "areaId": 3, "hideWorld": 0, },1543: { "worldId": 6, "name": "CaveOfTheDeadEntrance", "display": "Cave of the Dead: Entrance", "areaId": 7, "hideWorld": 0, },1537: { "worldId": 6, "name": "ColiseumGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },1540: { "worldId": 6, "name": "ColiseumFoyer", "display": "Coliseum Foyer", "areaId": 4, "hideWorld": 0, },1536: { "worldId": 6, "name": "Coliseum", "display": "The Coliseum", "areaId": 0, "hideWorld": 0, },1547: { "worldId": 6, "name": "UnderworldCavernsEntrance", "display": "Underworld Caverns: Entrance", "areaId": 11, "hideWorld": 0, },1552: { "worldId": 6, "name": "UnderworldCavernsLostRoad", "display": "Underworld Caverns: The Lost Road", "areaId": 16, "hideWorld": 0, },1553: { "worldId": 6, "name": "UnderworldCavernsAtrium", "display": "Underworld Caverns: Atrium", "areaId": 17, "hideWorld": 0, },1548: { "worldId": 6, "name": "UnderworldLock", "display": "The Lock", "areaId": 12, "hideWorld": 0, },1544: { "worldId": 6, "name": "UnderworldLock2", "display": "The Lock", "areaId": 8, "hideWorld": 0, },1554: { "worldId": 6, "name": "ColiseumGatesRuined", "display": "Coliseum Gates", "areaId": 18, "hideWorld": 0, },3075: { "worldId": 12, "name": "CastleCourtyard", "display": "Courtyard", "areaId": 3, "hideWorld": 0, },3074: { "worldId": 12, "name": "CastleColonnade", "display": "Colonnade", "areaId": 2, "hideWorld": 0, },3073: { "worldId": 12, "name": "CastleLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },3072: { "worldId": 12, "name": "CastleAudienceChamber", "display": "Audience Chamber", "areaId": 0, "hideWorld": 0, },3076: { "worldId": 12, "name": "CastleCornerstone", "display": "The Hall of the Cornerstone", "areaId": 4, "hideWorld": 0, },3328: { "worldId": 13, "name": "RiverCornerstoneHill", "display": "Cornerstone Hill", "areaId": 0, "hideWorld": 0, },3329: { "worldId": 13, "name": "RiverPier", "display": "Pier", "areaId": 1, "hideWorld": 0, },3335: { "worldId": 13, "name": "MickeyHouse", "display": "Mickey’s House", "areaId": 7, "hideWorld": 0, },3334: { "worldId": 13, "name": "Fire", "display": "Scene of the Fire", "areaId": 6, "hideWorld": 0, },3332: { "worldId": 13, "name": "Lilliput", "display": "Lilliput", "areaId": 4, "hideWorld": 0, },3333: { "worldId": 13, "name": "BuildingSite", "display": "Building Site", "areaId": 5, "hideWorld": 0, },3336: { "worldId": 13, "name": "VillainFlashback", "display": "Villain’s Vale", "areaId": 8, "hideWorld": 1, },3331: { "worldId": 13, "name": "RiverWharf", "display": "Wharf", "areaId": 3, "hideWorld": 0, },3330: { "worldId": 13, "name": "RiverWaterway", "display": "Waterway", "areaId": 2, "hideWorld": 0, },4104: { "worldId": 16, "name": "PortRockFace", "display": "Isla de Muerta: Rock Face", "areaId": 8, "hideWorld": 0, },4105: { "worldId": 16, "name": "PortCaveMouth", "display": "Isla de Muerta: Cave Mouth", "areaId": 9, "hideWorld": 0, },4097: { "worldId": 16, "name": "PortHarbor", "display": "Harbor", "areaId": 1, "hideWorld": 0, },4098: { "worldId": 16, "name": "PortTown", "display": "Town", "areaId": 2, "hideWorld": 0, },4096: { "worldId": 16, "name": "PortRampart", "display": "Rampart", "areaId": 0, "hideWorld": 0, },4099: { "worldId": 16, "name": "PortInterceptor", "display": "The Interceptor", "areaId": 3, "hideWorld": 0, },4100: { "worldId": 16, "name": "PortInterceptorHold", "display": "The Interceptor: Ship’s Hold", "areaId": 4, "hideWorld": 0, },4117: { "worldId": 16, "name": "PortInterceptorBattle", "display": "The Interceptor", "areaId": 21, "hideWorld": 0, },4103: { "worldId": 16, "name": "PortInterceptorDualBattle", "display": "The Interceptor", "areaId": 7, "hideWorld": 0, },4108: { "worldId": 16, "name": "PortPowderStore", "display": "Isla de Muerta: Powder Store", "areaId": 12, "hideWorld": 0, },4109: { "worldId": 16, "name": "PortNook", "display": "Isla de Muerta: Moonlight Nook", "areaId": 13, "hideWorld": 0, },4106: { "worldId": 16, "name": "PortHeap", "display": "Isla de Muerta: Treasure Heap", "areaId": 10, "hideWorld": 0, },3586: { "worldId": 14, "name": "HalloweenGraveyard", "display": "Graveyard", "areaId": 2, "hideWorld": 0, },3585: { "worldId": 14, "name": "HalloweenLab", "display": "Dr. Finkelstein’s Lab", "areaId": 1, "hideWorld": 0, },3584: { "worldId": 14, "name": "HalloweenSquare", "display": "Halloween Town Square", "areaId": 0, "hideWorld": 1, },3588: { "worldId": 14, "name": "HalloweenHinterlands", "display": "Hinterlands", "areaId": 4, "hideWorld": 0, },3589: { "worldId": 14, "name": "HalloweenYuletide", "display": "Christmas Town: Yuletide Hill", "areaId": 5, "hideWorld": 1, },3590: { "worldId": 14, "name": "HalloweenCandyCane", "display": "Christmas Town: Candy Cane Lane", "areaId": 6, "hideWorld": 1, },3592: { "worldId": 14, "name": "HalloweenSanta", "display": "Christmas Town: Santa’s House", "areaId": 8, "hideWorld": 1, },3587: { "worldId": 14, "name": "HalloweenHill", "display": "Curly Hill", "areaId": 3, "hideWorld": 0, },3593: { "worldId": 14, "name": "HalloweenFactory", "display": "Christmas Town: Toy Factory: Shipping and Receiving", "areaId": 9, "hideWorld": 1, },1794: { "worldId": 7, "name": "AgrabahShop", "display": "The Peddler’s Shop", "areaId": 2, "hideWorld": 0, },1792: { "worldId": 7, "name": "Agrabah", "display": "Agrabah", "areaId": 0, "hideWorld": 1, },1793: { "worldId": 7, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 1, "hideWorld": 0, },1798: { "worldId": 7, "name": "AgrabahWalls", "display": "Palace Walls", "areaId": 6, "hideWorld": 0, },1799: { "worldId": 7, "name": "AgrabahCaveEntrance", "display": "The Cave of Wonders: Entrance", "areaId": 7, "hideWorld": 0, },1804: { "worldId": 7, "name": "AgrabahCaveValley", "display": "The Cave of Wonders: Valley of Stone", "areaId": 12, "hideWorld": 0, },1801: { "worldId": 7, "name": "AgrabahCaveGuardians", "display": "The Cave of Wonders: Stone Guardians", "areaId": 9, "hideWorld": 0, },1805: { "worldId": 7, "name": "AgrabahCaveChasm", "display": "The Cave of Wonders: Chasm of Challenges", "areaId": 13, "hideWorld": 0, },1802: { "worldId": 7, "name": "AgrabahCaveTreasure", "display": "The Cave of Wonders: Treasure Room", "areaId": 10, "hideWorld": 0, },1795: { "worldId": 7, "name": "AgrabahPalace", "display": "The Palace", "areaId": 3, "hideWorld": 0, },2566: { "worldId": 10, "name": "PrideGorge", "display": "Gorge", "areaId": 6, "hideWorld": 0, },2565: { "worldId": 10, "name": "PrideGraveyard", "display": "Elephant Graveyard", "areaId": 5, "hideWorld": 0, },2564: { "worldId": 10, "name": "PrideSavannah", "display": "The Savannah", "areaId": 4, "hideWorld": 0, },2560: { "worldId": 10, "name": "PrideRock", "display": "Pride Rock", "areaId": 0, "hideWorld": 0, },2561: { "worldId": 10, "name": "PrideHollow", "display": "Stone Hollow", "areaId": 1, "hideWorld": 0, },2563: { "worldId": 10, "name": "PrideValley", "display": "Wildebeest Valley", "areaId": 3, "hideWorld": 0, },2567: { "worldId": 10, "name": "PrideWastelands", "display": "Wastelands", "areaId": 7, "hideWorld": 0, },2568: { "worldId": 10, "name": "PrideJungle", "display": "Jungle", "areaId": 8, "hideWorld": 0, },2569: { "worldId": 10, "name": "PrideOasis", "display": "Oasis", "areaId": 9, "hideWorld": 0, },2562: { "worldId": 10, "name": "PrideDen", "display": "The King’s Den", "areaId": 2, "hideWorld": 0, },2573: { "worldId": 10, "name": "PridePeak", "display": "Peak", "areaId": 13, "hideWorld": 0, },2574: { "worldId": 10, "name": "PridePeakBattle", "display": "Peak", "areaId": 14, "hideWorld": 0, },1545: { "worldId": 6, "name": "ColiseumTourney1", "display": "The Underdrome", "areaId": 9, "hideWorld": 0, },1549: { "worldId": 6, "name": "ColiseumVictory", "display": "The Underdrome", "areaId": 13, "hideWorld": 0, },4112: { "worldId": 16, "name": "PortRockFace2", "display": "Isla de Muerta: Rock Face", "areaId": 16, "hideWorld": 0, },1032: { "worldId": 4, "name": "Bailey", "display": "Bailey", "areaId": 8, "hideWorld": 0, },1031: { "worldId": 4, "name": "RestorationSite", "display": "Restoration Site", "areaId": 7, "hideWorld": 0, },1030: { "worldId": 4, "name": "Postern", "display": "Postern", "areaId": 6, "hideWorld": 0, },1035: { "worldId": 4, "name": "Corridors", "display": "Corridors", "areaId": 11, "hideWorld": 0, },1029: { "worldId": 4, "name": "AnsemStudy", "display": "Ansem’s Study", "areaId": 5, "hideWorld": 0, },4352: { "worldId": 17, "name": "SpaceCell", "display": "Pit Cell", "areaId": 0, "hideWorld": 0, },4353: { "worldId": 17, "name": "SpaceCanyon", "display": "Canyon", "areaId": 1, "hideWorld": 0, },4354: { "worldId": 17, "name": "SpaceGrid", "display": "Game Grid", "areaId": 2, "hideWorld": 0, },4355: { "worldId": 17, "name": "SpaceDataspace", "display": "Dataspace", "areaId": 3, "hideWorld": 0, },4356: { "worldId": 17, "name": "SpaceIOTowerHallway", "display": "I/O Tower: Hallway", "areaId": 4, "hideWorld": 0, },4357: { "worldId": 17, "name": "SpaceIOCommunications", "display": "I/O Tower: Communications Room", "areaId": 5, "hideWorld": 0, },1043: { "worldId": 4, "name": "RestorationSiteCutscene", "display": "Restoration Site", "areaId": 19, "hideWorld": 0, },1044: { "worldId": 4, "name": "CorridorsBattle", "display": "Corridors", "areaId": 20, "hideWorld": 0, },1045: { "worldId": 4, "name": "CavernDepths", "display": "Cavern of Remembrance: Depths", "areaId": 21, "hideWorld": 1, },1042: { "worldId": 4, "name": "RestorationSiteCutscene2", "display": "Restoration Site", "areaId": 18, "hideWorld": 0, },1028: { "worldId": 4, "name": "CastleGate", "display": "Castle Gate", "areaId": 4, "hideWorld": 0, },1040: { "worldId": 4, "name": "RavineTrail", "display": "Ravine Trail", "areaId": 16, "hideWorld": 0, },1027: { "worldId": 4, "name": "CrystalFissure", "display": "Crystal Fissure", "areaId": 3, "hideWorld": 0, },1026: { "worldId": 4, "name": "GreatMawCutscene", "display": "The Great Maw", "areaId": 2, "hideWorld": 0, },1039: { "worldId": 4, "name": "AnsemStudyCutscene", "display": "Ansem’s Study", "areaId": 15, "hideWorld": 0, },1041: { "worldId": 4, "name": "GreatMaw", "display": "The Great Maw", "areaId": 17, "hideWorld": 0, },2058: { "worldId": 8, "name": "DragonAntechamber", "display": "Antechamber", "areaId": 10, "hideWorld": 0, },2059: { "worldId": 8, "name": "DragonThrone", "display": "Throne Room", "areaId": 11, "hideWorld": 0, },1295: { "worldId": 5, "name": "BeastBridge", "display": "Bridge", "areaId": 15, "hideWorld": 0, },1555: { "worldId": 6, "name": "ColiseumTourneyHades", "display": "The Underdrome", "areaId": 19, "hideWorld": 0, },4101: { "worldId": 16, "name": "PortPearl", "display": "The Black Pearl", "areaId": 5, "hideWorld": 0, },4102: { "worldId": 16, "name": "PortPearlCaptain", "display": "The Black Pearl: Captain’s Stateroom", "areaId": 6, "hideWorld": 0, },4115: { "worldId": 16, "name": "PortPearlBattle", "display": "The Black Pearl", "areaId": 19, "hideWorld": 0, },4107: { "worldId": 16, "name": "PortGraveyardInterceptor", "display": "Ship Graveyard: The Interceptor’s Hold", "areaId": 11, "hideWorld": 0, },4111: { "worldId": 16, "name": "PortGraveyardRow", "display": "Ship Graveyard: Seadrift Row", "areaId": 15, "hideWorld": 0, },4110: { "worldId": 16, "name": "PortGraveyardKeep", "display": "Ship Graveyard: Seadrift Keep", "areaId": 14, "hideWorld": 0, },4120: { "worldId": 16, "name": "PortHarborCutscene", "display": "Harbor", "areaId": 24, "hideWorld": 0, },3594: { "worldId": 14, "name": "HalloweenWrapping", "display": "Christmas Town: The Wrapping Room", "areaId": 10, "hideWorld": 1, },3591: { "worldId": 14, "name": "HalloweenPlaza", "display": "Christmas Town: Christmas Tree Plaza", "areaId": 7, "hideWorld": 1, },1807: { "worldId": 7, "name": "AgrabahShop2", "display": "The Peddler’s Shop", "areaId": 15, "hideWorld": 0, },1806: { "worldId": 7, "name": "AgrabahSand", "display": "Sandswept Ruins", "areaId": 14, "hideWorld": 0, },1803: { "worldId": 7, "name": "AgrabahRuin", "display": "Ruined Chamber", "areaId": 11, "hideWorld": 0, },1797: { "worldId": 7, "name": "AgrabahAbove", "display": "Above the City", "areaId": 5, "hideWorld": 0, },2575: { "worldId": 10, "name": "PrideSavannahBattle", "display": "The Savannah", "areaId": 15, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6153,36 +6204,271 @@
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="n">
         <f aca="false">B175+C175*256</f>
-        <v>0</v>
+        <v>3594</v>
+      </c>
+      <c r="B175" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C175" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F175" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G175" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A175,": { ""worldId"": ",C175,", ""name"": """,D175,""", ""display"": """,E175,""", ""areaId"": ",B175,", ""hideWorld"": ",F175,", },")</f>
+        <v>3594: { "worldId": 14, "name": "HalloweenWrapping", "display": "Christmas Town: The Wrapping Room", "areaId": 10, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
         <f aca="false">B176+C176*256</f>
-        <v>0</v>
+        <v>3591</v>
+      </c>
+      <c r="B176" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C176" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F176" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G176" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A176,": { ""worldId"": ",C176,", ""name"": """,D176,""", ""display"": """,E176,""", ""areaId"": ",B176,", ""hideWorld"": ",F176,", },")</f>
+        <v>3591: { "worldId": 14, "name": "HalloweenPlaza", "display": "Christmas Town: Christmas Tree Plaza", "areaId": 7, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="n">
         <f aca="false">B177+C177*256</f>
-        <v>0</v>
+        <v>1807</v>
+      </c>
+      <c r="B177" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C177" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G177" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A177,": { ""worldId"": ",C177,", ""name"": """,D177,""", ""display"": """,E177,""", ""areaId"": ",B177,", ""hideWorld"": ",F177,", },")</f>
+        <v>1807: { "worldId": 7, "name": "AgrabahShop2", "display": "The Peddler’s Shop", "areaId": 15, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="n">
         <f aca="false">B178+C178*256</f>
-        <v>0</v>
+        <v>1806</v>
+      </c>
+      <c r="B178" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C178" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G178" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A178,": { ""worldId"": ",C178,", ""name"": """,D178,""", ""display"": """,E178,""", ""areaId"": ",B178,", ""hideWorld"": ",F178,", },")</f>
+        <v>1806: { "worldId": 7, "name": "AgrabahSand", "display": "Sandswept Ruins", "areaId": 14, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
         <f aca="false">B179+C179*256</f>
-        <v>0</v>
+        <v>1803</v>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C179" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G179" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A179,": { ""worldId"": ",C179,", ""name"": """,D179,""", ""display"": """,E179,""", ""areaId"": ",B179,", ""hideWorld"": ",F179,", },")</f>
+        <v>1803: { "worldId": 7, "name": "AgrabahRuin", "display": "Ruined Chamber", "areaId": 11, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
         <f aca="false">B180+C180*256</f>
+        <v>1797</v>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C180" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G180" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A180,": { ""worldId"": ",C180,", ""name"": """,D180,""", ""display"": """,E180,""", ""areaId"": ",B180,", ""hideWorld"": ",F180,", },")</f>
+        <v>1797: { "worldId": 7, "name": "AgrabahAbove", "display": "Above the City", "areaId": 5, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="n">
+        <f aca="false">B181+C181*256</f>
+        <v>2575</v>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C181" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G181" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A181,": { ""worldId"": ",C181,", ""name"": """,D181,""", ""display"": """,E181,""", ""areaId"": ",B181,", ""hideWorld"": ",F181,", },")</f>
+        <v>2575: { "worldId": 10, "name": "PrideSavannahBattle", "display": "The Savannah", "areaId": 15, "hideWorld": 0, },</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="n">
+        <f aca="false">B182+C182*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="n">
+        <f aca="false">B183+C183*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="n">
+        <f aca="false">B184+C184*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="n">
+        <f aca="false">B185+C185*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="n">
+        <f aca="false">B186+C186*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="n">
+        <f aca="false">B187+C187*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="n">
+        <f aca="false">B188+C188*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="n">
+        <f aca="false">B189+C189*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="n">
+        <f aca="false">B190+C190*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="n">
+        <f aca="false">B191+C191*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="n">
+        <f aca="false">B192+C192*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="n">
+        <f aca="false">B193+C193*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="n">
+        <f aca="false">B194+C194*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="n">
+        <f aca="false">B195+C195*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="n">
+        <f aca="false">B196+C196*256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="n">
+        <f aca="false">B197+C197*256</f>
         <v>0</v>
       </c>
     </row>
@@ -6221,22 +6507,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -6246,18 +6532,18 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 },"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 },"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 },"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -6281,7 +6567,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -6299,13 +6585,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -6329,7 +6615,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -6347,13 +6633,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -6377,7 +6663,7 @@
         <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
@@ -6401,7 +6687,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -6425,7 +6711,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
@@ -6443,13 +6729,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -6467,13 +6753,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
@@ -6497,7 +6783,7 @@
         <v>225</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -6521,7 +6807,7 @@
         <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
@@ -6539,13 +6825,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -6569,7 +6855,7 @@
         <v>269</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -6587,13 +6873,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -6617,7 +6903,7 @@
         <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -6641,7 +6927,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -6665,7 +6951,7 @@
         <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -6689,7 +6975,7 @@
         <v>307</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -6707,13 +6993,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -6737,7 +7023,7 @@
         <v>312</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -6755,13 +7041,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
@@ -6785,7 +7071,7 @@
         <v>193</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -6798,7 +7084,79 @@
       </c>
       <c r="G24" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C24,""": { ""locationCode"": """,B24,""", ""eventId"": 0x",A24,", ""score"": ",E24,", ""isBoss"": ",D24,", ""lv1"": ",F24," }, ")</f>
-        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C25,""": { ""locationCode"": """,B25,""", ""eventId"": 0x",A25,", ""score"": ",E25,", ""isBoss"": ",D25,", ""lv1"": ",F25," }, ")</f>
+        <v>"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C26,""": { ""locationCode"": """,B26,""", ""eventId"": 0x",A26,", ""score"": ",E26,", ""isBoss"": ",D26,", ""lv1"": ",F26," }, ")</f>
+        <v>"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("""",C27,""": { ""locationCode"": """,B27,""", ""eventId"": 0x",A27,", ""score"": ",E27,", ""isBoss"": ",D27,", ""lv1"": ",F27," }, ")</f>
+        <v>"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6833,7 +7191,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6857,10 +7215,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>365</v>
+        <v>382</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""" },")</f>
@@ -6869,10 +7227,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""" },")</f>
@@ -6881,10 +7239,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""" },")</f>
@@ -6893,10 +7251,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""" },")</f>
@@ -6905,10 +7263,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""" },")</f>
@@ -6917,10 +7275,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>374</v>
+        <v>391</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""" },")</f>
@@ -6929,10 +7287,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""" },")</f>
@@ -6941,10 +7299,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""" },")</f>
@@ -6953,10 +7311,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""" },")</f>
@@ -6965,10 +7323,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""" },")</f>
@@ -6977,10 +7335,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""" },")</f>
@@ -7062,16 +7420,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>386</v>
+        <v>403</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -7086,13 +7444,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -7104,13 +7462,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -7122,13 +7480,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>411</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -7140,13 +7498,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>396</v>
+        <v>413</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -7158,13 +7516,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>397</v>
+        <v>414</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -7176,13 +7534,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -7194,13 +7552,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -7212,13 +7570,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>404</v>
+        <v>421</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -7230,13 +7588,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
@@ -7248,13 +7606,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>3</v>
@@ -7266,13 +7624,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
@@ -7284,13 +7642,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>412</v>
+        <v>429</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>3</v>
@@ -7302,13 +7660,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>413</v>
+        <v>430</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>3</v>
@@ -7320,13 +7678,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>3</v>
@@ -7338,13 +7696,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>3</v>
@@ -7356,13 +7714,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>420</v>
+        <v>437</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3</v>
@@ -7374,13 +7732,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>421</v>
+        <v>438</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>422</v>
+        <v>439</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>3</v>
@@ -7392,13 +7750,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>423</v>
+        <v>440</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
@@ -7410,13 +7768,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>3</v>
@@ -7428,13 +7786,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>427</v>
+        <v>444</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>428</v>
+        <v>445</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
@@ -7480,25 +7838,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>429</v>
+        <v>446</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>430</v>
+        <v>447</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>431</v>
+        <v>448</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7552,13 +7910,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>436</v>
+        <v>453</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7615,16 +7973,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>441</v>
+        <v>458</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7683,7 +8041,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>443</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Refactored newest three achievements to use the generator
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="1151">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -3203,6 +3203,9 @@
   </si>
   <si>
     <t xml:space="preserve">Generate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Score Address</t>
   </si>
   <si>
     <t xml:space="preserve">Struggle?</t>
@@ -3930,7 +3933,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C234" activeCellId="0" sqref="C234"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9826,7 +9829,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G62" activeCellId="0" sqref="G62"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18315,10 +18318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18331,8 +18334,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18376,19 +18380,22 @@
         <v>1059</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(N2:N1000)</f>
-        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "" },5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "" },8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora." },9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora." },10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora." },11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "" },13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "" },15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "" },16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="Q1" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(O2:O1000)</f>
+        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora.", "useScore": 0, },9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora.", "useScore": 0, },10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora.", "useScore": 0, },11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>14</v>
@@ -18397,7 +18404,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>10</v>
@@ -18409,13 +18416,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>488</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>1</v>
@@ -18423,14 +18430,17 @@
       <c r="L2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A2,""", ""basicTarget"": ",B2,", ""basicScore"": ",C2,", ""advancedName"": """,D2,""", ""advancedTarget"": ",E2,", ""advancedScore"": ",F2,", ""lowerIsBetter"": ",G2,", ""description"": """,H2,""", ""eventKey"": """,I2,""", ""leaderboardDesc"": """,J2,""", ""generate"": ",K2,", ""struggle"": ",L2,", ""struggleDesc"": """,M2,""" },")</f>
-        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A2,""", ""basicTarget"": ",B2,", ""basicScore"": ",C2,", ""advancedName"": """,D2,""", ""advancedTarget"": ",E2,", ""advancedScore"": ",F2,", ""lowerIsBetter"": ",G2,", ""description"": """,H2,""", ""eventKey"": """,I2,""", ""leaderboardDesc"": """,J2,""", ""generate"": ",K2,", ""struggle"": ",M2,", ""struggleDesc"": """,N2,""", ""useScore"": ",L2,", },")</f>
+        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>15</v>
@@ -18439,7 +18449,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>7.5</v>
@@ -18451,13 +18461,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>490</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>1</v>
@@ -18465,14 +18475,17 @@
       <c r="L3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A3,""", ""basicTarget"": ",B3,", ""basicScore"": ",C3,", ""advancedName"": """,D3,""", ""advancedTarget"": ",E3,", ""advancedScore"": ",F3,", ""lowerIsBetter"": ",G3,", ""description"": """,H3,""", ""eventKey"": """,I3,""", ""leaderboardDesc"": """,J3,""", ""generate"": ",K3,", ""struggle"": ",L3,", ""struggleDesc"": """,M3,""" },")</f>
-        <v>3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A3,""", ""basicTarget"": ",B3,", ""basicScore"": ",C3,", ""advancedName"": """,D3,""", ""advancedTarget"": ",E3,", ""advancedScore"": ",F3,", ""lowerIsBetter"": ",G3,", ""description"": """,H3,""", ""eventKey"": """,I3,""", ""leaderboardDesc"": """,J3,""", ""generate"": ",K3,", ""struggle"": ",M3,", ""struggleDesc"": """,N3,""", ""useScore"": ",L3,", },")</f>
+        <v>3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>70</v>
@@ -18481,7 +18494,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>100</v>
@@ -18493,13 +18506,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>492</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>0</v>
@@ -18507,14 +18520,17 @@
       <c r="L4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A4,""", ""basicTarget"": ",B4,", ""basicScore"": ",C4,", ""advancedName"": """,D4,""", ""advancedTarget"": ",E4,", ""advancedScore"": ",F4,", ""lowerIsBetter"": ",G4,", ""description"": """,H4,""", ""eventKey"": """,I4,""", ""leaderboardDesc"": """,J4,""", ""generate"": ",K4,", ""struggle"": ",L4,", ""struggleDesc"": """,M4,""" },")</f>
-        <v>4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A4,""", ""basicTarget"": ",B4,", ""basicScore"": ",C4,", ""advancedName"": """,D4,""", ""advancedTarget"": ",E4,", ""advancedScore"": ",F4,", ""lowerIsBetter"": ",G4,", ""description"": """,H4,""", ""eventKey"": """,I4,""", ""leaderboardDesc"": """,J4,""", ""generate"": ",K4,", ""struggle"": ",M4,", ""struggleDesc"": """,N4,""", ""useScore"": ",L4,", },")</f>
+        <v>4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>50</v>
@@ -18523,7 +18539,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>30</v>
@@ -18535,13 +18551,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>494</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>1</v>
@@ -18549,14 +18565,17 @@
       <c r="L5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A5,""", ""basicTarget"": ",B5,", ""basicScore"": ",C5,", ""advancedName"": """,D5,""", ""advancedTarget"": ",E5,", ""advancedScore"": ",F5,", ""lowerIsBetter"": ",G5,", ""description"": """,H5,""", ""eventKey"": """,I5,""", ""leaderboardDesc"": """,J5,""", ""generate"": ",K5,", ""struggle"": ",L5,", ""struggleDesc"": """,M5,""" },")</f>
-        <v>5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A5,""", ""basicTarget"": ",B5,", ""basicScore"": ",C5,", ""advancedName"": """,D5,""", ""advancedTarget"": ",E5,", ""advancedScore"": ",F5,", ""lowerIsBetter"": ",G5,", ""description"": """,H5,""", ""eventKey"": """,I5,""", ""leaderboardDesc"": """,J5,""", ""generate"": ",K5,", ""struggle"": ",M5,", ""struggleDesc"": """,N5,""", ""useScore"": ",L5,", },")</f>
+        <v>5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>15</v>
@@ -18565,7 +18584,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>10</v>
@@ -18577,13 +18596,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>496</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>1</v>
@@ -18591,14 +18610,17 @@
       <c r="L6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A6,""", ""basicTarget"": ",B6,", ""basicScore"": ",C6,", ""advancedName"": """,D6,""", ""advancedTarget"": ",E6,", ""advancedScore"": ",F6,", ""lowerIsBetter"": ",G6,", ""description"": """,H6,""", ""eventKey"": """,I6,""", ""leaderboardDesc"": """,J6,""", ""generate"": ",K6,", ""struggle"": ",L6,", ""struggleDesc"": """,M6,""" },")</f>
-        <v>6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A6,""", ""basicTarget"": ",B6,", ""basicScore"": ",C6,", ""advancedName"": """,D6,""", ""advancedTarget"": ",E6,", ""advancedScore"": ",F6,", ""lowerIsBetter"": ",G6,", ""description"": """,H6,""", ""eventKey"": """,I6,""", ""leaderboardDesc"": """,J6,""", ""generate"": ",K6,", ""struggle"": ",M6,", ""struggleDesc"": """,N6,""", ""useScore"": ",L6,", },")</f>
+        <v>6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>10</v>
@@ -18607,7 +18629,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -18619,13 +18641,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>498</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>0</v>
@@ -18633,14 +18655,17 @@
       <c r="L7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A7,""", ""basicTarget"": ",B7,", ""basicScore"": ",C7,", ""advancedName"": """,D7,""", ""advancedTarget"": ",E7,", ""advancedScore"": ",F7,", ""lowerIsBetter"": ",G7,", ""description"": """,H7,""", ""eventKey"": """,I7,""", ""leaderboardDesc"": """,J7,""", ""generate"": ",K7,", ""struggle"": ",L7,", ""struggleDesc"": """,M7,""" },")</f>
-        <v>7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A7,""", ""basicTarget"": ",B7,", ""basicScore"": ",C7,", ""advancedName"": """,D7,""", ""advancedTarget"": ",E7,", ""advancedScore"": ",F7,", ""lowerIsBetter"": ",G7,", ""description"": """,H7,""", ""eventKey"": """,I7,""", ""leaderboardDesc"": """,J7,""", ""generate"": ",K7,", ""struggle"": ",M7,", ""struggleDesc"": """,N7,""", ""useScore"": ",L7,", },")</f>
+        <v>7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0</v>
@@ -18649,7 +18674,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>30</v>
@@ -18661,31 +18686,34 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>500</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>1088</v>
-      </c>
-      <c r="N8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A8,""", ""basicTarget"": ",B8,", ""basicScore"": ",C8,", ""advancedName"": """,D8,""", ""advancedTarget"": ",E8,", ""advancedScore"": ",F8,", ""lowerIsBetter"": ",G8,", ""description"": """,H8,""", ""eventKey"": """,I8,""", ""leaderboardDesc"": """,J8,""", ""generate"": ",K8,", ""struggle"": ",L8,", ""struggleDesc"": """,M8,""" },")</f>
-        <v>8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora." },</v>
+      <c r="N8" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A8,""", ""basicTarget"": ",B8,", ""basicScore"": ",C8,", ""advancedName"": """,D8,""", ""advancedTarget"": ",E8,", ""advancedScore"": ",F8,", ""lowerIsBetter"": ",G8,", ""description"": """,H8,""", ""eventKey"": """,I8,""", ""leaderboardDesc"": """,J8,""", ""generate"": ",K8,", ""struggle"": ",M8,", ""struggleDesc"": """,N8,""", ""useScore"": ",L8,", },")</f>
+        <v>8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora.", "useScore": 0, },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -18694,7 +18722,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>30</v>
@@ -18706,31 +18734,34 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>502</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>1093</v>
-      </c>
-      <c r="N9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A9,""", ""basicTarget"": ",B9,", ""basicScore"": ",C9,", ""advancedName"": """,D9,""", ""advancedTarget"": ",E9,", ""advancedScore"": ",F9,", ""lowerIsBetter"": ",G9,", ""description"": """,H9,""", ""eventKey"": """,I9,""", ""leaderboardDesc"": """,J9,""", ""generate"": ",K9,", ""struggle"": ",L9,", ""struggleDesc"": """,M9,""" },")</f>
-        <v>9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora." },</v>
+      <c r="N9" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A9,""", ""basicTarget"": ",B9,", ""basicScore"": ",C9,", ""advancedName"": """,D9,""", ""advancedTarget"": ",E9,", ""advancedScore"": ",F9,", ""lowerIsBetter"": ",G9,", ""description"": """,H9,""", ""eventKey"": """,I9,""", ""leaderboardDesc"": """,J9,""", ""generate"": ",K9,", ""struggle"": ",M9,", ""struggleDesc"": """,N9,""", ""useScore"": ",L9,", },")</f>
+        <v>9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora.", "useScore": 0, },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0</v>
@@ -18739,7 +18770,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>30</v>
@@ -18751,31 +18782,34 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>504</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>1098</v>
-      </c>
-      <c r="N10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A10,""", ""basicTarget"": ",B10,", ""basicScore"": ",C10,", ""advancedName"": """,D10,""", ""advancedTarget"": ",E10,", ""advancedScore"": ",F10,", ""lowerIsBetter"": ",G10,", ""description"": """,H10,""", ""eventKey"": """,I10,""", ""leaderboardDesc"": """,J10,""", ""generate"": ",K10,", ""struggle"": ",L10,", ""struggleDesc"": """,M10,""" },")</f>
-        <v>10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora." },</v>
+      <c r="N10" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A10,""", ""basicTarget"": ",B10,", ""basicScore"": ",C10,", ""advancedName"": """,D10,""", ""advancedTarget"": ",E10,", ""advancedScore"": ",F10,", ""lowerIsBetter"": ",G10,", ""description"": """,H10,""", ""eventKey"": """,I10,""", ""leaderboardDesc"": """,J10,""", ""generate"": ",K10,", ""struggle"": ",M10,", ""struggleDesc"": """,N10,""", ""useScore"": ",L10,", },")</f>
+        <v>10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora.", "useScore": 0, },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>1000</v>
@@ -18784,7 +18818,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2000</v>
@@ -18796,13 +18830,13 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>506</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>0</v>
@@ -18810,14 +18844,17 @@
       <c r="L11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A11,""", ""basicTarget"": ",B11,", ""basicScore"": ",C11,", ""advancedName"": """,D11,""", ""advancedTarget"": ",E11,", ""advancedScore"": ",F11,", ""lowerIsBetter"": ",G11,", ""description"": """,H11,""", ""eventKey"": """,I11,""", ""leaderboardDesc"": """,J11,""", ""generate"": ",K11,", ""struggle"": ",L11,", ""struggleDesc"": """,M11,""" },")</f>
-        <v>11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A11,""", ""basicTarget"": ",B11,", ""basicScore"": ",C11,", ""advancedName"": """,D11,""", ""advancedTarget"": ",E11,", ""advancedScore"": ",F11,", ""lowerIsBetter"": ",G11,", ""description"": """,H11,""", ""eventKey"": """,I11,""", ""leaderboardDesc"": """,J11,""", ""generate"": ",K11,", ""struggle"": ",M11,", ""struggleDesc"": """,N11,""", ""useScore"": ",L11,", },")</f>
+        <v>11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1000</v>
@@ -18826,7 +18863,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>2000</v>
@@ -18838,13 +18875,13 @@
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="K12" s="1" t="n">
         <v>0</v>
@@ -18852,14 +18889,17 @@
       <c r="L12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N12" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A12,""", ""basicTarget"": ",B12,", ""basicScore"": ",C12,", ""advancedName"": """,D12,""", ""advancedTarget"": ",E12,", ""advancedScore"": ",F12,", ""lowerIsBetter"": ",G12,", ""description"": """,H12,""", ""eventKey"": """,I12,""", ""leaderboardDesc"": """,J12,""", ""generate"": ",K12,", ""struggle"": ",L12,", ""struggleDesc"": """,M12,""" },")</f>
-        <v>12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A12,""", ""basicTarget"": ",B12,", ""basicScore"": ",C12,", ""advancedName"": """,D12,""", ""advancedTarget"": ",E12,", ""advancedScore"": ",F12,", ""lowerIsBetter"": ",G12,", ""description"": """,H12,""", ""eventKey"": """,I12,""", ""leaderboardDesc"": """,J12,""", ""generate"": ",K12,", ""struggle"": ",M12,", ""struggleDesc"": """,N12,""", ""useScore"": ",L12,", },")</f>
+        <v>12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>200</v>
@@ -18868,7 +18908,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>500</v>
@@ -18880,13 +18920,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>516</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>0</v>
@@ -18894,14 +18934,17 @@
       <c r="L13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N13" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A13,""", ""basicTarget"": ",B13,", ""basicScore"": ",C13,", ""advancedName"": """,D13,""", ""advancedTarget"": ",E13,", ""advancedScore"": ",F13,", ""lowerIsBetter"": ",G13,", ""description"": """,H13,""", ""eventKey"": """,I13,""", ""leaderboardDesc"": """,J13,""", ""generate"": ",K13,", ""struggle"": ",L13,", ""struggleDesc"": """,M13,""" },")</f>
-        <v>13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A13,""", ""basicTarget"": ",B13,", ""basicScore"": ",C13,", ""advancedName"": """,D13,""", ""advancedTarget"": ",E13,", ""advancedScore"": ",F13,", ""lowerIsBetter"": ",G13,", ""description"": """,H13,""", ""eventKey"": """,I13,""", ""leaderboardDesc"": """,J13,""", ""generate"": ",K13,", ""struggle"": ",M13,", ""struggleDesc"": """,N13,""", ""useScore"": ",L13,", },")</f>
+        <v>13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>40</v>
@@ -18910,7 +18953,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>16.5</v>
@@ -18922,13 +18965,13 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>517</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>1</v>
@@ -18936,14 +18979,17 @@
       <c r="L14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N14" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A14,""", ""basicTarget"": ",B14,", ""basicScore"": ",C14,", ""advancedName"": """,D14,""", ""advancedTarget"": ",E14,", ""advancedScore"": ",F14,", ""lowerIsBetter"": ",G14,", ""description"": """,H14,""", ""eventKey"": """,I14,""", ""leaderboardDesc"": """,J14,""", ""generate"": ",K14,", ""struggle"": ",L14,", ""struggleDesc"": """,M14,""" },")</f>
-        <v>14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A14,""", ""basicTarget"": ",B14,", ""basicScore"": ",C14,", ""advancedName"": """,D14,""", ""advancedTarget"": ",E14,", ""advancedScore"": ",F14,", ""lowerIsBetter"": ",G14,", ""description"": """,H14,""", ""eventKey"": """,I14,""", ""leaderboardDesc"": """,J14,""", ""generate"": ",K14,", ""struggle"": ",M14,", ""struggleDesc"": """,N14,""", ""useScore"": ",L14,", },")</f>
+        <v>14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>10</v>
@@ -18952,7 +18998,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>35</v>
@@ -18964,13 +19010,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>519</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>0</v>
@@ -18978,14 +19024,17 @@
       <c r="L15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N15" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A15,""", ""basicTarget"": ",B15,", ""basicScore"": ",C15,", ""advancedName"": """,D15,""", ""advancedTarget"": ",E15,", ""advancedScore"": ",F15,", ""lowerIsBetter"": ",G15,", ""description"": """,H15,""", ""eventKey"": """,I15,""", ""leaderboardDesc"": """,J15,""", ""generate"": ",K15,", ""struggle"": ",L15,", ""struggleDesc"": """,M15,""" },")</f>
-        <v>15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A15,""", ""basicTarget"": ",B15,", ""basicScore"": ",C15,", ""advancedName"": """,D15,""", ""advancedTarget"": ",E15,", ""advancedScore"": ",F15,", ""lowerIsBetter"": ",G15,", ""description"": """,H15,""", ""eventKey"": """,I15,""", ""leaderboardDesc"": """,J15,""", ""generate"": ",K15,", ""struggle"": ",M15,", ""struggleDesc"": """,N15,""", ""useScore"": ",L15,", },")</f>
+        <v>15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>1000</v>
@@ -18994,7 +19043,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>1500</v>
@@ -19006,13 +19055,13 @@
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>520</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>0</v>
@@ -19020,14 +19069,17 @@
       <c r="L16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N16" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A16,""", ""basicTarget"": ",B16,", ""basicScore"": ",C16,", ""advancedName"": """,D16,""", ""advancedTarget"": ",E16,", ""advancedScore"": ",F16,", ""lowerIsBetter"": ",G16,", ""description"": """,H16,""", ""eventKey"": """,I16,""", ""leaderboardDesc"": """,J16,""", ""generate"": ",K16,", ""struggle"": ",L16,", ""struggleDesc"": """,M16,""" },")</f>
-        <v>16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+      <c r="M16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A16,""", ""basicTarget"": ",B16,", ""basicScore"": ",C16,", ""advancedName"": """,D16,""", ""advancedTarget"": ",E16,", ""advancedScore"": ",F16,", ""lowerIsBetter"": ",G16,", ""description"": """,H16,""", ""eventKey"": """,I16,""", ""leaderboardDesc"": """,J16,""", ""generate"": ",K16,", ""struggle"": ",M16,", ""struggleDesc"": """,N16,""", ""useScore"": ",L16,", },")</f>
+        <v>16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>20</v>
@@ -19036,7 +19088,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>30</v>
@@ -19048,28 +19100,31 @@
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>522</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A17,""", ""basicTarget"": ",B17,", ""basicScore"": ",C17,", ""advancedName"": """,D17,""", ""advancedTarget"": ",E17,", ""advancedScore"": ",F17,", ""lowerIsBetter"": ",G17,", ""description"": """,H17,""", ""eventKey"": """,I17,""", ""leaderboardDesc"": """,J17,""", ""generate"": ",K17,", ""struggle"": ",L17,", ""struggleDesc"": """,M17,""" },")</f>
-        <v>17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A17,""", ""basicTarget"": ",B17,", ""basicScore"": ",C17,", ""advancedName"": """,D17,""", ""advancedTarget"": ",E17,", ""advancedScore"": ",F17,", ""lowerIsBetter"": ",G17,", ""description"": """,H17,""", ""eventKey"": """,I17,""", ""leaderboardDesc"": """,J17,""", ""generate"": ",K17,", ""struggle"": ",M17,", ""struggleDesc"": """,N17,""", ""useScore"": ",L17,", },")</f>
+        <v>17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>18000</v>
@@ -19078,7 +19133,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>19900</v>
@@ -19090,28 +19145,31 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>523</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A18,""", ""basicTarget"": ",B18,", ""basicScore"": ",C18,", ""advancedName"": """,D18,""", ""advancedTarget"": ",E18,", ""advancedScore"": ",F18,", ""lowerIsBetter"": ",G18,", ""description"": """,H18,""", ""eventKey"": """,I18,""", ""leaderboardDesc"": """,J18,""", ""generate"": ",K18,", ""struggle"": ",L18,", ""struggleDesc"": """,M18,""" },")</f>
-        <v>18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+        <v>1</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A18,""", ""basicTarget"": ",B18,", ""basicScore"": ",C18,", ""advancedName"": """,D18,""", ""advancedTarget"": ",E18,", ""advancedScore"": ",F18,", ""lowerIsBetter"": ",G18,", ""description"": """,H18,""", ""eventKey"": """,I18,""", ""leaderboardDesc"": """,J18,""", ""generate"": ",K18,", ""struggle"": ",M18,", ""struggleDesc"": """,N18,""", ""useScore"": ",L18,", },")</f>
+        <v>18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>8000</v>
@@ -19120,7 +19178,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>10000</v>
@@ -19132,23 +19190,26 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>524</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A19,""", ""basicTarget"": ",B19,", ""basicScore"": ",C19,", ""advancedName"": """,D19,""", ""advancedTarget"": ",E19,", ""advancedScore"": ",F19,", ""lowerIsBetter"": ",G19,", ""description"": """,H19,""", ""eventKey"": """,I19,""", ""leaderboardDesc"": """,J19,""", ""generate"": ",K19,", ""struggle"": ",L19,", ""struggleDesc"": """,M19,""" },")</f>
-        <v>19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 0, "struggle": 0, "struggleDesc": "" },</v>
+        <v>1</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A19,""", ""basicTarget"": ",B19,", ""basicScore"": ",C19,", ""advancedName"": """,D19,""", ""advancedTarget"": ",E19,", ""advancedScore"": ",F19,", ""lowerIsBetter"": ",G19,", ""description"": """,H19,""", ""eventKey"": """,I19,""", ""leaderboardDesc"": """,J19,""", ""generate"": ",K19,", ""struggle"": ",M19,", ""struggleDesc"": """,N19,""", ""useScore"": ",L19,", },")</f>
+        <v>19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
   </sheetData>
@@ -19187,25 +19248,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19259,13 +19320,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19322,16 +19383,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19390,7 +19451,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Refactored the Sand Slider and Workshop Raver achievements to use the generator
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -18321,7 +18321,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18390,7 +18390,7 @@
       </c>
       <c r="Q1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(O2:O1000)</f>
-        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora.", "useScore": 0, },9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora.", "useScore": 0, },10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora.", "useScore": 0, },11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
+        <v>2: { "basicName": "Overachieving Courier", "basicTarget": 14, "basicScore": 3, "advancedName": "Professional Courier", "advancedTarget": 10, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Mail Delivery minigame in {0} seconds or less.", "eventKey": "Mail Delivery", "leaderboardDesc": "Deliver mail as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },3: { "basicName": "Overachieving Packmule", "basicTarget": 15, "basicScore": 3, "advancedName": "Professional Packmule", "advancedTarget": 7.5, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Cargo Climb minigame in {0} seconds or less.", "eventKey": "Cargo Climb", "leaderboardDesc": "Push the cargo to the garage as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },4: { "basicName": "Overachieving Showoff", "basicTarget": 70, "basicScore": 3, "advancedName": "Professional Showoff", "advancedTarget": 100, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Grandstander minigame with a score of {0} or more points.", "eventKey": "Grandstander", "leaderboardDesc": "Hit the ball as many times as you can before it touches the ground!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },5: { "basicName": "Overachieving Mounter", "basicTarget": 50, "basicScore": 5, "advancedName": "Professional Mounter", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Poster Duty minigame in {0} seconds or less.", "eventKey": "Poster Duty", "leaderboardDesc": "Put up 20 posters as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },6: { "basicName": "Overachieving Exterminator", "basicTarget": 15, "basicScore": 5, "advancedName": "Professional Exterminator", "advancedTarget": 10, "advancedScore": 10, "lowerIsBetter": 1, "description": "Complete the Bumble-Buster minigame in {0} seconds or less.", "eventKey": "Bumble-Buster", "leaderboardDesc": "Get rid of all the bees as quickly as you can!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },7: { "basicName": "Overachieving Garbageman", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Garbageman", "advancedTarget": 6, "advancedScore": 5, "lowerIsBetter": 1, "description": "Complete the Junk Sweep minigame in {0} swings or fewer.", "eventKey": "Junk Sweep", "leaderboardDesc": "Get rid of all the junk in as few swings as possible!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },8: { "basicName": "Overseeded – Hayner", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Semifinalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Hayner with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Hayner", "leaderboardDesc": "Win a Struggle match against Hayner by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Hayner by knockout within {0} as Sora.", "useScore": 0, },9: { "basicName": "Overseeded – Setzer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Finalist", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Setzer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Setzer", "leaderboardDesc": "Win a Struggle match against Setzer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Setzer by knockout within {0} as Sora.", "useScore": 0, },10: { "basicName": "Overseeded – Seifer", "basicTarget": 0, "basicScore": 3, "advancedName": "Struggle Champion", "advancedTarget": 30, "advancedScore": 5, "lowerIsBetter": 1, "description": "Win a Struggle match against Seifer with a margin of 100 or more points as Sora.", "eventKey": "Struggle: Seifer", "leaderboardDesc": "Win a Struggle match against Seifer by knockout as quickly as possible!", "generate": 1, "struggle": 1, "struggleDesc": "Win a Struggle match against Seifer by knockout within {0} as Sora.", "useScore": 0, },11: { "basicName": "Overachieving Street Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Street Raver", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Street Rave minigame with a score of {0} or more points.", "eventKey": "Skateboard Street Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Street Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },12: { "basicName": "Overachieving Trainee", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Trainee", "advancedTarget": 2000, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete Phil's Training on Maniac Mode with a score of {0} or more points.", "eventKey": "Phil’s Training – Maniac Mode", "leaderboardDesc": "Get as many points as you can in Phil’s Training on Maniac Mode!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },13: { "basicName": "Overachieving Freestyler", "basicTarget": 200, "basicScore": 3, "advancedName": "Professional Freestyler", "advancedTarget": 500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Freestyle minigame with a score of {0} or more points.", "eventKey": "Skateboard Freestyle", "leaderboardDesc": "Get as many points as you can in the Skateboard Freestyle minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },14: { "basicName": "Overachieving Speedrunner", "basicTarget": 40, "basicScore": 3, "advancedName": "Professional Speedrunner", "advancedTarget": 16.5, "advancedScore": 25, "lowerIsBetter": 1, "description": "Complete the Skateboard Time Attack minigame in {0} seconds or less.", "eventKey": "Skateboard Time Attack", "leaderboardDesc": "Ride through all the checkpoints as fast as possible!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 0, },15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },17: { "basicName": "Overachieving Cyclist", "basicTarget": 20, "basicScore": 3, "advancedName": "Professional Cyclist", "advancedTarget": 30, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Light Cycle minigame with a score of {0} or more.", "eventKey": "Light Cycle", "leaderboardDesc": "Get as many points as you can in the Light Cycle minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },18: { "basicName": "Overachieving Rescuer", "basicTarget": 18000, "basicScore": 3, "advancedName": "Professional Rescuer", "advancedTarget": 19900, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Blustery Rescue minigame with a score of {0} or more.", "eventKey": "A Blustery Rescue", "leaderboardDesc": "Get as many points as you can in the Blustery Rescue minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },19: { "basicName": "Overachieving Gatherer", "basicTarget": 8000, "basicScore": 3, "advancedName": "Professional Gatherer", "advancedTarget": 10000, "advancedScore": 25, "lowerIsBetter": 0, "description": "Complete the Hunny Slider minigame with a score of {0} or more.", "eventKey": "Hunny Slider", "leaderboardDesc": "Get as many points as you can in the Hunny Slider minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19019,17 +19019,17 @@
         <v>1119</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A15,""", ""basicTarget"": ",B15,", ""basicScore"": ",C15,", ""advancedName"": """,D15,""", ""advancedTarget"": ",E15,", ""advancedScore"": ",F15,", ""lowerIsBetter"": ",G15,", ""description"": """,H15,""", ""eventKey"": """,I15,""", ""leaderboardDesc"": """,J15,""", ""generate"": ",K15,", ""struggle"": ",M15,", ""struggleDesc"": """,N15,""", ""useScore"": ",L15,", },")</f>
-        <v>15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
+        <v>15: { "basicName": "Overachieving Slider", "basicTarget": 10, "basicScore": 3, "advancedName": "Professional Slider", "advancedTarget": 35, "advancedScore": 10, "lowerIsBetter": 0, "description": "Complete the Skateboard Sand Slider minigame with a score of {0} or more.", "eventKey": "Skateboard Sand Slider", "leaderboardDesc": "Ride through as many checkpoints as you can before time runs out!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19064,17 +19064,17 @@
         <v>1123</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(ROW(),": { ", ,"""basicName"": """,A16,""", ""basicTarget"": ",B16,", ""basicScore"": ",C16,", ""advancedName"": """,D16,""", ""advancedTarget"": ",E16,", ""advancedScore"": ",F16,", ""lowerIsBetter"": ",G16,", ""description"": """,H16,""", ""eventKey"": """,I16,""", ""leaderboardDesc"": """,J16,""", ""generate"": ",K16,", ""struggle"": ",M16,", ""struggleDesc"": """,N16,""", ""useScore"": ",L16,", },")</f>
-        <v>16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 0, "struggle": 0, "struggleDesc": "", "useScore": 0, },</v>
+        <v>16: { "basicName": "Overachieving Workshop Raver", "basicTarget": 1000, "basicScore": 3, "advancedName": "Professional Workshop Raver", "advancedTarget": 1500, "advancedScore": 5, "lowerIsBetter": 0, "description": "Complete the Skateboard Workshop Rave minigame with a score of {0} or more.", "eventKey": "Skateboard Workshop Rave", "leaderboardDesc": "Get as many points as you can in the Skateboard Workshop Rave minigame!", "generate": 1, "struggle": 0, "struggleDesc": "", "useScore": 1, },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added EX Mission achievements
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="1270">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -3616,31 +3616,229 @@
     <t xml:space="preserve">Gate ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Mission 1 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission 1 Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission 2 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission 2 Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission 3 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission 3 Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 1 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 1 Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 2 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 2 Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 3 Base Addr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Mission 3 Score</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asteroid Sweep</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033bc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bc50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bc90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c2d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c350</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stardust Sweep</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033bcd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bd10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bd50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c3d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c410</t>
+  </si>
+  <si>
     <t xml:space="preserve">Broken Highway</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033bd90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bdd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033be10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c4d0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ancient Highway</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033be50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033be90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bed0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c590</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phantom Storm</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033bf10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bf50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033bf90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c5d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c650</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sunlight Storm</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033bfd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c6d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c710</t>
+  </si>
+  <si>
     <t xml:space="preserve">Splash Island</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033c090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c0d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c7d0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Floating Island</t>
   </si>
   <si>
+    <t xml:space="preserve">0x0033c150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c1d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c890</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assault of the Dreadnought</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c8d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0033c950</t>
   </si>
 </sst>
 </file>
@@ -3772,7 +3970,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="E11:E12 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4087,7 +4285,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D178" activeCellId="1" sqref="E11:E12 D178"/>
+      <selection pane="bottomLeft" activeCell="D178" activeCellId="0" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10377,7 +10575,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B74" activeCellId="1" sqref="E11:E12 B74"/>
+      <selection pane="bottomLeft" activeCell="B74" activeCellId="0" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10417,7 +10615,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 }, "Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 }, "Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, "Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, "Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, "Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, "Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 }, "Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 }, "Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, "Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 }, "MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 }, "Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 }, "Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 }, "Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 }, "Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 }, "Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 }, "Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 }, "Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 }, "Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 }, "Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 }, "Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 }, "Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 }, "Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 }, "Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 }, "Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 }, "Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 }, "Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 }, "Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 }, "Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 }, "A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 }, "The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 }, "Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 }, "Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 }, "Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 }, "Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 }, "Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 }, "Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, "Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, "Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, "Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, "Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 }, "Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 }, "Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, "Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 }, "MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 }, "Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 }, "Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 }, "Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 }, "Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 }, "Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 }, "Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 }, "Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 }, "Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 }, "Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 }, "Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 }, "Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 }, "Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 }, "Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 }, "Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 }, "Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 }, "Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 }, "Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 }, "Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 }, "A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 }, "The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 }, "Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 }, "Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 }, "Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 }, "Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10441,7 +10639,7 @@
       </c>
       <c r="G2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2,", ""lv1"": ",F2," }, ")</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10465,7 +10663,7 @@
       </c>
       <c r="G3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3,", ""lv1"": ",F3," }, ")</f>
-        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10489,7 +10687,7 @@
       </c>
       <c r="G4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4,", ""lv1"": ",F4," }, ")</f>
-        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10513,7 +10711,7 @@
       </c>
       <c r="G5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5,", ""lv1"": ",F5," }, ")</f>
-        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10537,7 +10735,7 @@
       </c>
       <c r="G6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6,", ""lv1"": ",F6," }, ")</f>
-        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10561,7 +10759,7 @@
       </c>
       <c r="G7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7,", ""lv1"": ",F7," }, ")</f>
-        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10585,7 +10783,7 @@
       </c>
       <c r="G8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8,", ""lv1"": ",F8," }, ")</f>
-        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10609,7 +10807,7 @@
       </c>
       <c r="G9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9,", ""lv1"": ",F9," }, ")</f>
-        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10633,7 +10831,7 @@
       </c>
       <c r="G10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10,", ""lv1"": ",F10," }, ")</f>
-        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10657,7 +10855,7 @@
       </c>
       <c r="G11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11,", ""lv1"": ",F11," }, ")</f>
-        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10681,7 +10879,7 @@
       </c>
       <c r="G12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12,", ""lv1"": ",F12," }, ")</f>
-        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10705,7 +10903,7 @@
       </c>
       <c r="G13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13,", ""lv1"": ",F13," }, ")</f>
-        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10729,7 +10927,7 @@
       </c>
       <c r="G14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14,", ""lv1"": ",F14," }, ")</f>
-        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10753,7 +10951,7 @@
       </c>
       <c r="G15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15,", ""lv1"": ",F15," }, ")</f>
-        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10777,7 +10975,7 @@
       </c>
       <c r="G16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C16,""": { ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16,", ""lv1"": ",F16," }, ")</f>
-        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10801,7 +10999,7 @@
       </c>
       <c r="G17" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C17,""": { ""locationCode"": """,B17,""", ""eventId"": 0x",A17,", ""score"": ",E17,", ""isBoss"": ",D17,", ""lv1"": ",F17," }, ")</f>
-        <v>"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10825,7 +11023,7 @@
       </c>
       <c r="G18" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C18,""": { ""locationCode"": """,B18,""", ""eventId"": 0x",A18,", ""score"": ",E18,", ""isBoss"": ",D18,", ""lv1"": ",F18," }, ")</f>
-        <v>"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10849,7 +11047,7 @@
       </c>
       <c r="G19" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C19,""": { ""locationCode"": """,B19,""", ""eventId"": 0x",A19,", ""score"": ",E19,", ""isBoss"": ",D19,", ""lv1"": ",F19," }, ")</f>
-        <v>"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10873,7 +11071,7 @@
       </c>
       <c r="G20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C20,""": { ""locationCode"": """,B20,""", ""eventId"": 0x",A20,", ""score"": ",E20,", ""isBoss"": ",D20,", ""lv1"": ",F20," }, ")</f>
-        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
+        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10897,7 +11095,7 @@
       </c>
       <c r="G21" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C21,""": { ""locationCode"": """,B21,""", ""eventId"": 0x",A21,", ""score"": ",E21,", ""isBoss"": ",D21,", ""lv1"": ",F21," }, ")</f>
-        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10921,7 +11119,7 @@
       </c>
       <c r="G22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C22,""": { ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22," }, ")</f>
-        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10945,7 +11143,7 @@
       </c>
       <c r="G23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C23,""": { ""locationCode"": """,B23,""", ""eventId"": 0x",A23,", ""score"": ",E23,", ""isBoss"": ",D23,", ""lv1"": ",F23," }, ")</f>
-        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10969,7 +11167,7 @@
       </c>
       <c r="G24" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C24,""": { ""locationCode"": """,B24,""", ""eventId"": 0x",A24,", ""score"": ",E24,", ""isBoss"": ",D24,", ""lv1"": ",F24," }, ")</f>
-        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10993,7 +11191,7 @@
       </c>
       <c r="G25" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C25,""": { ""locationCode"": """,B25,""", ""eventId"": 0x",A25,", ""score"": ",E25,", ""isBoss"": ",D25,", ""lv1"": ",F25," }, ")</f>
-        <v>"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11017,7 +11215,7 @@
       </c>
       <c r="G26" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C26,""": { ""locationCode"": """,B26,""", ""eventId"": 0x",A26,", ""score"": ",E26,", ""isBoss"": ",D26,", ""lv1"": ",F26," }, ")</f>
-        <v>"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11041,7 +11239,7 @@
       </c>
       <c r="G27" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C27,""": { ""locationCode"": """,B27,""", ""eventId"": 0x",A27,", ""score"": ",E27,", ""isBoss"": ",D27,", ""lv1"": ",F27," }, ")</f>
-        <v>"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11065,7 +11263,7 @@
       </c>
       <c r="G28" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C28,""": { ""locationCode"": """,B28,""", ""eventId"": 0x",A28,", ""score"": ",E28,", ""isBoss"": ",D28,", ""lv1"": ",F28," }, ")</f>
-        <v>"Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11089,7 +11287,7 @@
       </c>
       <c r="G29" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C29,""": { ""locationCode"": """,B29,""", ""eventId"": 0x",A29,", ""score"": ",E29,", ""isBoss"": ",D29,", ""lv1"": ",F29," }, ")</f>
-        <v>"Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11113,7 +11311,7 @@
       </c>
       <c r="G30" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C30,""": { ""locationCode"": """,B30,""", ""eventId"": 0x",A30,", ""score"": ",E30,", ""isBoss"": ",D30,", ""lv1"": ",F30," }, ")</f>
-        <v>"MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11137,7 +11335,7 @@
       </c>
       <c r="G31" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C31,""": { ""locationCode"": """,B31,""", ""eventId"": 0x",A31,", ""score"": ",E31,", ""isBoss"": ",D31,", ""lv1"": ",F31," }, ")</f>
-        <v>"Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11161,7 +11359,7 @@
       </c>
       <c r="G32" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C32,""": { ""locationCode"": """,B32,""", ""eventId"": 0x",A32,", ""score"": ",E32,", ""isBoss"": ",D32,", ""lv1"": ",F32," }, ")</f>
-        <v>"Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11185,7 +11383,7 @@
       </c>
       <c r="G33" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C33,""": { ""locationCode"": """,B33,""", ""eventId"": 0x",A33,", ""score"": ",E33,", ""isBoss"": ",D33,", ""lv1"": ",F33," }, ")</f>
-        <v>"Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11209,7 +11407,7 @@
       </c>
       <c r="G34" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C34,""": { ""locationCode"": """,B34,""", ""eventId"": 0x",A34,", ""score"": ",E34,", ""isBoss"": ",D34,", ""lv1"": ",F34," }, ")</f>
-        <v>"Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11233,7 +11431,7 @@
       </c>
       <c r="G35" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C35,""": { ""locationCode"": """,B35,""", ""eventId"": 0x",A35,", ""score"": ",E35,", ""isBoss"": ",D35,", ""lv1"": ",F35," }, ")</f>
-        <v>"Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11257,7 +11455,7 @@
       </c>
       <c r="G36" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C36,""": { ""locationCode"": """,B36,""", ""eventId"": 0x",A36,", ""score"": ",E36,", ""isBoss"": ",D36,", ""lv1"": ",F36," }, ")</f>
-        <v>"Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11281,7 +11479,7 @@
       </c>
       <c r="G37" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C37,""": { ""locationCode"": """,B37,""", ""eventId"": 0x",A37,", ""score"": ",E37,", ""isBoss"": ",D37,", ""lv1"": ",F37," }, ")</f>
-        <v>"Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11305,7 +11503,7 @@
       </c>
       <c r="G38" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C38,""": { ""locationCode"": """,B38,""", ""eventId"": 0x",A38,", ""score"": ",E38,", ""isBoss"": ",D38,", ""lv1"": ",F38," }, ")</f>
-        <v>"Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11329,7 +11527,7 @@
       </c>
       <c r="G39" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C39,""": { ""locationCode"": """,B39,""", ""eventId"": 0x",A39,", ""score"": ",E39,", ""isBoss"": ",D39,", ""lv1"": ",F39," }, ")</f>
-        <v>"Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11353,7 +11551,7 @@
       </c>
       <c r="G40" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C40,""": { ""locationCode"": """,B40,""", ""eventId"": 0x",A40,", ""score"": ",E40,", ""isBoss"": ",D40,", ""lv1"": ",F40," }, ")</f>
-        <v>"Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11377,7 +11575,7 @@
       </c>
       <c r="G41" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C41,""": { ""locationCode"": """,B41,""", ""eventId"": 0x",A41,", ""score"": ",E41,", ""isBoss"": ",D41,", ""lv1"": ",F41," }, ")</f>
-        <v>"Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11401,7 +11599,7 @@
       </c>
       <c r="G42" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C42,""": { ""locationCode"": """,B42,""", ""eventId"": 0x",A42,", ""score"": ",E42,", ""isBoss"": ",D42,", ""lv1"": ",F42," }, ")</f>
-        <v>"Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11425,7 +11623,7 @@
       </c>
       <c r="G43" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C43,""": { ""locationCode"": """,B43,""", ""eventId"": 0x",A43,", ""score"": ",E43,", ""isBoss"": ",D43,", ""lv1"": ",F43," }, ")</f>
-        <v>"Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11449,7 +11647,7 @@
       </c>
       <c r="G44" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C44,""": { ""locationCode"": """,B44,""", ""eventId"": 0x",A44,", ""score"": ",E44,", ""isBoss"": ",D44,", ""lv1"": ",F44," }, ")</f>
-        <v>"Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11473,7 +11671,7 @@
       </c>
       <c r="G45" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C45,""": { ""locationCode"": """,B45,""", ""eventId"": 0x",A45,", ""score"": ",E45,", ""isBoss"": ",D45,", ""lv1"": ",F45," }, ")</f>
-        <v>"Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11497,7 +11695,7 @@
       </c>
       <c r="G46" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C46,""": { ""locationCode"": """,B46,""", ""eventId"": 0x",A46,", ""score"": ",E46,", ""isBoss"": ",D46,", ""lv1"": ",F46," }, ")</f>
-        <v>"Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11521,7 +11719,7 @@
       </c>
       <c r="G47" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C47,""": { ""locationCode"": """,B47,""", ""eventId"": 0x",A47,", ""score"": ",E47,", ""isBoss"": ",D47,", ""lv1"": ",F47," }, ")</f>
-        <v>"Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11545,7 +11743,7 @@
       </c>
       <c r="G48" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C48,""": { ""locationCode"": """,B48,""", ""eventId"": 0x",A48,", ""score"": ",E48,", ""isBoss"": ",D48,", ""lv1"": ",F48," }, ")</f>
-        <v>"Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11569,7 +11767,7 @@
       </c>
       <c r="G49" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C49,""": { ""locationCode"": """,B49,""", ""eventId"": 0x",A49,", ""score"": ",E49,", ""isBoss"": ",D49,", ""lv1"": ",F49," }, ")</f>
-        <v>"Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11593,7 +11791,7 @@
       </c>
       <c r="G50" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C50,""": { ""locationCode"": """,B50,""", ""eventId"": 0x",A50,", ""score"": ",E50,", ""isBoss"": ",D50,", ""lv1"": ",F50," }, ")</f>
-        <v>"Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11617,7 +11815,7 @@
       </c>
       <c r="G51" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C51,""": { ""locationCode"": """,B51,""", ""eventId"": 0x",A51,", ""score"": ",E51,", ""isBoss"": ",D51,", ""lv1"": ",F51," }, ")</f>
-        <v>"Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11641,7 +11839,7 @@
       </c>
       <c r="G52" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C52,""": { ""locationCode"": """,B52,""", ""eventId"": 0x",A52,", ""score"": ",E52,", ""isBoss"": ",D52,", ""lv1"": ",F52," }, ")</f>
-        <v>"Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11665,7 +11863,7 @@
       </c>
       <c r="G53" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C53,""": { ""locationCode"": """,B53,""", ""eventId"": 0x",A53,", ""score"": ",E53,", ""isBoss"": ",D53,", ""lv1"": ",F53," }, ")</f>
-        <v>"Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11689,7 +11887,7 @@
       </c>
       <c r="G54" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C54,""": { ""locationCode"": """,B54,""", ""eventId"": 0x",A54,", ""score"": ",E54,", ""isBoss"": ",D54,", ""lv1"": ",F54," }, ")</f>
-        <v>"Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
+        <v>"Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 },</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11713,7 +11911,7 @@
       </c>
       <c r="G55" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C55,""": { ""locationCode"": """,B55,""", ""eventId"": 0x",A55,", ""score"": ",E55,", ""isBoss"": ",D55,", ""lv1"": ",F55," }, ")</f>
-        <v>"Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11737,7 +11935,7 @@
       </c>
       <c r="G56" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C56,""": { ""locationCode"": """,B56,""", ""eventId"": 0x",A56,", ""score"": ",E56,", ""isBoss"": ",D56,", ""lv1"": ",F56," }, ")</f>
-        <v>"Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11761,7 +11959,7 @@
       </c>
       <c r="G57" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C57,""": { ""locationCode"": """,B57,""", ""eventId"": 0x",A57,", ""score"": ",E57,", ""isBoss"": ",D57,", ""lv1"": ",F57," }, ")</f>
-        <v>"Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11785,7 +11983,7 @@
       </c>
       <c r="G58" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C58,""": { ""locationCode"": """,B58,""", ""eventId"": 0x",A58,", ""score"": ",E58,", ""isBoss"": ",D58,", ""lv1"": ",F58," }, ")</f>
-        <v>"Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11809,7 +12007,7 @@
       </c>
       <c r="G59" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C59,""": { ""locationCode"": """,B59,""", ""eventId"": 0x",A59,", ""score"": ",E59,", ""isBoss"": ",D59,", ""lv1"": ",F59," }, ")</f>
-        <v>"Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11833,7 +12031,7 @@
       </c>
       <c r="G60" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C60,""": { ""locationCode"": """,B60,""", ""eventId"": 0x",A60,", ""score"": ",E60,", ""isBoss"": ",D60,", ""lv1"": ",F60," }, ")</f>
-        <v>"Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11857,7 +12055,7 @@
       </c>
       <c r="G61" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C61,""": { ""locationCode"": """,B61,""", ""eventId"": 0x",A61,", ""score"": ",E61,", ""isBoss"": ",D61,", ""lv1"": ",F61," }, ")</f>
-        <v>"A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11881,7 +12079,7 @@
       </c>
       <c r="G62" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C62,""": { ""locationCode"": """,B62,""", ""eventId"": 0x",A62,", ""score"": ",E62,", ""isBoss"": ",D62,", ""lv1"": ",F62," }, ")</f>
-        <v>"Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11905,7 +12103,7 @@
       </c>
       <c r="G63" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C63,""": { ""locationCode"": """,B63,""", ""eventId"": 0x",A63,", ""score"": ",E63,", ""isBoss"": ",D63,", ""lv1"": ",F63," }, ")</f>
-        <v>"Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11929,7 +12127,7 @@
       </c>
       <c r="G64" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C64,""": { ""locationCode"": """,B64,""", ""eventId"": 0x",A64,", ""score"": ",E64,", ""isBoss"": ",D64,", ""lv1"": ",F64," }, ")</f>
-        <v>"The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11953,7 +12151,7 @@
       </c>
       <c r="G65" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C65,""": { ""locationCode"": """,B65,""", ""eventId"": 0x",A65,", ""score"": ",E65,", ""isBoss"": ",D65,", ""lv1"": ",F65," }, ")</f>
-        <v>"The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11977,7 +12175,7 @@
       </c>
       <c r="G66" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C66,""": { ""locationCode"": """,B66,""", ""eventId"": 0x",A66,", ""score"": ",E66,", ""isBoss"": ",D66,", ""lv1"": ",F66," }, ")</f>
-        <v>"Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12001,7 +12199,7 @@
       </c>
       <c r="G67" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C67,""": { ""locationCode"": """,B67,""", ""eventId"": 0x",A67,", ""score"": ",E67,", ""isBoss"": ",D67,", ""lv1"": ",F67," }, ")</f>
-        <v>"Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12025,7 +12223,7 @@
       </c>
       <c r="G68" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C68,""": { ""locationCode"": """,B68,""", ""eventId"": 0x",A68,", ""score"": ",E68,", ""isBoss"": ",D68,", ""lv1"": ",F68," }, ")</f>
-        <v>"Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12049,7 +12247,7 @@
       </c>
       <c r="G69" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C69,""": { ""locationCode"": """,B69,""", ""eventId"": 0x",A69,", ""score"": ",E69,", ""isBoss"": ",D69,", ""lv1"": ",F69," }, ")</f>
-        <v>"Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12073,7 +12271,7 @@
       </c>
       <c r="G70" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C70,""": { ""locationCode"": """,B70,""", ""eventId"": 0x",A70,", ""score"": ",E70,", ""isBoss"": ",D70,", ""lv1"": ",F70," }, ")</f>
-        <v>"A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12097,7 +12295,7 @@
       </c>
       <c r="G71" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C71,""": { ""locationCode"": """,B71,""", ""eventId"": 0x",A71,", ""score"": ",E71,", ""isBoss"": ",D71,", ""lv1"": ",F71," }, ")</f>
-        <v>"Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12121,7 +12319,7 @@
       </c>
       <c r="G72" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C72,""": { ""locationCode"": """,B72,""", ""eventId"": 0x",A72,", ""score"": ",E72,", ""isBoss"": ",D72,", ""lv1"": ",F72," }, ")</f>
-        <v>"Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12145,7 +12343,7 @@
       </c>
       <c r="G73" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C73,""": { ""locationCode"": """,B73,""", ""eventId"": 0x",A73,", ""score"": ",E73,", ""isBoss"": ",D73,", ""lv1"": ",F73," }, ")</f>
-        <v>"Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
+        <v>"Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12170,7 +12368,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="E11:E12 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12397,7 +12595,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="1" sqref="E11:E12 A29"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19134,7 +19332,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="E11:E12 A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20266,16 +20464,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E11:E12"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="1" width="12.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20286,180 +20487,540 @@
         <v>1194</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1202</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1204</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>1205</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(C2:C10000)</f>
-        <v>2: { "name": "Asteroid Sweep", "gateId": 0, },3: { "name": "Stardust Sweep", "gateId": 1, },4: { "name": "Broken Highway", "gateId": 2, },5: { "name": "Ancient Highway", "gateId": 3, },6: { "name": "Phantom Storm", "gateId": 4, },7: { "name": "Sunlight Storm", "gateId": 5, },8: { "name": "Splash Island", "gateId": 6, },9: { "name": "Floating Island", "gateId": 7, },10: { "name": "Assault of the Dreadnought", "gateId": 8, },</v>
+      <c r="Q1" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(O2:O10000)</f>
+        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1195</v>
+        <v>1207</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A2,""", ""gateId"": ",B2,", },")</f>
-        <v>2: { "name": "Asteroid Sweep", "gateId": 0, },</v>
+      <c r="C2" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A2,""", ""gateId"": ",B2,", ""miss1BaseAddr"": ",C2,", ""miss1EXBaseAddr"": ",I2,", ""mission1Score"": ",D2,", ""mission2Score"": ",F2,", ""mission3Score"": ",H2,", ""exMission1Score"": ",J2,", ""exMission2Score"": ",L2,", ""exMission3Score"": ",N2," },")</f>
+        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1196</v>
+        <v>1214</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A3,""", ""gateId"": ",B3,", },")</f>
-        <v>3: { "name": "Stardust Sweep", "gateId": 1, },</v>
+      <c r="C3" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A3,""", ""gateId"": ",B3,", ""miss1BaseAddr"": ",C3,", ""miss1EXBaseAddr"": ",I3,", ""mission1Score"": ",D3,", ""mission2Score"": ",F3,", ""mission3Score"": ",H3,", ""exMission1Score"": ",J3,", ""exMission2Score"": ",L3,", ""exMission3Score"": ",N3," },")</f>
+        <v>3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1197</v>
+        <v>1221</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A4,""", ""gateId"": ",B4,", },")</f>
-        <v>4: { "name": "Broken Highway", "gateId": 2, },</v>
+      <c r="C4" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A4,""", ""gateId"": ",B4,", ""miss1BaseAddr"": ",C4,", ""miss1EXBaseAddr"": ",I4,", ""mission1Score"": ",D4,", ""mission2Score"": ",F4,", ""mission3Score"": ",H4,", ""exMission1Score"": ",J4,", ""exMission2Score"": ",L4,", ""exMission3Score"": ",N4," },")</f>
+        <v>4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1198</v>
+        <v>1228</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A5,""", ""gateId"": ",B5,", },")</f>
-        <v>5: { "name": "Ancient Highway", "gateId": 3, },</v>
+      <c r="C5" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A5,""", ""gateId"": ",B5,", ""miss1BaseAddr"": ",C5,", ""miss1EXBaseAddr"": ",I5,", ""mission1Score"": ",D5,", ""mission2Score"": ",F5,", ""mission3Score"": ",H5,", ""exMission1Score"": ",J5,", ""exMission2Score"": ",L5,", ""exMission3Score"": ",N5," },")</f>
+        <v>5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1199</v>
+        <v>1235</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A6,""", ""gateId"": ",B6,", },")</f>
-        <v>6: { "name": "Phantom Storm", "gateId": 4, },</v>
+      <c r="C6" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A6,""", ""gateId"": ",B6,", ""miss1BaseAddr"": ",C6,", ""miss1EXBaseAddr"": ",I6,", ""mission1Score"": ",D6,", ""mission2Score"": ",F6,", ""mission3Score"": ",H6,", ""exMission1Score"": ",J6,", ""exMission2Score"": ",L6,", ""exMission3Score"": ",N6," },")</f>
+        <v>6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1200</v>
+        <v>1242</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A7,""", ""gateId"": ",B7,", },")</f>
-        <v>7: { "name": "Sunlight Storm", "gateId": 5, },</v>
+      <c r="C7" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A7,""", ""gateId"": ",B7,", ""miss1BaseAddr"": ",C7,", ""miss1EXBaseAddr"": ",I7,", ""mission1Score"": ",D7,", ""mission2Score"": ",F7,", ""mission3Score"": ",H7,", ""exMission1Score"": ",J7,", ""exMission2Score"": ",L7,", ""exMission3Score"": ",N7," },")</f>
+        <v>7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1201</v>
+        <v>1249</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A8,""", ""gateId"": ",B8,", },")</f>
-        <v>8: { "name": "Splash Island", "gateId": 6, },</v>
+      <c r="C8" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A8,""", ""gateId"": ",B8,", ""miss1BaseAddr"": ",C8,", ""miss1EXBaseAddr"": ",I8,", ""mission1Score"": ",D8,", ""mission2Score"": ",F8,", ""mission3Score"": ",H8,", ""exMission1Score"": ",J8,", ""exMission2Score"": ",L8,", ""exMission3Score"": ",N8," },")</f>
+        <v>8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1202</v>
+        <v>1256</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A9,""", ""gateId"": ",B9,", },")</f>
-        <v>9: { "name": "Floating Island", "gateId": 7, },</v>
+      <c r="C9" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A9,""", ""gateId"": ",B9,", ""miss1BaseAddr"": ",C9,", ""miss1EXBaseAddr"": ",I9,", ""mission1Score"": ",D9,", ""mission2Score"": ",F9,", ""mission3Score"": ",H9,", ""exMission1Score"": ",J9,", ""exMission2Score"": ",L9,", ""exMission3Score"": ",N9," },")</f>
+        <v>9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1203</v>
+        <v>1263</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A10,""", ""gateId"": ",B10,", },")</f>
-        <v>10: { "name": "Assault of the Dreadnought", "gateId": 8, },</v>
+      <c r="C10" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A10,""", ""gateId"": ",B10,", ""miss1BaseAddr"": ",C10,", ""miss1EXBaseAddr"": ",I10,", ""mission1Score"": ",D10,", ""mission2Score"": ",F10,", ""mission3Score"": ",H10,", ""exMission1Score"": ",J10,", ""exMission2Score"": ",L10,", ""exMission3Score"": ",N10," },")</f>
+        <v>10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1"/>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1"/>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1"/>
+      <c r="O15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1"/>
+      <c r="O16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
+      <c r="O17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+      <c r="O18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1"/>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="1"/>
+      <c r="O22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="1"/>
+      <c r="O24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="1"/>
+      <c r="O25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="1"/>
+      <c r="O26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="1"/>
+      <c r="O27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="1"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added Synthesis achievements and updated the save protection to allow for them
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="Minigames" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Gummi Ship Missions" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Puzzle Pieces" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Treasure Chests" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Locations!$C$1:$C$250</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2759" uniqueCount="1353">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -3831,6 +3832,264 @@
   </si>
   <si>
     <t xml:space="preserve">0x0032dffd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dedc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dedd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythril Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP Boost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frost Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torn Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cornerstone Hill Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi-Potion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythril Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frost Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star Recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blazing Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blazing Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Boost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underworld Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032dee9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caverns Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032deea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucid Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032deeb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega Recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032deec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032deed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basement Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucid Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032deef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halloween Town Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serenity Gem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightning Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega Potion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythril Gem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightning Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas Town Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naval Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bright Shard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather Charm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukulele Charm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032def9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100-Acre Wood Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032defa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032defb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orichalcum+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythril Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serenity Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orichalcum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultimate Recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tower Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df0a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df0b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bright Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0032df0c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Crystal</t>
   </si>
 </sst>
 </file>
@@ -3870,12 +4129,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3912,7 +4183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3929,7 +4200,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3951,6 +4234,66 @@
       </fill>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -4278,7 +4621,7 @@
   </sheetPr>
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F254" activeCellId="0" sqref="F254"/>
@@ -10711,7 +11054,7 @@
       </c>
       <c r="I1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1006)</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 },"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 },"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 },"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 },"Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },"Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 },"MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },"Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 },"Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 },"Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 },"Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 },"Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 },"Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },"Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },"Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 },"Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 },"Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 },"Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 },"Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 },"Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 },"Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 },"Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 },"Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 },"Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 },"Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 },"Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 },"Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 },"Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 },"Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 },"Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 },"Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 },"Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 },"Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 },"Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 },"Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 },"Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 },"Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 },"A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },"Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },"Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 },"The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },"The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 },"Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 },"Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 },"Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 },"Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },"A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },"Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },"Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },"Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 }, "Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 }, "Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 }, "Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 }, "Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 }, "Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 }, "Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 }, "Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 }, "Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 }, "Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 }, "Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 }, "Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 }, "Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 }, "Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, "Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, "Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, "Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, "Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, "Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, "Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, "Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 }, "Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 }, "Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, "Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 }, "MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 }, "Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 }, "Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 }, "Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 }, "Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, "Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 }, "Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 }, "Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 }, "Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 }, "Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 }, "Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 }, "Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 }, "Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 }, "Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 }, "Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 }, "Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 }, "Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 }, "Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 }, "Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 }, "Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 }, "Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 }, "Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 }, "A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 }, "The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 }, "Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 }, "Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 }, "Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 }, "Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, "A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, "Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, "Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10735,7 +11078,7 @@
       </c>
       <c r="G2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C2,""": { ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2,", ""lv1"": ",F2," }, ")</f>
-        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Twilight Thorn": { "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10759,7 +11102,7 @@
       </c>
       <c r="G3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C3,""": { ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3,", ""lv1"": ",F3," }, ")</f>
-        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Axel": { "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10783,7 +11126,7 @@
       </c>
       <c r="G4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C4,""": { ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4,", ""lv1"": ",F4," }, ")</f>
-        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Shan-Yu": { "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10807,7 +11150,7 @@
       </c>
       <c r="G5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C5,""": { ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5,", ""lv1"": ",F5," }, ")</f>
-        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Thresholder": { "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10831,7 +11174,7 @@
       </c>
       <c r="G6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C6,""": { ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6,", ""lv1"": ",F6," }, ")</f>
-        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Dark Thorn": { "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10855,7 +11198,7 @@
       </c>
       <c r="G7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C7,""": { ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7,", ""lv1"": ",F7," }, ")</f>
-        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Cerberus": { "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10879,7 +11222,7 @@
       </c>
       <c r="G8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C8,""": { ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8,", ""lv1"": ",F8," }, ")</f>
-        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Olympus Pete": { "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10903,7 +11246,7 @@
       </c>
       <c r="G9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C9,""": { ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9,", ""lv1"": ",F9," }, ")</f>
-        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Timeless Pete": { "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10927,7 +11270,7 @@
       </c>
       <c r="G10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C10,""": { ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10,", ""lv1"": ",F10," }, ")</f>
-        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Hydra": { "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10951,7 +11294,7 @@
       </c>
       <c r="G11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C11,""": { ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11,", ""lv1"": ",F11," }, ")</f>
-        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Barbossa": { "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10975,7 +11318,7 @@
       </c>
       <c r="G12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C12,""": { ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12,", ""lv1"": ",F12," }, ")</f>
-        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Prison Keeper": { "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10999,7 +11342,7 @@
       </c>
       <c r="G13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C13,""": { ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13,", ""lv1"": ",F13," }, ")</f>
-        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Oogie Boogie": { "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11023,7 +11366,7 @@
       </c>
       <c r="G14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C14,""": { ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14,", ""lv1"": ",F14," }, ")</f>
-        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Volcano and Blizzard": { "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11047,7 +11390,7 @@
       </c>
       <c r="G15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C15,""": { ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15,", ""lv1"": ",F15," }, ")</f>
-        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Scar": { "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11071,7 +11414,7 @@
       </c>
       <c r="G16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C16,""": { ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16,", ""lv1"": ",F16," }, ")</f>
-        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Pain and Panic Cup": { "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11095,7 +11438,7 @@
       </c>
       <c r="G17" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C17,""": { ""locationCode"": """,B17,""", ""eventId"": 0x",A17,", ""score"": ",E17,", ""isBoss"": ",D17,", ""lv1"": ",F17," }, ")</f>
-        <v>"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Monitors": { "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11119,7 +11462,7 @@
       </c>
       <c r="G18" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C18,""": { ""locationCode"": """,B18,""", ""eventId"": 0x",A18,", ""score"": ",E18,", ""isBoss"": ",D18,", ""lv1"": ",F18," }, ")</f>
-        <v>"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Hostile Program": { "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11143,7 +11486,7 @@
       </c>
       <c r="G19" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C19,""": { ""locationCode"": """,B19,""", ""eventId"": 0x",A19,", ""score"": ",E19,", ""isBoss"": ",D19,", ""lv1"": ",F19," }, ")</f>
-        <v>"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Demyx": { "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11167,7 +11510,7 @@
       </c>
       <c r="G20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C20,""": { ""locationCode"": """,B20,""", ""eventId"": 0x",A20,", ""score"": ",E20,", ""isBoss"": ",D20,", ""lv1"": ",F20," }, ")</f>
-        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 },</v>
+        <v>"Battle of 1000 Heartless": { "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11191,7 +11534,7 @@
       </c>
       <c r="G21" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C21,""": { ""locationCode"": """,B21,""", ""eventId"": 0x",A21,", ""score"": ",E21,", ""isBoss"": ",D21,", ""lv1"": ",F21," }, ")</f>
-        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Storm Rider": { "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11215,7 +11558,7 @@
       </c>
       <c r="G22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C22,""": { ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22," }, ")</f>
-        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Xaldin": { "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11239,7 +11582,7 @@
       </c>
       <c r="G23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C23,""": { ""locationCode"": """,B23,""", ""eventId"": 0x",A23,", ""score"": ",E23,", ""isBoss"": ",D23,", ""lv1"": ",F23," }, ")</f>
-        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Hades": { "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11263,7 +11606,7 @@
       </c>
       <c r="G24" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C24,""": { ""locationCode"": """,B24,""", ""eventId"": 0x",A24,", ""score"": ",E24,", ""isBoss"": ",D24,", ""lv1"": ",F24," }, ")</f>
-        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Grim Reaper II": { "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11287,7 +11630,7 @@
       </c>
       <c r="G25" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C25,""": { ""locationCode"": """,B25,""", ""eventId"": 0x",A25,", ""score"": ",E25,", ""isBoss"": ",D25,", ""lv1"": ",F25," }, ")</f>
-        <v>"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Experiment": { "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11311,7 +11654,7 @@
       </c>
       <c r="G26" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C26,""": { ""locationCode"": """,B26,""", ""eventId"": 0x",A26,", ""score"": ",E26,", ""isBoss"": ",D26,", ""lv1"": ",F26," }, ")</f>
-        <v>"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Sandswept Ruins Escape": { "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11335,7 +11678,7 @@
       </c>
       <c r="G27" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C27,""": { ""locationCode"": """,B27,""", ""eventId"": 0x",A27,", ""score"": ",E27,", ""isBoss"": ",D27,", ""lv1"": ",F27," }, ")</f>
-        <v>"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Jafar": { "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11359,7 +11702,7 @@
       </c>
       <c r="G28" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C28,""": { ""locationCode"": """,B28,""", ""eventId"": 0x",A28,", ""score"": ",E28,", ""isBoss"": ",D28,", ""lv1"": ",F28," }, ")</f>
-        <v>"Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Groundshaker": { "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11383,7 +11726,7 @@
       </c>
       <c r="G29" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C29,""": { ""locationCode"": """,B29,""", ""eventId"": 0x",A29,", ""score"": ",E29,", ""isBoss"": ",D29,", ""lv1"": ",F29," }, ")</f>
-        <v>"Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Solar Sailer": { "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11407,7 +11750,7 @@
       </c>
       <c r="G30" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C30,""": { ""locationCode"": """,B30,""", ""eventId"": 0x",A30,", ""score"": ",E30,", ""isBoss"": ",D30,", ""lv1"": ",F30," }, ")</f>
-        <v>"MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"MCP": { "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11431,7 +11774,7 @@
       </c>
       <c r="G31" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C31,""": { ""locationCode"": """,B31,""", ""eventId"": 0x",A31,", ""score"": ",E31,", ""isBoss"": ",D31,", ""lv1"": ",F31," }, ")</f>
-        <v>"Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Sephiroth": { "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11455,7 +11798,7 @@
       </c>
       <c r="G32" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C32,""": { ""locationCode"": """,B32,""", ""eventId"": 0x",A32,", ""score"": ",E32,", ""isBoss"": ",D32,", ""lv1"": ",F32," }, ")</f>
-        <v>"Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Roxas": { "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11479,7 +11822,7 @@
       </c>
       <c r="G33" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C33,""": { ""locationCode"": """,B33,""", ""eventId"": 0x",A33,", ""score"": ",E33,", ""isBoss"": ",D33,", ""lv1"": ",F33," }, ")</f>
-        <v>"Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Xigbar": { "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11503,7 +11846,7 @@
       </c>
       <c r="G34" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C34,""": { ""locationCode"": """,B34,""", ""eventId"": 0x",A34,", ""score"": ",E34,", ""isBoss"": ",D34,", ""lv1"": ",F34," }, ")</f>
-        <v>"Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Luxord": { "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11527,7 +11870,7 @@
       </c>
       <c r="G35" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C35,""": { ""locationCode"": """,B35,""", ""eventId"": 0x",A35,", ""score"": ",E35,", ""isBoss"": ",D35,", ""lv1"": ",F35," }, ")</f>
-        <v>"Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Saïx": { "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11551,7 +11894,7 @@
       </c>
       <c r="G36" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C36,""": { ""locationCode"": """,B36,""", ""eventId"": 0x",A36,", ""score"": ",E36,", ""isBoss"": ",D36,", ""lv1"": ",F36," }, ")</f>
-        <v>"Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Xemnas I": { "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11575,7 +11918,7 @@
       </c>
       <c r="G37" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C37,""": { ""locationCode"": """,B37,""", ""eventId"": 0x",A37,", ""score"": ",E37,", ""isBoss"": ",D37,", ""lv1"": ",F37," }, ")</f>
-        <v>"Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Xemnas Cannons": { "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11599,7 +11942,7 @@
       </c>
       <c r="G38" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C38,""": { ""locationCode"": """,B38,""", ""eventId"": 0x",A38,", ""score"": ",E38,", ""isBoss"": ",D38,", ""lv1"": ",F38," }, ")</f>
-        <v>"Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Ending Sequence": { "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11623,7 +11966,7 @@
       </c>
       <c r="G39" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C39,""": { ""locationCode"": """,B39,""", ""eventId"": 0x",A39,", ""score"": ",E39,", ""isBoss"": ",D39,", ""lv1"": ",F39," }, ")</f>
-        <v>"Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Final Xemnas": { "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11647,7 +11990,7 @@
       </c>
       <c r="G40" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C40,""": { ""locationCode"": """,B40,""", ""eventId"": 0x",A40,", ""score"": ",E40,", ""isBoss"": ",D40,", ""lv1"": ",F40," }, ")</f>
-        <v>"Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Mail Delivery": { "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11671,7 +12014,7 @@
       </c>
       <c r="G41" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C41,""": { ""locationCode"": """,B41,""", ""eventId"": 0x",A41,", ""score"": ",E41,", ""isBoss"": ",D41,", ""lv1"": ",F41," }, ")</f>
-        <v>"Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Cargo Climb": { "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11695,7 +12038,7 @@
       </c>
       <c r="G42" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C42,""": { ""locationCode"": """,B42,""", ""eventId"": 0x",A42,", ""score"": ",E42,", ""isBoss"": ",D42,", ""lv1"": ",F42," }, ")</f>
-        <v>"Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Grandstander": { "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11719,7 +12062,7 @@
       </c>
       <c r="G43" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C43,""": { ""locationCode"": """,B43,""", ""eventId"": 0x",A43,", ""score"": ",E43,", ""isBoss"": ",D43,", ""lv1"": ",F43," }, ")</f>
-        <v>"Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Poster Duty": { "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11743,7 +12086,7 @@
       </c>
       <c r="G44" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C44,""": { ""locationCode"": """,B44,""", ""eventId"": 0x",A44,", ""score"": ",E44,", ""isBoss"": ",D44,", ""lv1"": ",F44," }, ")</f>
-        <v>"Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Bumble-Buster": { "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11767,7 +12110,7 @@
       </c>
       <c r="G45" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C45,""": { ""locationCode"": """,B45,""", ""eventId"": 0x",A45,", ""score"": ",E45,", ""isBoss"": ",D45,", ""lv1"": ",F45," }, ")</f>
-        <v>"Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Junk Sweep": { "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11791,7 +12134,7 @@
       </c>
       <c r="G46" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C46,""": { ""locationCode"": """,B46,""", ""eventId"": 0x",A46,", ""score"": ",E46,", ""isBoss"": ",D46,", ""lv1"": ",F46," }, ")</f>
-        <v>"Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Struggle: Hayner": { "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11815,7 +12158,7 @@
       </c>
       <c r="G47" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C47,""": { ""locationCode"": """,B47,""", ""eventId"": 0x",A47,", ""score"": ",E47,", ""isBoss"": ",D47,", ""lv1"": ",F47," }, ")</f>
-        <v>"Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Struggle: Setzer": { "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11839,7 +12182,7 @@
       </c>
       <c r="G48" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C48,""": { ""locationCode"": """,B48,""", ""eventId"": 0x",A48,", ""score"": ",E48,", ""isBoss"": ",D48,", ""lv1"": ",F48," }, ")</f>
-        <v>"Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Struggle: Seifer": { "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11863,7 +12206,7 @@
       </c>
       <c r="G49" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C49,""": { ""locationCode"": """,B49,""", ""eventId"": 0x",A49,", ""score"": ",E49,", ""isBoss"": ",D49,", ""lv1"": ",F49," }, ")</f>
-        <v>"Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Skateboard Street Rave": { "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11887,7 +12230,7 @@
       </c>
       <c r="G50" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C50,""": { ""locationCode"": """,B50,""", ""eventId"": 0x",A50,", ""score"": ",E50,", ""isBoss"": ",D50,", ""lv1"": ",F50," }, ")</f>
-        <v>"Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Zexion’s Absent Silhouette": { "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11911,7 +12254,7 @@
       </c>
       <c r="G51" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C51,""": { ""locationCode"": """,B51,""", ""eventId"": 0x",A51,", ""score"": ",E51,", ""isBoss"": ",D51,", ""lv1"": ",F51," }, ")</f>
-        <v>"Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Marluxia’s Absent Silhouette": { "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11935,7 +12278,7 @@
       </c>
       <c r="G52" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C52,""": { ""locationCode"": """,B52,""", ""eventId"": 0x",A52,", ""score"": ",E52,", ""isBoss"": ",D52,", ""lv1"": ",F52," }, ")</f>
-        <v>"Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Larxene’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11959,7 +12302,7 @@
       </c>
       <c r="G53" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C53,""": { ""locationCode"": """,B53,""", ""eventId"": 0x",A53,", ""score"": ",E53,", ""isBoss"": ",D53,", ""lv1"": ",F53," }, ")</f>
-        <v>"Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Lexaeus’s Absent Silhouette": { "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11983,7 +12326,7 @@
       </c>
       <c r="G54" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C54,""": { ""locationCode"": """,B54,""", ""eventId"": 0x",A54,", ""score"": ",E54,", ""isBoss"": ",D54,", ""lv1"": ",F54," }, ")</f>
-        <v>"Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 },</v>
+        <v>"Vexen’s Absent Silhouette": { "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1 }, </v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12007,7 +12350,7 @@
       </c>
       <c r="G55" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C55,""": { ""locationCode"": """,B55,""", ""eventId"": 0x",A55,", ""score"": ",E55,", ""isBoss"": ",D55,", ""lv1"": ",F55," }, ")</f>
-        <v>"Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Phil’s Training – Maniac Mode": { "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12031,7 +12374,7 @@
       </c>
       <c r="G56" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C56,""": { ""locationCode"": """,B56,""", ""eventId"": 0x",A56,", ""score"": ",E56,", ""isBoss"": ",D56,", ""lv1"": ",F56," }, ")</f>
-        <v>"Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Skateboard Freestyle": { "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12055,7 +12398,7 @@
       </c>
       <c r="G57" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C57,""": { ""locationCode"": """,B57,""", ""eventId"": 0x",A57,", ""score"": ",E57,", ""isBoss"": ",D57,", ""lv1"": ",F57," }, ")</f>
-        <v>"Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Skateboard Time Attack": { "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12079,7 +12422,7 @@
       </c>
       <c r="G58" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C58,""": { ""locationCode"": """,B58,""", ""eventId"": 0x",A58,", ""score"": ",E58,", ""isBoss"": ",D58,", ""lv1"": ",F58," }, ")</f>
-        <v>"Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Skateboard Sand Slider": { "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12103,7 +12446,7 @@
       </c>
       <c r="G59" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C59,""": { ""locationCode"": """,B59,""", ""eventId"": 0x",A59,", ""score"": ",E59,", ""isBoss"": ",D59,", ""lv1"": ",F59," }, ")</f>
-        <v>"Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Skateboard Workshop Rave": { "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12127,7 +12470,7 @@
       </c>
       <c r="G60" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C60,""": { ""locationCode"": """,B60,""", ""eventId"": 0x",A60,", ""score"": ",E60,", ""isBoss"": ",D60,", ""lv1"": ",F60," }, ")</f>
-        <v>"Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Light Cycle": { "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12151,7 +12494,7 @@
       </c>
       <c r="G61" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C61,""": { ""locationCode"": """,B61,""", ""eventId"": 0x",A61,", ""score"": ",E61,", ""isBoss"": ",D61,", ""lv1"": ",F61," }, ")</f>
-        <v>"A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"A Blustery Rescue": { "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12175,7 +12518,7 @@
       </c>
       <c r="G62" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C62,""": { ""locationCode"": """,B62,""", ""eventId"": 0x",A62,", ""score"": ",E62,", ""isBoss"": ",D62,", ""lv1"": ",F62," }, ")</f>
-        <v>"Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Hunny Slider": { "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12199,7 +12542,7 @@
       </c>
       <c r="G63" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C63,""": { ""locationCode"": """,B63,""", ""eventId"": 0x",A63,", ""score"": ",E63,", ""isBoss"": ",D63,", ""lv1"": ",F63," }, ")</f>
-        <v>"Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Balloon Bounce": { "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12223,7 +12566,7 @@
       </c>
       <c r="G64" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C64,""": { ""locationCode"": """,B64,""", ""eventId"": 0x",A64,", ""score"": ",E64,", ""isBoss"": ",D64,", ""lv1"": ",F64," }, ")</f>
-        <v>"The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"The Expotition": { "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12247,7 +12590,7 @@
       </c>
       <c r="G65" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C65,""": { ""locationCode"": """,B65,""", ""eventId"": 0x",A65,", ""score"": ",E65,", ""isBoss"": ",D65,", ""lv1"": ",F65," }, ")</f>
-        <v>"The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"The Hunny Pot": { "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12271,7 +12614,7 @@
       </c>
       <c r="G66" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C66,""": { ""locationCode"": """,B66,""", ""eventId"": 0x",A66,", ""score"": ",E66,", ""isBoss"": ",D66,", ""lv1"": ",F66," }, ")</f>
-        <v>"Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Swim This Way": { "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12295,7 +12638,7 @@
       </c>
       <c r="G67" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C67,""": { ""locationCode"": """,B67,""", ""eventId"": 0x",A67,", ""score"": ",E67,", ""isBoss"": ",D67,", ""lv1"": ",F67," }, ")</f>
-        <v>"Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Part of Your World": { "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12319,7 +12662,7 @@
       </c>
       <c r="G68" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C68,""": { ""locationCode"": """,B68,""", ""eventId"": 0x",A68,", ""score"": ",E68,", ""isBoss"": ",D68,", ""lv1"": ",F68," }, ")</f>
-        <v>"Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Under the Sea": { "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12343,7 +12686,7 @@
       </c>
       <c r="G69" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C69,""": { ""locationCode"": """,B69,""", ""eventId"": 0x",A69,", ""score"": ",E69,", ""isBoss"": ",D69,", ""lv1"": ",F69," }, ")</f>
-        <v>"Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Ursula’s Revenge": { "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12367,7 +12710,7 @@
       </c>
       <c r="G70" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C70,""": { ""locationCode"": """,B70,""", ""eventId"": 0x",A70,", ""score"": ",E70,", ""isBoss"": ",D70,", ""lv1"": ",F70," }, ")</f>
-        <v>"A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"A New Day Is Dawning": { "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12391,7 +12734,7 @@
       </c>
       <c r="G71" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C71,""": { ""locationCode"": """,B71,""", ""eventId"": 0x",A71,", ""score"": ",E71,", ""isBoss"": ",D71,", ""lv1"": ",F71," }, ")</f>
-        <v>"Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Gift Wrapping": { "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12415,7 +12758,7 @@
       </c>
       <c r="G72" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C72,""": { ""locationCode"": """,B72,""", ""eventId"": 0x",A72,", ""score"": ",E72,", ""isBoss"": ",D72,", ""lv1"": ",F72," }, ")</f>
-        <v>"Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Xemnas Dragon": { "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12439,7 +12782,7 @@
       </c>
       <c r="G73" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("""",C73,""": { ""locationCode"": """,B73,""", ""eventId"": 0x",A73,", ""score"": ",E73,", ""isBoss"": ",D73,", ""lv1"": ",F73," }, ")</f>
-        <v>"Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 },</v>
+        <v>"Magic Carpet": { "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0 }, </v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21017,7 +21360,7 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21038,7 +21381,7 @@
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="str">
+      <c r="F1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1111)</f>
         <v>2: { "addr": 0x0032dfd0, "bit": 0 },3: { "addr": 0x0032dfd0, "bit": 1 },4: { "addr": 0x0032dfd0, "bit": 2 },5: { "addr": 0x0032dfd0, "bit": 3 },6: { "addr": 0x0032dfd0, "bit": 4 },7: { "addr": 0x0032dfd0, "bit": 5 },8: { "addr": 0x0032dfd0, "bit": 6 },9: { "addr": 0x0032dfd0, "bit": 7 },10: { "addr": 0x0032dfd1, "bit": 0 },11: { "addr": 0x0032dfd1, "bit": 1 },12: { "addr": 0x0032dfd1, "bit": 2 },13: { "addr": 0x0032dfd1, "bit": 3 },14: { "addr": 0x0032dfd8, "bit": 0 },15: { "addr": 0x0032dfd8, "bit": 1 },16: { "addr": 0x0032dfd8, "bit": 2 },17: { "addr": 0x0032dfd8, "bit": 3 },18: { "addr": 0x0032dfd8, "bit": 4 },19: { "addr": 0x0032dfd8, "bit": 5 },20: { "addr": 0x0032dfd8, "bit": 6 },21: { "addr": 0x0032dfd8, "bit": 7 },22: { "addr": 0x0032dfd9, "bit": 0 },23: { "addr": 0x0032dfd9, "bit": 1 },24: { "addr": 0x0032dfd9, "bit": 2 },25: { "addr": 0x0032dfd9, "bit": 3 },26: { "addr": 0x0032dfe0, "bit": 0 },27: { "addr": 0x0032dfe0, "bit": 1 },28: { "addr": 0x0032dfe0, "bit": 2 },29: { "addr": 0x0032dfe0, "bit": 3 },30: { "addr": 0x0032dfe0, "bit": 4 },31: { "addr": 0x0032dfe0, "bit": 5 },32: { "addr": 0x0032dfe0, "bit": 6 },33: { "addr": 0x0032dfe0, "bit": 7 },34: { "addr": 0x0032dfe1, "bit": 0 },35: { "addr": 0x0032dfe1, "bit": 1 },36: { "addr": 0x0032dfe1, "bit": 2 },37: { "addr": 0x0032dfe1, "bit": 3 },38: { "addr": 0x0032dfe8, "bit": 0 },39: { "addr": 0x0032dfe8, "bit": 1 },40: { "addr": 0x0032dfe8, "bit": 2 },41: { "addr": 0x0032dfe8, "bit": 3 },42: { "addr": 0x0032dfe8, "bit": 4 },43: { "addr": 0x0032dfe8, "bit": 5 },44: { "addr": 0x0032dfe8, "bit": 6 },45: { "addr": 0x0032dfe8, "bit": 7 },46: { "addr": 0x0032dfe9, "bit": 0 },47: { "addr": 0x0032dfe9, "bit": 1 },48: { "addr": 0x0032dfe9, "bit": 2 },49: { "addr": 0x0032dfe9, "bit": 3 },50: { "addr": 0x0032dff0, "bit": 0 },51: { "addr": 0x0032dff0, "bit": 1 },52: { "addr": 0x0032dff0, "bit": 2 },53: { "addr": 0x0032dff0, "bit": 3 },54: { "addr": 0x0032dff0, "bit": 4 },55: { "addr": 0x0032dff0, "bit": 5 },56: { "addr": 0x0032dff0, "bit": 6 },57: { "addr": 0x0032dff0, "bit": 7 },58: { "addr": 0x0032dff1, "bit": 0 },59: { "addr": 0x0032dff1, "bit": 1 },60: { "addr": 0x0032dff1, "bit": 2 },61: { "addr": 0x0032dff1, "bit": 3 },62: { "addr": 0x0032dff1, "bit": 4 },63: { "addr": 0x0032dff1, "bit": 5 },64: { "addr": 0x0032dff1, "bit": 6 },65: { "addr": 0x0032dff1, "bit": 7 },66: { "addr": 0x0032dff2, "bit": 0 },67: { "addr": 0x0032dff2, "bit": 1 },68: { "addr": 0x0032dff2, "bit": 2 },69: { "addr": 0x0032dff2, "bit": 3 },70: { "addr": 0x0032dff2, "bit": 4 },71: { "addr": 0x0032dff2, "bit": 5 },72: { "addr": 0x0032dff2, "bit": 6 },73: { "addr": 0x0032dff2, "bit": 7 },74: { "addr": 0x0032dff3, "bit": 0 },75: { "addr": 0x0032dff3, "bit": 1 },76: { "addr": 0x0032dff3, "bit": 2 },77: { "addr": 0x0032dff3, "bit": 3 },78: { "addr": 0x0032dff3, "bit": 4 },79: { "addr": 0x0032dff3, "bit": 5 },80: { "addr": 0x0032dff3, "bit": 6 },81: { "addr": 0x0032dff3, "bit": 7 },82: { "addr": 0x0032dff4, "bit": 0 },83: { "addr": 0x0032dff4, "bit": 1 },84: { "addr": 0x0032dff4, "bit": 2 },85: { "addr": 0x0032dff4, "bit": 3 },86: { "addr": 0x0032dff4, "bit": 4 },87: { "addr": 0x0032dff4, "bit": 5 },88: { "addr": 0x0032dff4, "bit": 6 },89: { "addr": 0x0032dff4, "bit": 7 },90: { "addr": 0x0032dff5, "bit": 0 },91: { "addr": 0x0032dff5, "bit": 1 },92: { "addr": 0x0032dff5, "bit": 2 },93: { "addr": 0x0032dff5, "bit": 3 },94: { "addr": 0x0032dff5, "bit": 4 },95: { "addr": 0x0032dff5, "bit": 5 },96: { "addr": 0x0032dff5, "bit": 6 },97: { "addr": 0x0032dff5, "bit": 7 },98: { "addr": 0x0032dff8, "bit": 0 },99: { "addr": 0x0032dff8, "bit": 1 },100: { "addr": 0x0032dff8, "bit": 2 },101: { "addr": 0x0032dff8, "bit": 3 },102: { "addr": 0x0032dff8, "bit": 4 },103: { "addr": 0x0032dff8, "bit": 5 },104: { "addr": 0x0032dff8, "bit": 6 },105: { "addr": 0x0032dff8, "bit": 7 },106: { "addr": 0x0032dff9, "bit": 0 },107: { "addr": 0x0032dff9, "bit": 1 },108: { "addr": 0x0032dff9, "bit": 2 },109: { "addr": 0x0032dff9, "bit": 3 },110: { "addr": 0x0032dff9, "bit": 4 },111: { "addr": 0x0032dff9, "bit": 5 },112: { "addr": 0x0032dff9, "bit": 6 },113: { "addr": 0x0032dff9, "bit": 7 },114: { "addr": 0x0032dffa, "bit": 0 },115: { "addr": 0x0032dffa, "bit": 1 },116: { "addr": 0x0032dffa, "bit": 2 },117: { "addr": 0x0032dffa, "bit": 3 },118: { "addr": 0x0032dffa, "bit": 4 },119: { "addr": 0x0032dffa, "bit": 5 },120: { "addr": 0x0032dffa, "bit": 6 },121: { "addr": 0x0032dffa, "bit": 7 },122: { "addr": 0x0032dffb, "bit": 0 },123: { "addr": 0x0032dffb, "bit": 1 },124: { "addr": 0x0032dffb, "bit": 2 },125: { "addr": 0x0032dffb, "bit": 3 },126: { "addr": 0x0032dffb, "bit": 4 },127: { "addr": 0x0032dffb, "bit": 5 },128: { "addr": 0x0032dffb, "bit": 6 },129: { "addr": 0x0032dffb, "bit": 7 },130: { "addr": 0x0032dffc, "bit": 0 },131: { "addr": 0x0032dffc, "bit": 1 },132: { "addr": 0x0032dffc, "bit": 2 },133: { "addr": 0x0032dffc, "bit": 3 },134: { "addr": 0x0032dffc, "bit": 4 },135: { "addr": 0x0032dffc, "bit": 5 },136: { "addr": 0x0032dffc, "bit": 6 },137: { "addr": 0x0032dffc, "bit": 7 },138: { "addr": 0x0032dffd, "bit": 0 },139: { "addr": 0x0032dffd, "bit": 1 },140: { "addr": 0x0032dffd, "bit": 2 },141: { "addr": 0x0032dffd, "bit": 3 },142: { "addr": 0x0032dffd, "bit": 4 },143: { "addr": 0x0032dffd, "bit": 5 },144: { "addr": 0x0032dffd, "bit": 6 },145: { "addr": 0x0032dffd, "bit": 7 },</v>
       </c>
@@ -22724,13 +23067,13 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="1" t="s">
         <v>1263</v>
       </c>
-      <c r="B114" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C114" s="0" t="s">
+      <c r="B114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>1261</v>
       </c>
       <c r="D114" s="1" t="str">
@@ -23212,4 +23555,2088 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F133"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(D2:D1129)</f>
+        <v>2: { "addr": 0x0032dedc, "bit": 1 },3: { "addr": 0x0032dedd, "bit": 2 },4: { "addr": 0x0032dedd, "bit": 6 },5: { "addr": 0x0032dedd, "bit": 7 },6: { "addr": 0x0032dede, "bit": 0 },7: { "addr": 0x0032dede, "bit": 1 },8: { "addr": 0x0032dede, "bit": 2 },9: { "addr": 0x0032dede, "bit": 3 },10: { "addr": 0x0032dee1, "bit": 1 },11: { "addr": 0x0032dee2, "bit": 0 },12: { "addr": 0x0032dee2, "bit": 1 },13: { "addr": 0x0032dee2, "bit": 3 },14: { "addr": 0x0032dee2, "bit": 4 },15: { "addr": 0x0032dee2, "bit": 5 },16: { "addr": 0x0032dee2, "bit": 6 },17: { "addr": 0x0032dee2, "bit": 7 },18: { "addr": 0x0032dee4, "bit": 0 },19: { "addr": 0x0032dee4, "bit": 1 },20: { "addr": 0x0032dee4, "bit": 2 },21: { "addr": 0x0032dee4, "bit": 3 },22: { "addr": 0x0032dee4, "bit": 4 },23: { "addr": 0x0032dee4, "bit": 5 },24: { "addr": 0x0032dee4, "bit": 6 },25: { "addr": 0x0032dee4, "bit": 7 },26: { "addr": 0x0032dee5, "bit": 4 },27: { "addr": 0x0032dee5, "bit": 5 },28: { "addr": 0x0032dee8, "bit": 0 },29: { "addr": 0x0032dee8, "bit": 3 },30: { "addr": 0x0032dee8, "bit": 4 },31: { "addr": 0x0032dee9, "bit": 0 },32: { "addr": 0x0032dee9, "bit": 2 },33: { "addr": 0x0032dee9, "bit": 4 },34: { "addr": 0x0032dee9, "bit": 6 },35: { "addr": 0x0032dee9, "bit": 7 },36: { "addr": 0x0032deea, "bit": 0 },37: { "addr": 0x0032deea, "bit": 1 },38: { "addr": 0x0032deea, "bit": 2 },39: { "addr": 0x0032deea, "bit": 4 },40: { "addr": 0x0032deea, "bit": 5 },41: { "addr": 0x0032deea, "bit": 7 },42: { "addr": 0x0032deeb, "bit": 0 },43: { "addr": 0x0032deeb, "bit": 2 },44: { "addr": 0x0032deeb, "bit": 3 },45: { "addr": 0x0032deeb, "bit": 4 },46: { "addr": 0x0032deeb, "bit": 7 },47: { "addr": 0x0032deec, "bit": 1 },48: { "addr": 0x0032deec, "bit": 2 },49: { "addr": 0x0032deec, "bit": 3 },50: { "addr": 0x0032deec, "bit": 4 },51: { "addr": 0x0032deec, "bit": 5 },52: { "addr": 0x0032deec, "bit": 6 },53: { "addr": 0x0032deec, "bit": 7 },54: { "addr": 0x0032deed, "bit": 0 },55: { "addr": 0x0032deed, "bit": 1 },56: { "addr": 0x0032deed, "bit": 3 },57: { "addr": 0x0032deef, "bit": 7 },58: { "addr": 0x0032def0, "bit": 0 },59: { "addr": 0x0032def0, "bit": 1 },60: { "addr": 0x0032def0, "bit": 2 },61: { "addr": 0x0032def0, "bit": 3 },62: { "addr": 0x0032def0, "bit": 4 },63: { "addr": 0x0032def0, "bit": 5 },64: { "addr": 0x0032def0, "bit": 6 },65: { "addr": 0x0032def1, "bit": 0 },66: { "addr": 0x0032def1, "bit": 1 },67: { "addr": 0x0032def1, "bit": 2 },68: { "addr": 0x0032def1, "bit": 3 },69: { "addr": 0x0032def1, "bit": 4 },70: { "addr": 0x0032def1, "bit": 6 },71: { "addr": 0x0032def2, "bit": 1 },72: { "addr": 0x0032def2, "bit": 2 },73: { "addr": 0x0032def2, "bit": 3 },74: { "addr": 0x0032def2, "bit": 4 },75: { "addr": 0x0032def2, "bit": 5 },76: { "addr": 0x0032def2, "bit": 6 },77: { "addr": 0x0032def2, "bit": 7 },78: { "addr": 0x0032def3, "bit": 1 },79: { "addr": 0x0032def3, "bit": 2 },80: { "addr": 0x0032def3, "bit": 3 },81: { "addr": 0x0032def3, "bit": 4 },82: { "addr": 0x0032def3, "bit": 5 },83: { "addr": 0x0032def4, "bit": 2 },84: { "addr": 0x0032def4, "bit": 6 },85: { "addr": 0x0032def6, "bit": 3 },86: { "addr": 0x0032def8, "bit": 7 },87: { "addr": 0x0032def9, "bit": 7 },88: { "addr": 0x0032defa, "bit": 0 },89: { "addr": 0x0032defa, "bit": 7 },90: { "addr": 0x0032defb, "bit": 0 },91: { "addr": 0x0032defb, "bit": 1 },92: { "addr": 0x0032df00, "bit": 5 },93: { "addr": 0x0032df00, "bit": 6 },94: { "addr": 0x0032df00, "bit": 7 },95: { "addr": 0x0032df01, "bit": 0 },96: { "addr": 0x0032df01, "bit": 1 },97: { "addr": 0x0032df01, "bit": 2 },98: { "addr": 0x0032df02, "bit": 0 },99: { "addr": 0x0032df02, "bit": 1 },100: { "addr": 0x0032df02, "bit": 2 },101: { "addr": 0x0032df02, "bit": 3 },102: { "addr": 0x0032df02, "bit": 7 },103: { "addr": 0x0032df03, "bit": 1 },104: { "addr": 0x0032df03, "bit": 2 },105: { "addr": 0x0032df03, "bit": 3 },106: { "addr": 0x0032df03, "bit": 4 },107: { "addr": 0x0032df03, "bit": 5 },108: { "addr": 0x0032df04, "bit": 0 },109: { "addr": 0x0032df04, "bit": 1 },110: { "addr": 0x0032df04, "bit": 5 },111: { "addr": 0x0032df04, "bit": 6 },112: { "addr": 0x0032df04, "bit": 7 },113: { "addr": 0x0032df05, "bit": 3 },114: { "addr": 0x0032df05, "bit": 5 },115: { "addr": 0x0032df06, "bit": 1 },116: { "addr": 0x0032df06, "bit": 2 },117: { "addr": 0x0032df06, "bit": 3 },118: { "addr": 0x0032df06, "bit": 4 },119: { "addr": 0x0032df06, "bit": 5 },120: { "addr": 0x0032df06, "bit": 6 },121: { "addr": 0x0032df06, "bit": 7 },122: { "addr": 0x0032df07, "bit": 7 },123: { "addr": 0x0032df08, "bit": 0 },124: { "addr": 0x0032df08, "bit": 1 },125: { "addr": 0x0032df08, "bit": 2 },126: { "addr": 0x0032df08, "bit": 3 },127: { "addr": 0x0032df09, "bit": 5 },128: { "addr": 0x0032df09, "bit": 7 },129: { "addr": 0x0032df0a, "bit": 0 },130: { "addr": 0x0032df0b, "bit": 0 },131: { "addr": 0x0032df0b, "bit": 1 },132: { "addr": 0x0032df0b, "bit": 7 },133: { "addr": 0x0032df0c, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A2,", ""bit"": ",B2," },")</f>
+        <v>2: { "addr": 0x0032dedc, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A3,", ""bit"": ",B3," },")</f>
+        <v>3: { "addr": 0x0032dedd, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A4,", ""bit"": ",B4," },")</f>
+        <v>4: { "addr": 0x0032dedd, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A5,", ""bit"": ",B5," },")</f>
+        <v>5: { "addr": 0x0032dedd, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A6,", ""bit"": ",B6," },")</f>
+        <v>6: { "addr": 0x0032dede, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A7,", ""bit"": ",B7," },")</f>
+        <v>7: { "addr": 0x0032dede, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A8,", ""bit"": ",B8," },")</f>
+        <v>8: { "addr": 0x0032dede, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A9,", ""bit"": ",B9," },")</f>
+        <v>9: { "addr": 0x0032dede, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A10,", ""bit"": ",B10," },")</f>
+        <v>10: { "addr": 0x0032dee1, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A11,", ""bit"": ",B11," },")</f>
+        <v>11: { "addr": 0x0032dee2, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A12,", ""bit"": ",B12," },")</f>
+        <v>12: { "addr": 0x0032dee2, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A13,", ""bit"": ",B13," },")</f>
+        <v>13: { "addr": 0x0032dee2, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A14,", ""bit"": ",B14," },")</f>
+        <v>14: { "addr": 0x0032dee2, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A15,", ""bit"": ",B15," },")</f>
+        <v>15: { "addr": 0x0032dee2, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A16,", ""bit"": ",B16," },")</f>
+        <v>16: { "addr": 0x0032dee2, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A17,", ""bit"": ",B17," },")</f>
+        <v>17: { "addr": 0x0032dee2, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A18,", ""bit"": ",B18," },")</f>
+        <v>18: { "addr": 0x0032dee4, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A19,", ""bit"": ",B19," },")</f>
+        <v>19: { "addr": 0x0032dee4, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A20,", ""bit"": ",B20," },")</f>
+        <v>20: { "addr": 0x0032dee4, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A21,", ""bit"": ",B21," },")</f>
+        <v>21: { "addr": 0x0032dee4, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A22,", ""bit"": ",B22," },")</f>
+        <v>22: { "addr": 0x0032dee4, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A23,", ""bit"": ",B23," },")</f>
+        <v>23: { "addr": 0x0032dee4, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A24,", ""bit"": ",B24," },")</f>
+        <v>24: { "addr": 0x0032dee4, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A25,", ""bit"": ",B25," },")</f>
+        <v>25: { "addr": 0x0032dee4, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A26,", ""bit"": ",B26," },")</f>
+        <v>26: { "addr": 0x0032dee5, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A27,", ""bit"": ",B27," },")</f>
+        <v>27: { "addr": 0x0032dee5, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A28,", ""bit"": ",B28," },")</f>
+        <v>28: { "addr": 0x0032dee8, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A29,", ""bit"": ",B29," },")</f>
+        <v>29: { "addr": 0x0032dee8, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A30,", ""bit"": ",B30," },")</f>
+        <v>30: { "addr": 0x0032dee8, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A31,", ""bit"": ",B31," },")</f>
+        <v>31: { "addr": 0x0032dee9, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A32,", ""bit"": ",B32," },")</f>
+        <v>32: { "addr": 0x0032dee9, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A33,", ""bit"": ",B33," },")</f>
+        <v>33: { "addr": 0x0032dee9, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A34,", ""bit"": ",B34," },")</f>
+        <v>34: { "addr": 0x0032dee9, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A35,", ""bit"": ",B35," },")</f>
+        <v>35: { "addr": 0x0032dee9, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A36,", ""bit"": ",B36," },")</f>
+        <v>36: { "addr": 0x0032deea, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A37,", ""bit"": ",B37," },")</f>
+        <v>37: { "addr": 0x0032deea, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A38,", ""bit"": ",B38," },")</f>
+        <v>38: { "addr": 0x0032deea, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A39,", ""bit"": ",B39," },")</f>
+        <v>39: { "addr": 0x0032deea, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A40,", ""bit"": ",B40," },")</f>
+        <v>40: { "addr": 0x0032deea, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D41" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A41,", ""bit"": ",B41," },")</f>
+        <v>41: { "addr": 0x0032deea, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A42,", ""bit"": ",B42," },")</f>
+        <v>42: { "addr": 0x0032deeb, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A43,", ""bit"": ",B43," },")</f>
+        <v>43: { "addr": 0x0032deeb, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A44,", ""bit"": ",B44," },")</f>
+        <v>44: { "addr": 0x0032deeb, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A45,", ""bit"": ",B45," },")</f>
+        <v>45: { "addr": 0x0032deeb, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A46,", ""bit"": ",B46," },")</f>
+        <v>46: { "addr": 0x0032deeb, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A47,", ""bit"": ",B47," },")</f>
+        <v>47: { "addr": 0x0032deec, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A48,", ""bit"": ",B48," },")</f>
+        <v>48: { "addr": 0x0032deec, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A49,", ""bit"": ",B49," },")</f>
+        <v>49: { "addr": 0x0032deec, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A50,", ""bit"": ",B50," },")</f>
+        <v>50: { "addr": 0x0032deec, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A51,", ""bit"": ",B51," },")</f>
+        <v>51: { "addr": 0x0032deec, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A52,", ""bit"": ",B52," },")</f>
+        <v>52: { "addr": 0x0032deec, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A53,", ""bit"": ",B53," },")</f>
+        <v>53: { "addr": 0x0032deec, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A54,", ""bit"": ",B54," },")</f>
+        <v>54: { "addr": 0x0032deed, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A55,", ""bit"": ",B55," },")</f>
+        <v>55: { "addr": 0x0032deed, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A56,", ""bit"": ",B56," },")</f>
+        <v>56: { "addr": 0x0032deed, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A57,", ""bit"": ",B57," },")</f>
+        <v>57: { "addr": 0x0032deef, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A58,", ""bit"": ",B58," },")</f>
+        <v>58: { "addr": 0x0032def0, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A59,", ""bit"": ",B59," },")</f>
+        <v>59: { "addr": 0x0032def0, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A60,", ""bit"": ",B60," },")</f>
+        <v>60: { "addr": 0x0032def0, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A61,", ""bit"": ",B61," },")</f>
+        <v>61: { "addr": 0x0032def0, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A62,", ""bit"": ",B62," },")</f>
+        <v>62: { "addr": 0x0032def0, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A63,", ""bit"": ",B63," },")</f>
+        <v>63: { "addr": 0x0032def0, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A64,", ""bit"": ",B64," },")</f>
+        <v>64: { "addr": 0x0032def0, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A65,", ""bit"": ",B65," },")</f>
+        <v>65: { "addr": 0x0032def1, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A66,", ""bit"": ",B66," },")</f>
+        <v>66: { "addr": 0x0032def1, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A67,", ""bit"": ",B67," },")</f>
+        <v>67: { "addr": 0x0032def1, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A68,", ""bit"": ",B68," },")</f>
+        <v>68: { "addr": 0x0032def1, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A69,", ""bit"": ",B69," },")</f>
+        <v>69: { "addr": 0x0032def1, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D70" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A70,", ""bit"": ",B70," },")</f>
+        <v>70: { "addr": 0x0032def1, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D71" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A71,", ""bit"": ",B71," },")</f>
+        <v>71: { "addr": 0x0032def2, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D72" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A72,", ""bit"": ",B72," },")</f>
+        <v>72: { "addr": 0x0032def2, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D73" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A73,", ""bit"": ",B73," },")</f>
+        <v>73: { "addr": 0x0032def2, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D74" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A74,", ""bit"": ",B74," },")</f>
+        <v>74: { "addr": 0x0032def2, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D75" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A75,", ""bit"": ",B75," },")</f>
+        <v>75: { "addr": 0x0032def2, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D76" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A76,", ""bit"": ",B76," },")</f>
+        <v>76: { "addr": 0x0032def2, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D77" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A77,", ""bit"": ",B77," },")</f>
+        <v>77: { "addr": 0x0032def2, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D78" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A78,", ""bit"": ",B78," },")</f>
+        <v>78: { "addr": 0x0032def3, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D79" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A79,", ""bit"": ",B79," },")</f>
+        <v>79: { "addr": 0x0032def3, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D80" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A80,", ""bit"": ",B80," },")</f>
+        <v>80: { "addr": 0x0032def3, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D81" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A81,", ""bit"": ",B81," },")</f>
+        <v>81: { "addr": 0x0032def3, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D82" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A82,", ""bit"": ",B82," },")</f>
+        <v>82: { "addr": 0x0032def3, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D83" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A83,", ""bit"": ",B83," },")</f>
+        <v>83: { "addr": 0x0032def4, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D84" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A84,", ""bit"": ",B84," },")</f>
+        <v>84: { "addr": 0x0032def4, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D85" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A85,", ""bit"": ",B85," },")</f>
+        <v>85: { "addr": 0x0032def6, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D86" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A86,", ""bit"": ",B86," },")</f>
+        <v>86: { "addr": 0x0032def8, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D87" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A87,", ""bit"": ",B87," },")</f>
+        <v>87: { "addr": 0x0032def9, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D88" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A88,", ""bit"": ",B88," },")</f>
+        <v>88: { "addr": 0x0032defa, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D89" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A89,", ""bit"": ",B89," },")</f>
+        <v>89: { "addr": 0x0032defa, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D90" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A90,", ""bit"": ",B90," },")</f>
+        <v>90: { "addr": 0x0032defb, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D91" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A91,", ""bit"": ",B91," },")</f>
+        <v>91: { "addr": 0x0032defb, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D92" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A92,", ""bit"": ",B92," },")</f>
+        <v>92: { "addr": 0x0032df00, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D93" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A93,", ""bit"": ",B93," },")</f>
+        <v>93: { "addr": 0x0032df00, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D94" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A94,", ""bit"": ",B94," },")</f>
+        <v>94: { "addr": 0x0032df00, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D95" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A95,", ""bit"": ",B95," },")</f>
+        <v>95: { "addr": 0x0032df01, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D96" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A96,", ""bit"": ",B96," },")</f>
+        <v>96: { "addr": 0x0032df01, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D97" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A97,", ""bit"": ",B97," },")</f>
+        <v>97: { "addr": 0x0032df01, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D98" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A98,", ""bit"": ",B98," },")</f>
+        <v>98: { "addr": 0x0032df02, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D99" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A99,", ""bit"": ",B99," },")</f>
+        <v>99: { "addr": 0x0032df02, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D100" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A100,", ""bit"": ",B100," },")</f>
+        <v>100: { "addr": 0x0032df02, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D101" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A101,", ""bit"": ",B101," },")</f>
+        <v>101: { "addr": 0x0032df02, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D102" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A102,", ""bit"": ",B102," },")</f>
+        <v>102: { "addr": 0x0032df02, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D103" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A103,", ""bit"": ",B103," },")</f>
+        <v>103: { "addr": 0x0032df03, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D104" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A104,", ""bit"": ",B104," },")</f>
+        <v>104: { "addr": 0x0032df03, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D105" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A105,", ""bit"": ",B105," },")</f>
+        <v>105: { "addr": 0x0032df03, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D106" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A106,", ""bit"": ",B106," },")</f>
+        <v>106: { "addr": 0x0032df03, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D107" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A107,", ""bit"": ",B107," },")</f>
+        <v>107: { "addr": 0x0032df03, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D108" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A108,", ""bit"": ",B108," },")</f>
+        <v>108: { "addr": 0x0032df04, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D109" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A109,", ""bit"": ",B109," },")</f>
+        <v>109: { "addr": 0x0032df04, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D110" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A110,", ""bit"": ",B110," },")</f>
+        <v>110: { "addr": 0x0032df04, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D111" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A111,", ""bit"": ",B111," },")</f>
+        <v>111: { "addr": 0x0032df04, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D112" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A112,", ""bit"": ",B112," },")</f>
+        <v>112: { "addr": 0x0032df04, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D113" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A113,", ""bit"": ",B113," },")</f>
+        <v>113: { "addr": 0x0032df05, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D114" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A114,", ""bit"": ",B114," },")</f>
+        <v>114: { "addr": 0x0032df05, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D115" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A115,", ""bit"": ",B115," },")</f>
+        <v>115: { "addr": 0x0032df06, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D116" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A116,", ""bit"": ",B116," },")</f>
+        <v>116: { "addr": 0x0032df06, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D117" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A117,", ""bit"": ",B117," },")</f>
+        <v>117: { "addr": 0x0032df06, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D118" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A118,", ""bit"": ",B118," },")</f>
+        <v>118: { "addr": 0x0032df06, "bit": 4 },</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A119,", ""bit"": ",B119," },")</f>
+        <v>119: { "addr": 0x0032df06, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D120" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A120,", ""bit"": ",B120," },")</f>
+        <v>120: { "addr": 0x0032df06, "bit": 6 },</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D121" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A121,", ""bit"": ",B121," },")</f>
+        <v>121: { "addr": 0x0032df06, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D122" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A122,", ""bit"": ",B122," },")</f>
+        <v>122: { "addr": 0x0032df07, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D123" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A123,", ""bit"": ",B123," },")</f>
+        <v>123: { "addr": 0x0032df08, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D124" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A124,", ""bit"": ",B124," },")</f>
+        <v>124: { "addr": 0x0032df08, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D125" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A125,", ""bit"": ",B125," },")</f>
+        <v>125: { "addr": 0x0032df08, "bit": 2 },</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D126" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A126,", ""bit"": ",B126," },")</f>
+        <v>126: { "addr": 0x0032df08, "bit": 3 },</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D127" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A127,", ""bit"": ",B127," },")</f>
+        <v>127: { "addr": 0x0032df09, "bit": 5 },</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D128" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A128,", ""bit"": ",B128," },")</f>
+        <v>128: { "addr": 0x0032df09, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D129" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A129,", ""bit"": ",B129," },")</f>
+        <v>129: { "addr": 0x0032df0a, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D130" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A130,", ""bit"": ",B130," },")</f>
+        <v>130: { "addr": 0x0032df0b, "bit": 0 },</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D131" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A131,", ""bit"": ",B131," },")</f>
+        <v>131: { "addr": 0x0032df0b, "bit": 1 },</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D132" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A132,", ""bit"": ",B132," },")</f>
+        <v>132: { "addr": 0x0032df0b, "bit": 7 },</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D133" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ""addr"": ",A133,", ""bit"": ",B133," },")</f>
+        <v>133: { "addr": 0x0032df0c, "bit": 3 },</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A104:A1048576 A1:A102">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BC3F4854-6765-4D80-B549-FE8030D3CB72}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="dataBar" priority="3">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4290752F-F1BF-4925-8F3D-58F19CEEEBC7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BC3F4854-6765-4D80-B549-FE8030D3CB72}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A104:A1048576 A1:A102</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4290752F-F1BF-4925-8F3D-58F19CEEEBC7}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A103</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Gummi Ship overqualification bug
Fixed a bug where a player who was overqualified (i.e., got an S+1 rank or above) would not earn an achievement at the mission's conclusion.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -21676,8 +21676,8 @@
   </sheetPr>
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W10" activeCellId="0" sqref="W10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21768,7 +21768,7 @@
       </c>
       <c r="Y1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(W2:W10000)</f>
-        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357045, "badge1Id": 402244, "mission2Id": 357046, "badge2Id": 402245, "mission3Id": 357047, "badge3Id": 402246, "exMission1Id": 357048, "exBadge1Id": 402247, "exMission2Id": 357049, "exBadge2Id": 402248, "exMission3Id": 357050, "exBadge3Id": 402249 },3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357051, "badge1Id": 402250, "mission2Id": 357053, "badge2Id": 402252, "mission3Id": 357055, "badge3Id": 402254, "exMission1Id": 357052, "exBadge1Id": 402251, "exMission2Id": 357054, "exBadge2Id": 402253, "exMission3Id": 357056, "exBadge3Id": 402255 },4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357057, "badge1Id": 402256, "mission2Id": 357059, "badge2Id": 402258, "mission3Id": 357061, "badge3Id": 402260, "exMission1Id": 357058, "exBadge1Id": 402257, "exMission2Id": 357060, "exBadge2Id": 402259, "exMission3Id": 357062, "exBadge3Id": 402261 },5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357063, "badge1Id": 402262, "mission2Id": 357065, "badge2Id": 402264, "mission3Id": 357067, "badge3Id": 402262, "exMission1Id": 357064, "exBadge1Id": 402263, "exMission2Id": 357066, "exBadge2Id": 402265, "exMission3Id": 357068, "exBadge3Id": 402267 },6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357069, "badge1Id": 402268, "mission2Id": 357071, "badge2Id": 402270, "mission3Id": 357073, "badge3Id": 402272, "exMission1Id": 357070, "exBadge1Id": 402269, "exMission2Id": 357072, "exBadge2Id": 402271, "exMission3Id": 357074, "exBadge3Id": 402273 },7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357075, "badge1Id": 402274, "mission2Id": 357077, "badge2Id": 402276, "mission3Id": 357079, "badge3Id": 402278, "exMission1Id": 357076, "exBadge1Id": 402275, "exMission2Id": 357078, "exBadge2Id": 402277, "exMission3Id": 357080, "exBadge3Id": 402279 },8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357081, "badge1Id": 402280, "mission2Id": 357083, "badge2Id": 402282, "mission3Id": 357085, "badge3Id": 402284, "exMission1Id": 357082, "exBadge1Id": 402281, "exMission2Id": 357084, "exBadge2Id": 402283, "exMission3Id": 357086, "exBadge3Id": 402285 },9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357087, "badge1Id": 402286, "mission2Id": 357089, "badge2Id": 402289, "mission3Id": 357091, "badge3Id": 402291, "exMission1Id": 357088, "exBadge1Id": 402287, "exMission2Id": 357090, "exBadge2Id": 402290, "exMission3Id": 357092, "exBadge3Id": 402292 },10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357093, "badge1Id": 402293, "mission2Id": 357095, "badge2Id": 402295, "mission3Id": 357097, "badge3Id": 402297, "exMission1Id": 357094, "exBadge1Id": 402294, "exMission2Id": 357096, "exBadge2Id": 402296, "exMission3Id": 357098, "exBadge3Id": 402298 },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21839,8 +21839,8 @@
         <v>402249</v>
       </c>
       <c r="W2" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A2,""", ""gateId"": ",B2,", ""miss1BaseAddr"": ",C2,", ""miss1EXBaseAddr"": ",M2,", ""mission1Score"": ",D2,", ""mission2Score"": ",G2,", ""mission3Score"": ",J2,", ""exMission1Score"": ",N2,", ""exMission2Score"": ",Q2,", ""exMission3Score"": ",T2," },")</f>
-        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A2,""", ""gateId"": ",B2,", ""miss1BaseAddr"": ",C2,", ""miss1EXBaseAddr"": ",M2,", ""mission1Score"": ",D2,", ""mission2Score"": ",G2,", ""mission3Score"": ",J2,", ""exMission1Score"": ",N2,", ""exMission2Score"": ",Q2,", ""exMission3Score"": ",T2,", ""mission1Id"": ",E2,", ""badge1Id"": ",F2,", ""mission2Id"": ",H2,", ""badge2Id"": ",I2,", ""mission3Id"": ",K2,", ""badge3Id"": ",L2,", ""exMission1Id"": ",O2,", ""exBadge1Id"": ",P2,", ""exMission2Id"": ",R2,", ""exBadge2Id"": ",S2,", ""exMission3Id"": ",U2,", ""exBadge3Id"": ",V2," },")</f>
+        <v>2: { "name": "Asteroid Sweep", "gateId": 0, "miss1BaseAddr": 0x0033bc10, "miss1EXBaseAddr": 0x0033c2d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357045, "badge1Id": 402244, "mission2Id": 357046, "badge2Id": 402245, "mission3Id": 357047, "badge3Id": 402246, "exMission1Id": 357048, "exBadge1Id": 402247, "exMission2Id": 357049, "exBadge2Id": 402248, "exMission3Id": 357050, "exBadge3Id": 402249 },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21911,8 +21911,8 @@
         <v>402255</v>
       </c>
       <c r="W3" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A3,""", ""gateId"": ",B3,", ""miss1BaseAddr"": ",C3,", ""miss1EXBaseAddr"": ",M3,", ""mission1Score"": ",D3,", ""mission2Score"": ",G3,", ""mission3Score"": ",J3,", ""exMission1Score"": ",N3,", ""exMission2Score"": ",Q3,", ""exMission3Score"": ",T3," },")</f>
-        <v>3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A3,""", ""gateId"": ",B3,", ""miss1BaseAddr"": ",C3,", ""miss1EXBaseAddr"": ",M3,", ""mission1Score"": ",D3,", ""mission2Score"": ",G3,", ""mission3Score"": ",J3,", ""exMission1Score"": ",N3,", ""exMission2Score"": ",Q3,", ""exMission3Score"": ",T3,", ""mission1Id"": ",E3,", ""badge1Id"": ",F3,", ""mission2Id"": ",H3,", ""badge2Id"": ",I3,", ""mission3Id"": ",K3,", ""badge3Id"": ",L3,", ""exMission1Id"": ",O3,", ""exBadge1Id"": ",P3,", ""exMission2Id"": ",R3,", ""exBadge2Id"": ",S3,", ""exMission3Id"": ",U3,", ""exBadge3Id"": ",V3," },")</f>
+        <v>3: { "name": "Stardust Sweep", "gateId": 1, "miss1BaseAddr": 0x0033bcd0, "miss1EXBaseAddr": 0x0033c390, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357051, "badge1Id": 402250, "mission2Id": 357053, "badge2Id": 402252, "mission3Id": 357055, "badge3Id": 402254, "exMission1Id": 357052, "exBadge1Id": 402251, "exMission2Id": 357054, "exBadge2Id": 402253, "exMission3Id": 357056, "exBadge3Id": 402255 },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21983,8 +21983,8 @@
         <v>402261</v>
       </c>
       <c r="W4" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A4,""", ""gateId"": ",B4,", ""miss1BaseAddr"": ",C4,", ""miss1EXBaseAddr"": ",M4,", ""mission1Score"": ",D4,", ""mission2Score"": ",G4,", ""mission3Score"": ",J4,", ""exMission1Score"": ",N4,", ""exMission2Score"": ",Q4,", ""exMission3Score"": ",T4," },")</f>
-        <v>4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A4,""", ""gateId"": ",B4,", ""miss1BaseAddr"": ",C4,", ""miss1EXBaseAddr"": ",M4,", ""mission1Score"": ",D4,", ""mission2Score"": ",G4,", ""mission3Score"": ",J4,", ""exMission1Score"": ",N4,", ""exMission2Score"": ",Q4,", ""exMission3Score"": ",T4,", ""mission1Id"": ",E4,", ""badge1Id"": ",F4,", ""mission2Id"": ",H4,", ""badge2Id"": ",I4,", ""mission3Id"": ",K4,", ""badge3Id"": ",L4,", ""exMission1Id"": ",O4,", ""exBadge1Id"": ",P4,", ""exMission2Id"": ",R4,", ""exBadge2Id"": ",S4,", ""exMission3Id"": ",U4,", ""exBadge3Id"": ",V4," },")</f>
+        <v>4: { "name": "Broken Highway", "gateId": 2, "miss1BaseAddr": 0x0033bd90, "miss1EXBaseAddr": 0x0033c450, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357057, "badge1Id": 402256, "mission2Id": 357059, "badge2Id": 402258, "mission3Id": 357061, "badge3Id": 402260, "exMission1Id": 357058, "exBadge1Id": 402257, "exMission2Id": 357060, "exBadge2Id": 402259, "exMission3Id": 357062, "exBadge3Id": 402261 },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22019,7 +22019,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>357063</v>
+        <v>357067</v>
       </c>
       <c r="L5" s="1" t="n">
         <v>402262</v>
@@ -22055,8 +22055,8 @@
         <v>402267</v>
       </c>
       <c r="W5" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A5,""", ""gateId"": ",B5,", ""miss1BaseAddr"": ",C5,", ""miss1EXBaseAddr"": ",M5,", ""mission1Score"": ",D5,", ""mission2Score"": ",G5,", ""mission3Score"": ",J5,", ""exMission1Score"": ",N5,", ""exMission2Score"": ",Q5,", ""exMission3Score"": ",T5," },")</f>
-        <v>5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A5,""", ""gateId"": ",B5,", ""miss1BaseAddr"": ",C5,", ""miss1EXBaseAddr"": ",M5,", ""mission1Score"": ",D5,", ""mission2Score"": ",G5,", ""mission3Score"": ",J5,", ""exMission1Score"": ",N5,", ""exMission2Score"": ",Q5,", ""exMission3Score"": ",T5,", ""mission1Id"": ",E5,", ""badge1Id"": ",F5,", ""mission2Id"": ",H5,", ""badge2Id"": ",I5,", ""mission3Id"": ",K5,", ""badge3Id"": ",L5,", ""exMission1Id"": ",O5,", ""exBadge1Id"": ",P5,", ""exMission2Id"": ",R5,", ""exBadge2Id"": ",S5,", ""exMission3Id"": ",U5,", ""exBadge3Id"": ",V5," },")</f>
+        <v>5: { "name": "Ancient Highway", "gateId": 3, "miss1BaseAddr": 0x0033be50, "miss1EXBaseAddr": 0x0033c510, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357063, "badge1Id": 402262, "mission2Id": 357065, "badge2Id": 402264, "mission3Id": 357067, "badge3Id": 402262, "exMission1Id": 357064, "exBadge1Id": 402263, "exMission2Id": 357066, "exBadge2Id": 402265, "exMission3Id": 357068, "exBadge3Id": 402267 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22127,8 +22127,8 @@
         <v>402273</v>
       </c>
       <c r="W6" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A6,""", ""gateId"": ",B6,", ""miss1BaseAddr"": ",C6,", ""miss1EXBaseAddr"": ",M6,", ""mission1Score"": ",D6,", ""mission2Score"": ",G6,", ""mission3Score"": ",J6,", ""exMission1Score"": ",N6,", ""exMission2Score"": ",Q6,", ""exMission3Score"": ",T6," },")</f>
-        <v>6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A6,""", ""gateId"": ",B6,", ""miss1BaseAddr"": ",C6,", ""miss1EXBaseAddr"": ",M6,", ""mission1Score"": ",D6,", ""mission2Score"": ",G6,", ""mission3Score"": ",J6,", ""exMission1Score"": ",N6,", ""exMission2Score"": ",Q6,", ""exMission3Score"": ",T6,", ""mission1Id"": ",E6,", ""badge1Id"": ",F6,", ""mission2Id"": ",H6,", ""badge2Id"": ",I6,", ""mission3Id"": ",K6,", ""badge3Id"": ",L6,", ""exMission1Id"": ",O6,", ""exBadge1Id"": ",P6,", ""exMission2Id"": ",R6,", ""exBadge2Id"": ",S6,", ""exMission3Id"": ",U6,", ""exBadge3Id"": ",V6," },")</f>
+        <v>6: { "name": "Phantom Storm", "gateId": 4, "miss1BaseAddr": 0x0033bf10, "miss1EXBaseAddr": 0x0033c5d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357069, "badge1Id": 402268, "mission2Id": 357071, "badge2Id": 402270, "mission3Id": 357073, "badge3Id": 402272, "exMission1Id": 357070, "exBadge1Id": 402269, "exMission2Id": 357072, "exBadge2Id": 402271, "exMission3Id": 357074, "exBadge3Id": 402273 },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22199,8 +22199,8 @@
         <v>402279</v>
       </c>
       <c r="W7" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A7,""", ""gateId"": ",B7,", ""miss1BaseAddr"": ",C7,", ""miss1EXBaseAddr"": ",M7,", ""mission1Score"": ",D7,", ""mission2Score"": ",G7,", ""mission3Score"": ",J7,", ""exMission1Score"": ",N7,", ""exMission2Score"": ",Q7,", ""exMission3Score"": ",T7," },")</f>
-        <v>7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A7,""", ""gateId"": ",B7,", ""miss1BaseAddr"": ",C7,", ""miss1EXBaseAddr"": ",M7,", ""mission1Score"": ",D7,", ""mission2Score"": ",G7,", ""mission3Score"": ",J7,", ""exMission1Score"": ",N7,", ""exMission2Score"": ",Q7,", ""exMission3Score"": ",T7,", ""mission1Id"": ",E7,", ""badge1Id"": ",F7,", ""mission2Id"": ",H7,", ""badge2Id"": ",I7,", ""mission3Id"": ",K7,", ""badge3Id"": ",L7,", ""exMission1Id"": ",O7,", ""exBadge1Id"": ",P7,", ""exMission2Id"": ",R7,", ""exBadge2Id"": ",S7,", ""exMission3Id"": ",U7,", ""exBadge3Id"": ",V7," },")</f>
+        <v>7: { "name": "Sunlight Storm", "gateId": 5, "miss1BaseAddr": 0x0033bfd0, "miss1EXBaseAddr": 0x0033c690, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357075, "badge1Id": 402274, "mission2Id": 357077, "badge2Id": 402276, "mission3Id": 357079, "badge3Id": 402278, "exMission1Id": 357076, "exBadge1Id": 402275, "exMission2Id": 357078, "exBadge2Id": 402277, "exMission3Id": 357080, "exBadge3Id": 402279 },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22271,8 +22271,8 @@
         <v>402285</v>
       </c>
       <c r="W8" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A8,""", ""gateId"": ",B8,", ""miss1BaseAddr"": ",C8,", ""miss1EXBaseAddr"": ",M8,", ""mission1Score"": ",D8,", ""mission2Score"": ",G8,", ""mission3Score"": ",J8,", ""exMission1Score"": ",N8,", ""exMission2Score"": ",Q8,", ""exMission3Score"": ",T8," },")</f>
-        <v>8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A8,""", ""gateId"": ",B8,", ""miss1BaseAddr"": ",C8,", ""miss1EXBaseAddr"": ",M8,", ""mission1Score"": ",D8,", ""mission2Score"": ",G8,", ""mission3Score"": ",J8,", ""exMission1Score"": ",N8,", ""exMission2Score"": ",Q8,", ""exMission3Score"": ",T8,", ""mission1Id"": ",E8,", ""badge1Id"": ",F8,", ""mission2Id"": ",H8,", ""badge2Id"": ",I8,", ""mission3Id"": ",K8,", ""badge3Id"": ",L8,", ""exMission1Id"": ",O8,", ""exBadge1Id"": ",P8,", ""exMission2Id"": ",R8,", ""exBadge2Id"": ",S8,", ""exMission3Id"": ",U8,", ""exBadge3Id"": ",V8," },")</f>
+        <v>8: { "name": "Splash Island", "gateId": 6, "miss1BaseAddr": 0x0033c090, "miss1EXBaseAddr": 0x0033c750, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357081, "badge1Id": 402280, "mission2Id": 357083, "badge2Id": 402282, "mission3Id": 357085, "badge3Id": 402284, "exMission1Id": 357082, "exBadge1Id": 402281, "exMission2Id": 357084, "exBadge2Id": 402283, "exMission3Id": 357086, "exBadge3Id": 402285 },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22343,8 +22343,8 @@
         <v>402292</v>
       </c>
       <c r="W9" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A9,""", ""gateId"": ",B9,", ""miss1BaseAddr"": ",C9,", ""miss1EXBaseAddr"": ",M9,", ""mission1Score"": ",D9,", ""mission2Score"": ",G9,", ""mission3Score"": ",J9,", ""exMission1Score"": ",N9,", ""exMission2Score"": ",Q9,", ""exMission3Score"": ",T9," },")</f>
-        <v>9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A9,""", ""gateId"": ",B9,", ""miss1BaseAddr"": ",C9,", ""miss1EXBaseAddr"": ",M9,", ""mission1Score"": ",D9,", ""mission2Score"": ",G9,", ""mission3Score"": ",J9,", ""exMission1Score"": ",N9,", ""exMission2Score"": ",Q9,", ""exMission3Score"": ",T9,", ""mission1Id"": ",E9,", ""badge1Id"": ",F9,", ""mission2Id"": ",H9,", ""badge2Id"": ",I9,", ""mission3Id"": ",K9,", ""badge3Id"": ",L9,", ""exMission1Id"": ",O9,", ""exBadge1Id"": ",P9,", ""exMission2Id"": ",R9,", ""exBadge2Id"": ",S9,", ""exMission3Id"": ",U9,", ""exBadge3Id"": ",V9," },")</f>
+        <v>9: { "name": "Floating Island", "gateId": 7, "miss1BaseAddr": 0x0033c150, "miss1EXBaseAddr": 0x0033c810, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357087, "badge1Id": 402286, "mission2Id": 357089, "badge2Id": 402289, "mission3Id": 357091, "badge3Id": 402291, "exMission1Id": 357088, "exBadge1Id": 402287, "exMission2Id": 357090, "exBadge2Id": 402290, "exMission3Id": 357092, "exBadge3Id": 402292 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22415,8 +22415,8 @@
         <v>402298</v>
       </c>
       <c r="W10" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A10,""", ""gateId"": ",B10,", ""miss1BaseAddr"": ",C10,", ""miss1EXBaseAddr"": ",M10,", ""mission1Score"": ",D10,", ""mission2Score"": ",G10,", ""mission3Score"": ",J10,", ""exMission1Score"": ",N10,", ""exMission2Score"": ",Q10,", ""exMission3Score"": ",T10," },")</f>
-        <v>10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10 },</v>
+        <f aca="false">_xlfn.CONCAT(ROW(),": { ","""name"": """,A10,""", ""gateId"": ",B10,", ""miss1BaseAddr"": ",C10,", ""miss1EXBaseAddr"": ",M10,", ""mission1Score"": ",D10,", ""mission2Score"": ",G10,", ""mission3Score"": ",J10,", ""exMission1Score"": ",N10,", ""exMission2Score"": ",Q10,", ""exMission3Score"": ",T10,", ""mission1Id"": ",E10,", ""badge1Id"": ",F10,", ""mission2Id"": ",H10,", ""badge2Id"": ",I10,", ""mission3Id"": ",K10,", ""badge3Id"": ",L10,", ""exMission1Id"": ",O10,", ""exBadge1Id"": ",P10,", ""exMission2Id"": ",R10,", ""exBadge2Id"": ",S10,", ""exMission3Id"": ",U10,", ""exBadge3Id"": ",V10," },")</f>
+        <v>10: { "name": "Assault of the Dreadnought", "gateId": 8, "miss1BaseAddr": 0x0033c210, "miss1EXBaseAddr": 0x0033c8d0, "mission1Score": 1, "mission2Score": 2, "mission3Score": 3, "exMission1Score": 5, "exMission2Score": 5, "exMission3Score": 10, "mission1Id": 357093, "badge1Id": 402293, "mission2Id": 357095, "badge2Id": 402295, "mission3Id": 357097, "badge3Id": 402297, "exMission1Id": 357094, "exBadge1Id": 402294, "exMission2Id": 357096, "exBadge2Id": 402296, "exMission3Id": 357098, "exBadge3Id": 402298 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26719,7 +26719,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3FA31AFC-B062-4414-BCAA-1073EA7852D0}</x14:id>
+          <x14:id>{F975F3CB-6474-46A4-B458-DC10E686D8EE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -26733,7 +26733,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7962ACDF-6054-4323-A2A8-8AF4B4FCEE50}</x14:id>
+          <x14:id>{287CD04D-A39F-49A1-B7FE-F0B1F0BA494E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -26749,7 +26749,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3FA31AFC-B062-4414-BCAA-1073EA7852D0}">
+          <x14:cfRule type="dataBar" id="{F975F3CB-6474-46A4-B458-DC10E686D8EE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -26760,7 +26760,7 @@
           <xm:sqref>A104:A1048576 A1:A102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7962ACDF-6054-4323-A2A8-8AF4B4FCEE50}">
+          <x14:cfRule type="dataBar" id="{287CD04D-A39F-49A1-B7FE-F0B1F0BA494E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Fixed some badge shenanigans
</commit_message>
<xml_diff>
--- a/Kingdom Hearts II Final Mix.xlsx
+++ b/Kingdom Hearts II Final Mix.xlsx
@@ -11139,9 +11139,9 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I52" activeCellId="0" sqref="I52"/>
+      <selection pane="bottomLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11195,7 +11195,7 @@
       </c>
       <c r="M1" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(K2:K1006)</f>
-        <v>2: { "eventKey": "Twilight Thorn", "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 1, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375937, "badgeId": "422503", "timeBattle": 0 }, 3: { "eventKey": "Axel", "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375938, "badgeId": "422504", "timeBattle": 0 }, 4: { "eventKey": "Shan-Yu", "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375939, "badgeId": "422505", "timeBattle": 0 }, 5: { "eventKey": "Thresholder", "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375940, "badgeId": "422506", "timeBattle": 0 }, 6: { "eventKey": "Dark Thorn", "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375941, "badgeId": "422507", "timeBattle": 0 }, 7: { "eventKey": "Cerberus", "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375942, "badgeId": "422508", "timeBattle": 0 }, 8: { "eventKey": "Olympus Pete", "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375943, "badgeId": "422509", "timeBattle": 0 }, 9: { "eventKey": "Timeless Pete", "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375944, "badgeId": "422510", "timeBattle": 0 }, 10: { "eventKey": "Hydra", "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375945, "badgeId": "422511", "timeBattle": 0 }, 11: { "eventKey": "Barbossa", "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375946, "badgeId": "422512", "timeBattle": 0 }, 12: { "eventKey": "Prison Keeper", "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375947, "badgeId": "422513", "timeBattle": 0 }, 13: { "eventKey": "Oogie Boogie", "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375948, "badgeId": "422514", "timeBattle": 0 }, 14: { "eventKey": "Volcano and Blizzard Lords", "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375949, "badgeId": "422515", "timeBattle": 0 }, 15: { "eventKey": "Scar", "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375950, "badgeId": "422516", "timeBattle": 0 }, 16: { "eventKey": "Pain and Panic Cup", "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 17: { "eventKey": "Monitors", "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 18: { "eventKey": "Hostile Program", "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375951, "badgeId": "422517", "timeBattle": 0 }, 19: { "eventKey": "Demyx", "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375952, "badgeId": "422518", "timeBattle": 0 }, 20: { "eventKey": "Battle of 1000 Heartless", "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1, "isProper": 1, "achId": 375953, "badgeId": "422519", "timeBattle": 0 }, 21: { "eventKey": "Storm Rider", "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375954, "badgeId": "422520", "timeBattle": 0 }, 22: { "eventKey": "Xaldin", "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375955, "badgeId": "422521", "timeBattle": 0 }, 23: { "eventKey": "Hades", "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375956, "badgeId": "422522", "timeBattle": 0 }, 24: { "eventKey": "Grim Reaper II", "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375957, "badgeId": "422523", "timeBattle": 0 }, 25: { "eventKey": "Experiment", "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375958, "badgeId": "422524", "timeBattle": 0 }, 26: { "eventKey": "Sandswept Ruins Escape", "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 27: { "eventKey": "Jafar", "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375959, "badgeId": "422525", "timeBattle": 0 }, 28: { "eventKey": "Groundshaker", "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375960, "badgeId": "422526", "timeBattle": 0 }, 29: { "eventKey": "Solar Sailer", "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 30: { "eventKey": "MCP", "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375961, "badgeId": "422527", "timeBattle": 0 }, 31: { "eventKey": "Sephiroth", "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375962, "badgeId": "422528", "timeBattle": 0 }, 32: { "eventKey": "Roxas", "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375963, "badgeId": "422529", "timeBattle": 0 }, 33: { "eventKey": "Xigbar", "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375964, "badgeId": "422530", "timeBattle": 0 }, 34: { "eventKey": "Luxord", "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375965, "badgeId": "422531", "timeBattle": 1 }, 35: { "eventKey": "Saïx", "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375967, "badgeId": "422532", "timeBattle": 0 }, 36: { "eventKey": "Xemnas I", "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422540", "timeBattle": 0 }, 37: { "eventKey": "Xemnas Cannons", "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 38: { "eventKey": "Ending Sequence", "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 39: { "eventKey": "Final Xemnas", "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375969, "badgeId": "422534", "timeBattle": 0 }, 40: { "eventKey": "Mail Delivery", "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 41: { "eventKey": "Cargo Climb", "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 42: { "eventKey": "Grandstander", "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 43: { "eventKey": "Poster Duty", "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 44: { "eventKey": "Bumble-Buster", "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 45: { "eventKey": "Junk Sweep", "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 46: { "eventKey": "Struggle: Hayner", "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 47: { "eventKey": "Struggle: Setzer", "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 48: { "eventKey": "Struggle: Seifer", "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 49: { "eventKey": "Skateboard Street Rave", "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 50: { "eventKey": "Zexion’s Absent Silhouette", "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375970, "badgeId": "422535", "timeBattle": 0 }, 51: { "eventKey": "Marluxia’s Absent Silhouette", "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375971, "badgeId": "422536", "timeBattle": 0 }, 52: { "eventKey": "Larxene’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375972, "badgeId": "422537", "timeBattle": 0 }, 53: { "eventKey": "Lexaeus’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375973, "badgeId": "422538", "timeBattle": 0 }, 54: { "eventKey": "Vexen’s Absent Silhouette", "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375974, "badgeId": "422539", "timeBattle": 0 }, 55: { "eventKey": "Phil’s Training – Maniac Mode", "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 56: { "eventKey": "Skateboard Freestyle", "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 57: { "eventKey": "Skateboard Time Attack", "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 58: { "eventKey": "Skateboard Sand Slider", "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 59: { "eventKey": "Skateboard Workshop Rave", "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 60: { "eventKey": "Light Cycle", "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 61: { "eventKey": "A Blustery Rescue", "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 62: { "eventKey": "Hunny Slider", "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 63: { "eventKey": "Balloon Bounce", "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 64: { "eventKey": "The Expotition", "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 65: { "eventKey": "The Hunny Pot", "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 66: { "eventKey": "Swim This Way", "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 67: { "eventKey": "Part of Your World", "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 68: { "eventKey": "Under the Sea", "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 69: { "eventKey": "Ursula’s Revenge", "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 70: { "eventKey": "A New Day Is Dawning", "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 71: { "eventKey": "Gift Wrapping", "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 72: { "eventKey": "Xemnas Dragon", "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 73: { "eventKey": "Magic Carpet", "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 74: { "eventKey": "Data Luxord", "locationCode": "NeverDivide", "eventId": 0x65, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375966, "badgeId": "422531", "timeBattle": 1 }, 75: { "eventKey": "Data Xemnas I", "locationCode": "NeverContortion", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422533", "timeBattle": 0 }, 76: { "eventKey": "Data Xemnas II", "locationCode": "NeverFinal", "eventId": 0x62, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375976, "badgeId": "422541", "timeBattle": 0 }, 77: { "eventKey": "Data Xigbar", "locationCode": "NeverHall", "eventId": 0x64, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375977, "badgeId": "422542", "timeBattle": 0 }, 78: { "eventKey": "Data Xaldin", "locationCode": "BeastBridge", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375978, "badgeId": "422543", "timeBattle": 0 }, 79: { "eventKey": "Data Vexen", "locationCode": "StationOfOblivionMansion", "eventId": 0x92, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375979, "badgeId": "422544", "timeBattle": 0 }, 80: { "eventKey": "Data Lexaeus", "locationCode": "StationOfOblivion2", "eventId": 0x93, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375980, "badgeId": "422545", "timeBattle": 0 }, 81: { "eventKey": "Data Zexion", "locationCode": "DestinyStorm", "eventId": 0x98, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375981, "badgeId": "422546", "timeBattle": 0 }, 82: { "eventKey": "Data Saïx", "locationCode": "NeverImpasse", "eventId": 0x66, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375982, "badgeId": "422547", "timeBattle": 0 }, 83: { "eventKey": "Data Axel", "locationCode": "BasementHallAxel", "eventId": 0xd5, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375983, "badgeId": "422548", "timeBattle": 0 }, 84: { "eventKey": "Data Demyx", "locationCode": "CastleGate", "eventId": 0x72, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375984, "badgeId": "422549", "timeBattle": 0 }, 85: { "eventKey": "Data Marluxia", "locationCode": "StationOfOblivion", "eventId": 0x96, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375985, "badgeId": "422550", "timeBattle": 0 }, 86: { "eventKey": "Data Larxene", "locationCode": "StationOfOblivion2", "eventId": 0x94, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375986, "badgeId": "422551", "timeBattle": 0 }, 87: { "eventKey": "Data Roxas", "locationCode": "NeverStation", "eventId": 0x63, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375987, "badgeId": "422552", "timeBattle": 0 }, 88: { "eventKey": "Lingering Will", "locationCode": "GraveyardBadlands", "eventId": 0x43, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, 89: { "eventKey": "Lingering Will 2", "locationCode": "GraveyardBadlands", "eventId": 0x49, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>2: { "eventKey": "Twilight Thorn", "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 1, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375937, "badgeId": "422503", "timeBattle": 0 },3: { "eventKey": "Axel", "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375938, "badgeId": "422504", "timeBattle": 0 },4: { "eventKey": "Shan-Yu", "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375939, "badgeId": "422505", "timeBattle": 0 },5: { "eventKey": "Thresholder", "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375940, "badgeId": "422506", "timeBattle": 0 },6: { "eventKey": "Dark Thorn", "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375941, "badgeId": "422507", "timeBattle": 0 },7: { "eventKey": "Cerberus", "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375942, "badgeId": "422508", "timeBattle": 0 },8: { "eventKey": "Olympus Pete", "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375943, "badgeId": "422509", "timeBattle": 0 },9: { "eventKey": "Timeless Pete", "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375944, "badgeId": "422510", "timeBattle": 0 },10: { "eventKey": "Hydra", "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375945, "badgeId": "422511", "timeBattle": 0 },11: { "eventKey": "Barbossa", "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375946, "badgeId": "422512", "timeBattle": 0 },12: { "eventKey": "Prison Keeper", "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375947, "badgeId": "422513", "timeBattle": 0 },13: { "eventKey": "Oogie Boogie", "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375948, "badgeId": "422514", "timeBattle": 0 },14: { "eventKey": "Volcano and Blizzard Lords", "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375949, "badgeId": "422515", "timeBattle": 0 },15: { "eventKey": "Scar", "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375950, "badgeId": "422516", "timeBattle": 0 },16: { "eventKey": "Pain and Panic Cup", "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },17: { "eventKey": "Monitors", "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },18: { "eventKey": "Hostile Program", "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375951, "badgeId": "422517", "timeBattle": 0 },19: { "eventKey": "Demyx", "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375952, "badgeId": "422518", "timeBattle": 0 },20: { "eventKey": "Battle of 1000 Heartless", "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1, "isProper": 1, "achId": 375953, "badgeId": "422519", "timeBattle": 0 },21: { "eventKey": "Storm Rider", "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375954, "badgeId": "422520", "timeBattle": 0 },22: { "eventKey": "Xaldin", "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375955, "badgeId": "422521", "timeBattle": 0 },23: { "eventKey": "Hades", "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375956, "badgeId": "422522", "timeBattle": 0 },24: { "eventKey": "Grim Reaper II", "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375957, "badgeId": "422523", "timeBattle": 0 },25: { "eventKey": "Experiment", "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375958, "badgeId": "422524", "timeBattle": 0 },26: { "eventKey": "Sandswept Ruins Escape", "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },27: { "eventKey": "Jafar", "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375959, "badgeId": "422525", "timeBattle": 0 },28: { "eventKey": "Groundshaker", "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375960, "badgeId": "422526", "timeBattle": 0 },29: { "eventKey": "Solar Sailer", "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },30: { "eventKey": "MCP", "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375961, "badgeId": "422527", "timeBattle": 0 },31: { "eventKey": "Sephiroth", "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375962, "badgeId": "422528", "timeBattle": 0 },32: { "eventKey": "Roxas", "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375963, "badgeId": "422529", "timeBattle": 0 },33: { "eventKey": "Xigbar", "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375964, "badgeId": "422530", "timeBattle": 0 },34: { "eventKey": "Luxord", "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375965, "badgeId": "422751", "timeBattle": 1 }, 35: { "eventKey": "Saïx", "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375967, "badgeId": "422532", "timeBattle": 0 },36: { "eventKey": "Xemnas I", "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422540", "timeBattle": 0 },37: { "eventKey": "Xemnas Cannons", "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },38: { "eventKey": "Ending Sequence", "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },39: { "eventKey": "Final Xemnas", "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375969, "badgeId": "422534", "timeBattle": 0 },40: { "eventKey": "Mail Delivery", "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },41: { "eventKey": "Cargo Climb", "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },42: { "eventKey": "Grandstander", "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },43: { "eventKey": "Poster Duty", "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },44: { "eventKey": "Bumble-Buster", "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },45: { "eventKey": "Junk Sweep", "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },46: { "eventKey": "Struggle: Hayner", "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },47: { "eventKey": "Struggle: Setzer", "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },48: { "eventKey": "Struggle: Seifer", "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },49: { "eventKey": "Skateboard Street Rave", "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },50: { "eventKey": "Zexion’s Absent Silhouette", "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375970, "badgeId": "422535", "timeBattle": 0 },51: { "eventKey": "Marluxia’s Absent Silhouette", "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375971, "badgeId": "422536", "timeBattle": 0 },52: { "eventKey": "Larxene’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375972, "badgeId": "422537", "timeBattle": 0 },53: { "eventKey": "Lexaeus’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375973, "badgeId": "422538", "timeBattle": 0 },54: { "eventKey": "Vexen’s Absent Silhouette", "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375974, "badgeId": "422539", "timeBattle": 0 },55: { "eventKey": "Phil’s Training – Maniac Mode", "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },56: { "eventKey": "Skateboard Freestyle", "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },57: { "eventKey": "Skateboard Time Attack", "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },58: { "eventKey": "Skateboard Sand Slider", "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },59: { "eventKey": "Skateboard Workshop Rave", "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },60: { "eventKey": "Light Cycle", "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },61: { "eventKey": "A Blustery Rescue", "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },62: { "eventKey": "Hunny Slider", "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },63: { "eventKey": "Balloon Bounce", "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },64: { "eventKey": "The Expotition", "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },65: { "eventKey": "The Hunny Pot", "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },66: { "eventKey": "Swim This Way", "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },67: { "eventKey": "Part of Your World", "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },68: { "eventKey": "Under the Sea", "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },69: { "eventKey": "Ursula’s Revenge", "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },70: { "eventKey": "A New Day Is Dawning", "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },71: { "eventKey": "Gift Wrapping", "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },72: { "eventKey": "Xemnas Dragon", "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },73: { "eventKey": "Magic Carpet", "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },74: { "eventKey": "Data Luxord", "locationCode": "NeverDivide", "eventId": 0x65, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375966, "badgeId": "422531", "timeBattle": 1 },75: { "eventKey": "Data Xemnas I", "locationCode": "NeverContortion", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422533", "timeBattle": 0 },76: { "eventKey": "Data Xemnas II", "locationCode": "NeverFinal", "eventId": 0x62, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375976, "badgeId": "422541", "timeBattle": 0 },77: { "eventKey": "Data Xigbar", "locationCode": "NeverHall", "eventId": 0x64, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375977, "badgeId": "422542", "timeBattle": 0 },78: { "eventKey": "Data Xaldin", "locationCode": "BeastBridge", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375978, "badgeId": "422543", "timeBattle": 0 },79: { "eventKey": "Data Vexen", "locationCode": "StationOfOblivionMansion", "eventId": 0x92, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375979, "badgeId": "422544", "timeBattle": 0 },80: { "eventKey": "Data Lexaeus", "locationCode": "StationOfOblivion2", "eventId": 0x93, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375980, "badgeId": "422545", "timeBattle": 0 },81: { "eventKey": "Data Zexion", "locationCode": "DestinyStorm", "eventId": 0x98, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375981, "badgeId": "422546", "timeBattle": 0 },82: { "eventKey": "Data Saïx", "locationCode": "NeverImpasse", "eventId": 0x66, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375982, "badgeId": "422547", "timeBattle": 0 },83: { "eventKey": "Data Axel", "locationCode": "BasementHallAxel", "eventId": 0xd5, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375983, "badgeId": "422548", "timeBattle": 0 },84: { "eventKey": "Data Demyx", "locationCode": "CastleGate", "eventId": 0x72, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375984, "badgeId": "422549", "timeBattle": 0 },85: { "eventKey": "Data Marluxia", "locationCode": "StationOfOblivion", "eventId": 0x96, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375985, "badgeId": "422550", "timeBattle": 0 },86: { "eventKey": "Data Larxene", "locationCode": "StationOfOblivion2", "eventId": 0x94, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375986, "badgeId": "422551", "timeBattle": 0 },87: { "eventKey": "Data Roxas", "locationCode": "NeverStation", "eventId": 0x63, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375987, "badgeId": "422552", "timeBattle": 0 },88: { "eventKey": "Lingering Will", "locationCode": "GraveyardBadlands", "eventId": 0x43, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },89: { "eventKey": "Lingering Will 2", "locationCode": "GraveyardBadlands", "eventId": 0x49, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11231,7 +11231,7 @@
       </c>
       <c r="K2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C2, """, ""locationCode"": """,B2,""", ""eventId"": 0x",A2,", ""score"": ",E2,", ""isBoss"": ",D2,", ""lv1"": ",F2,", ""isProper"": ",G2,", ""achId"": ",IF(ISBLANK(H2), 0, H2),", ""badgeId"": """,IF(ISBLANK(I2), 0, I2),""", ""timeBattle"": ",J2," }, ")</f>
-        <v>2: { "eventKey": "Twilight Thorn", "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 1, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375937, "badgeId": "422503", "timeBattle": 0 }, </v>
+        <v>2: { "eventKey": "Twilight Thorn", "locationCode": "StationOfAwakening", "eventId": 0x9d, "score": 1, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375937, "badgeId": "422503", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11267,7 +11267,7 @@
       </c>
       <c r="K3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C3, """, ""locationCode"": """,B3,""", ""eventId"": 0x",A3,", ""score"": ",E3,", ""isBoss"": ",D3,", ""lv1"": ",F3,", ""isProper"": ",G3,", ""achId"": ",IF(ISBLANK(H3), 0, H3),", ""badgeId"": """,IF(ISBLANK(I3), 0, I3),""", ""timeBattle"": ",J3," }, ")</f>
-        <v>3: { "eventKey": "Axel", "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375938, "badgeId": "422504", "timeBattle": 0 }, </v>
+        <v>3: { "eventKey": "Axel", "locationCode": "BasementHallAxel", "eventId": 0x89, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375938, "badgeId": "422504", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11303,7 +11303,7 @@
       </c>
       <c r="K4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C4, """, ""locationCode"": """,B4,""", ""eventId"": 0x",A4,", ""score"": ",E4,", ""isBoss"": ",D4,", ""lv1"": ",F4,", ""isProper"": ",G4,", ""achId"": ",IF(ISBLANK(H4), 0, H4),", ""badgeId"": """,IF(ISBLANK(I4), 0, I4),""", ""timeBattle"": ",J4," }, ")</f>
-        <v>4: { "eventKey": "Shan-Yu", "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375939, "badgeId": "422505", "timeBattle": 0 }, </v>
+        <v>4: { "eventKey": "Shan-Yu", "locationCode": "PalaceGate", "eventId": 0x4b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375939, "badgeId": "422505", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11339,7 +11339,7 @@
       </c>
       <c r="K5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C5, """, ""locationCode"": """,B5,""", ""eventId"": 0x",A5,", ""score"": ",E5,", ""isBoss"": ",D5,", ""lv1"": ",F5,", ""isProper"": ",G5,", ""achId"": ",IF(ISBLANK(H5), 0, H5),", ""badgeId"": """,IF(ISBLANK(I5), 0, I5),""", ""timeBattle"": ",J5," }, ")</f>
-        <v>5: { "eventKey": "Thresholder", "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375940, "badgeId": "422506", "timeBattle": 0 }, </v>
+        <v>5: { "eventKey": "Thresholder", "locationCode": "Undercroft", "eventId": 0x48, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375940, "badgeId": "422506", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11375,7 +11375,7 @@
       </c>
       <c r="K6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C6, """, ""locationCode"": """,B6,""", ""eventId"": 0x",A6,", ""score"": ",E6,", ""isBoss"": ",D6,", ""lv1"": ",F6,", ""isProper"": ",G6,", ""achId"": ",IF(ISBLANK(H6), 0, H6),", ""badgeId"": """,IF(ISBLANK(I6), 0, I6),""", ""timeBattle"": ",J6," }, ")</f>
-        <v>6: { "eventKey": "Dark Thorn", "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375941, "badgeId": "422507", "timeBattle": 0 }, </v>
+        <v>6: { "eventKey": "Dark Thorn", "locationCode": "BallroomBattle", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375941, "badgeId": "422507", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11411,7 +11411,7 @@
       </c>
       <c r="K7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C7, """, ""locationCode"": """,B7,""", ""eventId"": 0x",A7,", ""score"": ",E7,", ""isBoss"": ",D7,", ""lv1"": ",F7,", ""isProper"": ",G7,", ""achId"": ",IF(ISBLANK(H7), 0, H7),", ""badgeId"": """,IF(ISBLANK(I7), 0, I7),""", ""timeBattle"": ",J7," }, ")</f>
-        <v>7: { "eventKey": "Cerberus", "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375942, "badgeId": "422508", "timeBattle": 0 }, </v>
+        <v>7: { "eventKey": "Cerberus", "locationCode": "CaveOfTheDeadEntrance", "eventId": 0x72, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375942, "badgeId": "422508", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11447,7 +11447,7 @@
       </c>
       <c r="K8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C8, """, ""locationCode"": """,B8,""", ""eventId"": 0x",A8,", ""score"": ",E8,", ""isBoss"": ",D8,", ""lv1"": ",F8,", ""isProper"": ",G8,", ""achId"": ",IF(ISBLANK(H8), 0, H8),", ""badgeId"": """,IF(ISBLANK(I8), 0, I8),""", ""timeBattle"": ",J8," }, ")</f>
-        <v>8: { "eventKey": "Olympus Pete", "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375943, "badgeId": "422509", "timeBattle": 0 }, </v>
+        <v>8: { "eventKey": "Olympus Pete", "locationCode": "UnderworldLock2", "eventId": 0x74, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375943, "badgeId": "422509", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11483,7 +11483,7 @@
       </c>
       <c r="K9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C9, """, ""locationCode"": """,B9,""", ""eventId"": 0x",A9,", ""score"": ",E9,", ""isBoss"": ",D9,", ""lv1"": ",F9,", ""isProper"": ",G9,", ""achId"": ",IF(ISBLANK(H9), 0, H9),", ""badgeId"": """,IF(ISBLANK(I9), 0, I9),""", ""timeBattle"": ",J9," }, ")</f>
-        <v>9: { "eventKey": "Timeless Pete", "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375944, "badgeId": "422510", "timeBattle": 0 }, </v>
+        <v>9: { "eventKey": "Timeless Pete", "locationCode": "RiverWharf", "eventId": 0x35, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375944, "badgeId": "422510", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11519,7 +11519,7 @@
       </c>
       <c r="K10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C10, """, ""locationCode"": """,B10,""", ""eventId"": 0x",A10,", ""score"": ",E10,", ""isBoss"": ",D10,", ""lv1"": ",F10,", ""isProper"": ",G10,", ""achId"": ",IF(ISBLANK(H10), 0, H10),", ""badgeId"": """,IF(ISBLANK(I10), 0, I10),""", ""timeBattle"": ",J10," }, ")</f>
-        <v>10: { "eventKey": "Hydra", "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375945, "badgeId": "422511", "timeBattle": 0 }, </v>
+        <v>10: { "eventKey": "Hydra", "locationCode": "ColiseumGatesRuined", "eventId": 0xab, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375945, "badgeId": "422511", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11555,7 +11555,7 @@
       </c>
       <c r="K11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C11, """, ""locationCode"": """,B11,""", ""eventId"": 0x",A11,", ""score"": ",E11,", ""isBoss"": ",D11,", ""lv1"": ",F11,", ""isProper"": ",G11,", ""achId"": ",IF(ISBLANK(H11), 0, H11),", ""badgeId"": """,IF(ISBLANK(I11), 0, I11),""", ""timeBattle"": ",J11," }, ")</f>
-        <v>11: { "eventKey": "Barbossa", "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375946, "badgeId": "422512", "timeBattle": 0 }, </v>
+        <v>11: { "eventKey": "Barbossa", "locationCode": "PortHeap", "eventId": 0x3c, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375946, "badgeId": "422512", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11591,7 +11591,7 @@
       </c>
       <c r="K12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C12, """, ""locationCode"": """,B12,""", ""eventId"": 0x",A12,", ""score"": ",E12,", ""isBoss"": ",D12,", ""lv1"": ",F12,", ""isProper"": ",G12,", ""achId"": ",IF(ISBLANK(H12), 0, H12),", ""badgeId"": """,IF(ISBLANK(I12), 0, I12),""", ""timeBattle"": ",J12," }, ")</f>
-        <v>12: { "eventKey": "Prison Keeper", "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375947, "badgeId": "422513", "timeBattle": 0 }, </v>
+        <v>12: { "eventKey": "Prison Keeper", "locationCode": "HalloweenHill", "eventId": 0x34, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375947, "badgeId": "422513", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11627,7 +11627,7 @@
       </c>
       <c r="K13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C13, """, ""locationCode"": """,B13,""", ""eventId"": 0x",A13,", ""score"": ",E13,", ""isBoss"": ",D13,", ""lv1"": ",F13,", ""isProper"": ",G13,", ""achId"": ",IF(ISBLANK(H13), 0, H13),", ""badgeId"": """,IF(ISBLANK(I13), 0, I13),""", ""timeBattle"": ",J13," }, ")</f>
-        <v>13: { "eventKey": "Oogie Boogie", "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375948, "badgeId": "422514", "timeBattle": 0 }, </v>
+        <v>13: { "eventKey": "Oogie Boogie", "locationCode": "HalloweenFactory", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375948, "badgeId": "422514", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="K14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C14, """, ""locationCode"": """,B14,""", ""eventId"": 0x",A14,", ""score"": ",E14,", ""isBoss"": ",D14,", ""lv1"": ",F14,", ""isProper"": ",G14,", ""achId"": ",IF(ISBLANK(H14), 0, H14),", ""badgeId"": """,IF(ISBLANK(I14), 0, I14),""", ""timeBattle"": ",J14," }, ")</f>
-        <v>14: { "eventKey": "Volcano and Blizzard Lords", "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375949, "badgeId": "422515", "timeBattle": 0 }, </v>
+        <v>14: { "eventKey": "Volcano and Blizzard Lords", "locationCode": "AgrabahPalace", "eventId": 0x3b, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375949, "badgeId": "422515", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11699,7 +11699,7 @@
       </c>
       <c r="K15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C15, """, ""locationCode"": """,B15,""", ""eventId"": 0x",A15,", ""score"": ",E15,", ""isBoss"": ",D15,", ""lv1"": ",F15,", ""isProper"": ",G15,", ""achId"": ",IF(ISBLANK(H15), 0, H15),", ""badgeId"": """,IF(ISBLANK(I15), 0, I15),""", ""timeBattle"": ",J15," }, ")</f>
-        <v>15: { "eventKey": "Scar", "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375950, "badgeId": "422516", "timeBattle": 0 }, </v>
+        <v>15: { "eventKey": "Scar", "locationCode": "PridePeakBattle", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375950, "badgeId": "422516", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11729,7 +11729,7 @@
       </c>
       <c r="K16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C16, """, ""locationCode"": """,B16,""", ""eventId"": 0x",A16,", ""score"": ",E16,", ""isBoss"": ",D16,", ""lv1"": ",F16,", ""isProper"": ",G16,", ""achId"": ",IF(ISBLANK(H16), 0, H16),", ""badgeId"": """,IF(ISBLANK(I16), 0, I16),""", ""timeBattle"": ",J16," }, ")</f>
-        <v>16: { "eventKey": "Pain and Panic Cup", "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>16: { "eventKey": "Pain and Panic Cup", "locationCode": "ColiseumTourney1", "eventId": 0xbd, "score": 10, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11759,7 +11759,7 @@
       </c>
       <c r="K17" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C17, """, ""locationCode"": """,B17,""", ""eventId"": 0x",A17,", ""score"": ",E17,", ""isBoss"": ",D17,", ""lv1"": ",F17,", ""isProper"": ",G17,", ""achId"": ",IF(ISBLANK(H17), 0, H17),", ""badgeId"": """,IF(ISBLANK(I17), 0, I17),""", ""timeBattle"": ",J17," }, ")</f>
-        <v>17: { "eventKey": "Monitors", "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>17: { "eventKey": "Monitors", "locationCode": "SpaceDataspace", "eventId": 0x36, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11795,7 +11795,7 @@
       </c>
       <c r="K18" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C18, """, ""locationCode"": """,B18,""", ""eventId"": 0x",A18,", ""score"": ",E18,", ""isBoss"": ",D18,", ""lv1"": ",F18,", ""isProper"": ",G18,", ""achId"": ",IF(ISBLANK(H18), 0, H18),", ""badgeId"": """,IF(ISBLANK(I18), 0, I18),""", ""timeBattle"": ",J18," }, ")</f>
-        <v>18: { "eventKey": "Hostile Program", "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375951, "badgeId": "422517", "timeBattle": 0 }, </v>
+        <v>18: { "eventKey": "Hostile Program", "locationCode": "SpaceIOTowerHallway", "eventId": 0x37, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375951, "badgeId": "422517", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11831,7 +11831,7 @@
       </c>
       <c r="K19" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C19, """, ""locationCode"": """,B19,""", ""eventId"": 0x",A19,", ""score"": ",E19,", ""isBoss"": ",D19,", ""lv1"": ",F19,", ""isProper"": ",G19,", ""achId"": ",IF(ISBLANK(H19), 0, H19),", ""badgeId"": """,IF(ISBLANK(I19), 0, I19),""", ""timeBattle"": ",J19," }, ")</f>
-        <v>19: { "eventKey": "Demyx", "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375952, "badgeId": "422518", "timeBattle": 0 }, </v>
+        <v>19: { "eventKey": "Demyx", "locationCode": "CastleGate", "eventId": 0x37, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375952, "badgeId": "422518", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11867,7 +11867,7 @@
       </c>
       <c r="K20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C20, """, ""locationCode"": """,B20,""", ""eventId"": 0x",A20,", ""score"": ",E20,", ""isBoss"": ",D20,", ""lv1"": ",F20,", ""isProper"": ",G20,", ""achId"": ",IF(ISBLANK(H20), 0, H20),", ""badgeId"": """,IF(ISBLANK(I20), 0, I20),""", ""timeBattle"": ",J20," }, ")</f>
-        <v>20: { "eventKey": "Battle of 1000 Heartless", "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1, "isProper": 1, "achId": 375953, "badgeId": "422519", "timeBattle": 0 }, </v>
+        <v>20: { "eventKey": "Battle of 1000 Heartless", "locationCode": "GreatMaw", "eventId": 0x42, "score": 10, "isBoss": 0, "lv1": 1, "isProper": 1, "achId": 375953, "badgeId": "422519", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11903,7 +11903,7 @@
       </c>
       <c r="K21" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C21, """, ""locationCode"": """,B21,""", ""eventId"": 0x",A21,", ""score"": ",E21,", ""isBoss"": ",D21,", ""lv1"": ",F21,", ""isProper"": ",G21,", ""achId"": ",IF(ISBLANK(H21), 0, H21),", ""badgeId"": """,IF(ISBLANK(I21), 0, I21),""", ""timeBattle"": ",J21," }, ")</f>
-        <v>21: { "eventKey": "Storm Rider", "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375954, "badgeId": "422520", "timeBattle": 0 }, </v>
+        <v>21: { "eventKey": "Storm Rider", "locationCode": "ImperialSquare", "eventId": 0x4f, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375954, "badgeId": "422520", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11939,7 +11939,7 @@
       </c>
       <c r="K22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C22, """, ""locationCode"": """,B22,""", ""eventId"": 0x",A22,", ""score"": ",E22,", ""isBoss"": ",D22,", ""lv1"": ",F22,", ""isProper"": ",G22,", ""achId"": ",IF(ISBLANK(H22), 0, H22),", ""badgeId"": """,IF(ISBLANK(I22), 0, I22),""", ""timeBattle"": ",J22," }, ")</f>
-        <v>22: { "eventKey": "Xaldin", "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375955, "badgeId": "422521", "timeBattle": 0 }, </v>
+        <v>22: { "eventKey": "Xaldin", "locationCode": "BeastBridge", "eventId": 0x52, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375955, "badgeId": "422521", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11975,7 +11975,7 @@
       </c>
       <c r="K23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C23, """, ""locationCode"": """,B23,""", ""eventId"": 0x",A23,", ""score"": ",E23,", ""isBoss"": ",D23,", ""lv1"": ",F23,", ""isProper"": ",G23,", ""achId"": ",IF(ISBLANK(H23), 0, H23),", ""badgeId"": """,IF(ISBLANK(I23), 0, I23),""", ""timeBattle"": ",J23," }, ")</f>
-        <v>23: { "eventKey": "Hades", "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375956, "badgeId": "422522", "timeBattle": 0 }, </v>
+        <v>23: { "eventKey": "Hades", "locationCode": "ColiseumTourneyHades", "eventId": 0xca, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375956, "badgeId": "422522", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12011,7 +12011,7 @@
       </c>
       <c r="K24" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C24, """, ""locationCode"": """,B24,""", ""eventId"": 0x",A24,", ""score"": ",E24,", ""isBoss"": ",D24,", ""lv1"": ",F24,", ""isProper"": ",G24,", ""achId"": ",IF(ISBLANK(H24), 0, H24),", ""badgeId"": """,IF(ISBLANK(I24), 0, I24),""", ""timeBattle"": ",J24," }, ")</f>
-        <v>24: { "eventKey": "Grim Reaper II", "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375957, "badgeId": "422523", "timeBattle": 0 }, </v>
+        <v>24: { "eventKey": "Grim Reaper II", "locationCode": "PortHarbor", "eventId": 0x36, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375957, "badgeId": "422523", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12047,7 +12047,7 @@
       </c>
       <c r="K25" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C25, """, ""locationCode"": """,B25,""", ""eventId"": 0x",A25,", ""score"": ",E25,", ""isBoss"": ",D25,", ""lv1"": ",F25,", ""isProper"": ",G25,", ""achId"": ",IF(ISBLANK(H25), 0, H25),", ""badgeId"": """,IF(ISBLANK(I25), 0, I25),""", ""timeBattle"": ",J25," }, ")</f>
-        <v>25: { "eventKey": "Experiment", "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375958, "badgeId": "422524", "timeBattle": 0 }, </v>
+        <v>25: { "eventKey": "Experiment", "locationCode": "HalloweenPlaza", "eventId": 0x40, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375958, "badgeId": "422524", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="K26" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C26, """, ""locationCode"": """,B26,""", ""eventId"": 0x",A26,", ""score"": ",E26,", ""isBoss"": ",D26,", ""lv1"": ",F26,", ""isProper"": ",G26,", ""achId"": ",IF(ISBLANK(H26), 0, H26),", ""badgeId"": """,IF(ISBLANK(I26), 0, I26),""", ""timeBattle"": ",J26," }, ")</f>
-        <v>26: { "eventKey": "Sandswept Ruins Escape", "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>26: { "eventKey": "Sandswept Ruins Escape", "locationCode": "AgrabahSand", "eventId": 0x3d, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12113,7 +12113,7 @@
       </c>
       <c r="K27" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C27, """, ""locationCode"": """,B27,""", ""eventId"": 0x",A27,", ""score"": ",E27,", ""isBoss"": ",D27,", ""lv1"": ",F27,", ""isProper"": ",G27,", ""achId"": ",IF(ISBLANK(H27), 0, H27),", ""badgeId"": """,IF(ISBLANK(I27), 0, I27),""", ""timeBattle"": ",J27," }, ")</f>
-        <v>27: { "eventKey": "Jafar", "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375959, "badgeId": "422525", "timeBattle": 0 }, </v>
+        <v>27: { "eventKey": "Jafar", "locationCode": "AgrabahAbove", "eventId": 0x3e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375959, "badgeId": "422525", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12149,7 +12149,7 @@
       </c>
       <c r="K28" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C28, """, ""locationCode"": """,B28,""", ""eventId"": 0x",A28,", ""score"": ",E28,", ""isBoss"": ",D28,", ""lv1"": ",F28,", ""isProper"": ",G28,", ""achId"": ",IF(ISBLANK(H28), 0, H28),", ""badgeId"": """,IF(ISBLANK(I28), 0, I28),""", ""timeBattle"": ",J28," }, ")</f>
-        <v>28: { "eventKey": "Groundshaker", "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375960, "badgeId": "422526", "timeBattle": 0 }, </v>
+        <v>28: { "eventKey": "Groundshaker", "locationCode": "PrideSavannahBattle", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375960, "badgeId": "422526", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12179,7 +12179,7 @@
       </c>
       <c r="K29" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C29, """, ""locationCode"": """,B29,""", ""eventId"": 0x",A29,", ""score"": ",E29,", ""isBoss"": ",D29,", ""lv1"": ",F29,", ""isProper"": ",G29,", ""achId"": ",IF(ISBLANK(H29), 0, H29),", ""badgeId"": """,IF(ISBLANK(I29), 0, I29),""", ""timeBattle"": ",J29," }, ")</f>
-        <v>29: { "eventKey": "Solar Sailer", "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>29: { "eventKey": "Solar Sailer", "locationCode": "SpaceSailerBattle", "eventId": 0x39, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12215,7 +12215,7 @@
       </c>
       <c r="K30" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C30, """, ""locationCode"": """,B30,""", ""eventId"": 0x",A30,", ""score"": ",E30,", ""isBoss"": ",D30,", ""lv1"": ",F30,", ""isProper"": ",G30,", ""achId"": ",IF(ISBLANK(H30), 0, H30),", ""badgeId"": """,IF(ISBLANK(I30), 0, I30),""", ""timeBattle"": ",J30," }, ")</f>
-        <v>30: { "eventKey": "MCP", "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375961, "badgeId": "422527", "timeBattle": 0 }, </v>
+        <v>30: { "eventKey": "MCP", "locationCode": "SpaceCore", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 0, "achId": 375961, "badgeId": "422527", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12251,7 +12251,7 @@
       </c>
       <c r="K31" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C31, """, ""locationCode"": """,B31,""", ""eventId"": 0x",A31,", ""score"": ",E31,", ""isBoss"": ",D31,", ""lv1"": ",F31,", ""isProper"": ",G31,", ""achId"": ",IF(ISBLANK(H31), 0, H31),", ""badgeId"": """,IF(ISBLANK(I31), 0, I31),""", ""timeBattle"": ",J31," }, ")</f>
-        <v>31: { "eventKey": "Sephiroth", "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375962, "badgeId": "422528", "timeBattle": 0 }, </v>
+        <v>31: { "eventKey": "Sephiroth", "locationCode": "DarkDepths", "eventId": 0x4b, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375962, "badgeId": "422528", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12287,7 +12287,7 @@
       </c>
       <c r="K32" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C32, """, ""locationCode"": """,B32,""", ""eventId"": 0x",A32,", ""score"": ",E32,", ""isBoss"": ",D32,", ""lv1"": ",F32,", ""isProper"": ",G32,", ""achId"": ",IF(ISBLANK(H32), 0, H32),", ""badgeId"": """,IF(ISBLANK(I32), 0, I32),""", ""timeBattle"": ",J32," }, ")</f>
-        <v>32: { "eventKey": "Roxas", "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375963, "badgeId": "422529", "timeBattle": 0 }, </v>
+        <v>32: { "eventKey": "Roxas", "locationCode": "NeverStation", "eventId": 0x41, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375963, "badgeId": "422529", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="K33" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C33, """, ""locationCode"": """,B33,""", ""eventId"": 0x",A33,", ""score"": ",E33,", ""isBoss"": ",D33,", ""lv1"": ",F33,", ""isProper"": ",G33,", ""achId"": ",IF(ISBLANK(H33), 0, H33),", ""badgeId"": """,IF(ISBLANK(I33), 0, I33),""", ""timeBattle"": ",J33," }, ")</f>
-        <v>33: { "eventKey": "Xigbar", "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375964, "badgeId": "422530", "timeBattle": 0 }, </v>
+        <v>33: { "eventKey": "Xigbar", "locationCode": "NeverHall", "eventId": 0x39, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375964, "badgeId": "422530", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12352,14 +12352,14 @@
         <v>375965</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>422531</v>
+        <v>422751</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K34" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C34, """, ""locationCode"": """,B34,""", ""eventId"": 0x",A34,", ""score"": ",E34,", ""isBoss"": ",D34,", ""lv1"": ",F34,", ""isProper"": ",G34,", ""achId"": ",IF(ISBLANK(H34), 0, H34),", ""badgeId"": """,IF(ISBLANK(I34), 0, I34),""", ""timeBattle"": ",J34," }, ")</f>
-        <v>34: { "eventKey": "Luxord", "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375965, "badgeId": "422531", "timeBattle": 1 }, </v>
+        <v>34: { "eventKey": "Luxord", "locationCode": "NeverDivide", "eventId": 0x3a, "score": 5, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375965, "badgeId": "422751", "timeBattle": 1 }, </v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12395,7 +12395,7 @@
       </c>
       <c r="K35" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C35, """, ""locationCode"": """,B35,""", ""eventId"": 0x",A35,", ""score"": ",E35,", ""isBoss"": ",D35,", ""lv1"": ",F35,", ""isProper"": ",G35,", ""achId"": ",IF(ISBLANK(H35), 0, H35),", ""badgeId"": """,IF(ISBLANK(I35), 0, I35),""", ""timeBattle"": ",J35," }, ")</f>
-        <v>35: { "eventKey": "Saïx", "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375967, "badgeId": "422532", "timeBattle": 0 }, </v>
+        <v>35: { "eventKey": "Saïx", "locationCode": "NeverImpasse", "eventId": 0x38, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375967, "badgeId": "422532", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="K36" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C36, """, ""locationCode"": """,B36,""", ""eventId"": 0x",A36,", ""score"": ",E36,", ""isBoss"": ",D36,", ""lv1"": ",F36,", ""isProper"": ",G36,", ""achId"": ",IF(ISBLANK(H36), 0, H36),", ""badgeId"": """,IF(ISBLANK(I36), 0, I36),""", ""timeBattle"": ",J36," }, ")</f>
-        <v>36: { "eventKey": "Xemnas I", "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422540", "timeBattle": 0 }, </v>
+        <v>36: { "eventKey": "Xemnas I", "locationCode": "NeverContortion", "eventId": 0x3b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422540", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12461,7 +12461,7 @@
       </c>
       <c r="K37" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C37, """, ""locationCode"": """,B37,""", ""eventId"": 0x",A37,", ""score"": ",E37,", ""isBoss"": ",D37,", ""lv1"": ",F37,", ""isProper"": ",G37,", ""achId"": ",IF(ISBLANK(H37), 0, H37),", ""badgeId"": """,IF(ISBLANK(I37), 0, I37),""", ""timeBattle"": ",J37," }, ")</f>
-        <v>37: { "eventKey": "Xemnas Cannons", "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>37: { "eventKey": "Xemnas Cannons", "locationCode": "NeverCannons", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12491,7 +12491,7 @@
       </c>
       <c r="K38" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C38, """, ""locationCode"": """,B38,""", ""eventId"": 0x",A38,", ""score"": ",E38,", ""isBoss"": ",D38,", ""lv1"": ",F38,", ""isProper"": ",G38,", ""achId"": ",IF(ISBLANK(H38), 0, H38),", ""badgeId"": """,IF(ISBLANK(I38), 0, I38),""", ""timeBattle"": ",J38," }, ")</f>
-        <v>38: { "eventKey": "Ending Sequence", "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>38: { "eventKey": "Ending Sequence", "locationCode": "DarkMargin", "eventId": 0x3a, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 1, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12527,7 +12527,7 @@
       </c>
       <c r="K39" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C39, """, ""locationCode"": """,B39,""", ""eventId"": 0x",A39,", ""score"": ",E39,", ""isBoss"": ",D39,", ""lv1"": ",F39,", ""isProper"": ",G39,", ""achId"": ",IF(ISBLANK(H39), 0, H39),", ""badgeId"": """,IF(ISBLANK(I39), 0, I39),""", ""timeBattle"": ",J39," }, ")</f>
-        <v>39: { "eventKey": "Final Xemnas", "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375969, "badgeId": "422534", "timeBattle": 0 }, </v>
+        <v>39: { "eventKey": "Final Xemnas", "locationCode": "NeverFinal", "eventId": 0x4a, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375969, "badgeId": "422534", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12557,7 +12557,7 @@
       </c>
       <c r="K40" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C40, """, ""locationCode"": """,B40,""", ""eventId"": 0x",A40,", ""score"": ",E40,", ""isBoss"": ",D40,", ""lv1"": ",F40,", ""isProper"": ",G40,", ""achId"": ",IF(ISBLANK(H40), 0, H40),", ""badgeId"": """,IF(ISBLANK(I40), 0, I40),""", ""timeBattle"": ",J40," }, ")</f>
-        <v>40: { "eventKey": "Mail Delivery", "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>40: { "eventKey": "Mail Delivery", "locationCode": "StationHeights", "eventId": 0xc3, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12587,7 +12587,7 @@
       </c>
       <c r="K41" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C41, """, ""locationCode"": """,B41,""", ""eventId"": 0x",A41,", ""score"": ",E41,", ""isBoss"": ",D41,", ""lv1"": ",F41,", ""isProper"": ",G41,", ""achId"": ",IF(ISBLANK(H41), 0, H41),", ""badgeId"": """,IF(ISBLANK(I41), 0, I41),""", ""timeBattle"": ",J41," }, ")</f>
-        <v>41: { "eventKey": "Cargo Climb", "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>41: { "eventKey": "Cargo Climb", "locationCode": "StationHeights", "eventId": 0xc1, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12617,7 +12617,7 @@
       </c>
       <c r="K42" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C42, """, ""locationCode"": """,B42,""", ""eventId"": 0x",A42,", ""score"": ",E42,", ""isBoss"": ",D42,", ""lv1"": ",F42,", ""isProper"": ",G42,", ""achId"": ",IF(ISBLANK(H42), 0, H42),", ""badgeId"": """,IF(ISBLANK(I42), 0, I42),""", ""timeBattle"": ",J42," }, ")</f>
-        <v>42: { "eventKey": "Grandstander", "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>42: { "eventKey": "Grandstander", "locationCode": "StationHeights", "eventId": 0xc2, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12647,7 +12647,7 @@
       </c>
       <c r="K43" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C43, """, ""locationCode"": """,B43,""", ""eventId"": 0x",A43,", ""score"": ",E43,", ""isBoss"": ",D43,", ""lv1"": ",F43,", ""isProper"": ",G43,", ""achId"": ",IF(ISBLANK(H43), 0, H43),", ""badgeId"": """,IF(ISBLANK(I43), 0, I43),""", ""timeBattle"": ",J43," }, ")</f>
-        <v>43: { "eventKey": "Poster Duty", "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>43: { "eventKey": "Poster Duty", "locationCode": "TramCommon", "eventId": 0xc9, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12677,7 +12677,7 @@
       </c>
       <c r="K44" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C44, """, ""locationCode"": """,B44,""", ""eventId"": 0x",A44,", ""score"": ",E44,", ""isBoss"": ",D44,", ""lv1"": ",F44,", ""isProper"": ",G44,", ""achId"": ",IF(ISBLANK(H44), 0, H44),", ""badgeId"": """,IF(ISBLANK(I44), 0, I44),""", ""timeBattle"": ",J44," }, ")</f>
-        <v>44: { "eventKey": "Bumble-Buster", "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>44: { "eventKey": "Bumble-Buster", "locationCode": "TramCommon", "eventId": 0xc8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12707,7 +12707,7 @@
       </c>
       <c r="K45" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C45, """, ""locationCode"": """,B45,""", ""eventId"": 0x",A45,", ""score"": ",E45,", ""isBoss"": ",D45,", ""lv1"": ",F45,", ""isProper"": ",G45,", ""achId"": ",IF(ISBLANK(H45), 0, H45),", ""badgeId"": """,IF(ISBLANK(I45), 0, I45),""", ""timeBattle"": ",J45," }, ")</f>
-        <v>45: { "eventKey": "Junk Sweep", "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>45: { "eventKey": "Junk Sweep", "locationCode": "TramCommon", "eventId": 0xc7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12737,7 +12737,7 @@
       </c>
       <c r="K46" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C46, """, ""locationCode"": """,B46,""", ""eventId"": 0x",A46,", ""score"": ",E46,", ""isBoss"": ",D46,", ""lv1"": ",F46,", ""isProper"": ",G46,", ""achId"": ",IF(ISBLANK(H46), 0, H46),", ""badgeId"": """,IF(ISBLANK(I46), 0, I46),""", ""timeBattle"": ",J46," }, ")</f>
-        <v>46: { "eventKey": "Struggle: Hayner", "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>46: { "eventKey": "Struggle: Hayner", "locationCode": "Sandlot", "eventId": 0xb6, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12767,7 +12767,7 @@
       </c>
       <c r="K47" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C47, """, ""locationCode"": """,B47,""", ""eventId"": 0x",A47,", ""score"": ",E47,", ""isBoss"": ",D47,", ""lv1"": ",F47,", ""isProper"": ",G47,", ""achId"": ",IF(ISBLANK(H47), 0, H47),", ""badgeId"": """,IF(ISBLANK(I47), 0, I47),""", ""timeBattle"": ",J47," }, ")</f>
-        <v>47: { "eventKey": "Struggle: Setzer", "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>47: { "eventKey": "Struggle: Setzer", "locationCode": "Sandlot", "eventId": 0xb7, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12797,7 +12797,7 @@
       </c>
       <c r="K48" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C48, """, ""locationCode"": """,B48,""", ""eventId"": 0x",A48,", ""score"": ",E48,", ""isBoss"": ",D48,", ""lv1"": ",F48,", ""isProper"": ",G48,", ""achId"": ",IF(ISBLANK(H48), 0, H48),", ""badgeId"": """,IF(ISBLANK(I48), 0, I48),""", ""timeBattle"": ",J48," }, ")</f>
-        <v>48: { "eventKey": "Struggle: Seifer", "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>48: { "eventKey": "Struggle: Seifer", "locationCode": "Sandlot", "eventId": 0xb8, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12827,7 +12827,7 @@
       </c>
       <c r="K49" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C49, """, ""locationCode"": """,B49,""", ""eventId"": 0x",A49,", ""score"": ",E49,", ""isBoss"": ",D49,", ""lv1"": ",F49,", ""isProper"": ",G49,", ""achId"": ",IF(ISBLANK(H49), 0, H49),", ""badgeId"": """,IF(ISBLANK(I49), 0, I49),""", ""timeBattle"": ",J49," }, ")</f>
-        <v>49: { "eventKey": "Skateboard Street Rave", "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>49: { "eventKey": "Skateboard Street Rave", "locationCode": "TramCommon", "eventId": 0xbb, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12863,7 +12863,7 @@
       </c>
       <c r="K50" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C50, """, ""locationCode"": """,B50,""", ""eventId"": 0x",A50,", ""score"": ",E50,", ""isBoss"": ",D50,", ""lv1"": ",F50,", ""isProper"": ",G50,", ""achId"": ",IF(ISBLANK(H50), 0, H50),", ""badgeId"": """,IF(ISBLANK(I50), 0, I50),""", ""timeBattle"": ",J50," }, ")</f>
-        <v>50: { "eventKey": "Zexion’s Absent Silhouette", "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375970, "badgeId": "422535", "timeBattle": 0 }, </v>
+        <v>50: { "eventKey": "Zexion’s Absent Silhouette", "locationCode": "DestinyStorm", "eventId": 0x97, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375970, "badgeId": "422535", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12899,7 +12899,7 @@
       </c>
       <c r="K51" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C51, """, ""locationCode"": """,B51,""", ""eventId"": 0x",A51,", ""score"": ",E51,", ""isBoss"": ",D51,", ""lv1"": ",F51,", ""isProper"": ",G51,", ""achId"": ",IF(ISBLANK(H51), 0, H51),", ""badgeId"": """,IF(ISBLANK(I51), 0, I51),""", ""timeBattle"": ",J51," }, ")</f>
-        <v>51: { "eventKey": "Marluxia’s Absent Silhouette", "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375971, "badgeId": "422536", "timeBattle": 0 }, </v>
+        <v>51: { "eventKey": "Marluxia’s Absent Silhouette", "locationCode": "StationOfOblivion", "eventId": 0x91, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375971, "badgeId": "422536", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12935,7 +12935,7 @@
       </c>
       <c r="K52" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C52, """, ""locationCode"": """,B52,""", ""eventId"": 0x",A52,", ""score"": ",E52,", ""isBoss"": ",D52,", ""lv1"": ",F52,", ""isProper"": ",G52,", ""achId"": ",IF(ISBLANK(H52), 0, H52),", ""badgeId"": """,IF(ISBLANK(I52), 0, I52),""", ""timeBattle"": ",J52," }, ")</f>
-        <v>52: { "eventKey": "Larxene’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375972, "badgeId": "422537", "timeBattle": 0 }, </v>
+        <v>52: { "eventKey": "Larxene’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x9b, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375972, "badgeId": "422537", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12971,7 +12971,7 @@
       </c>
       <c r="K53" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C53, """, ""locationCode"": """,B53,""", ""eventId"": 0x",A53,", ""score"": ",E53,", ""isBoss"": ",D53,", ""lv1"": ",F53,", ""isProper"": ",G53,", ""achId"": ",IF(ISBLANK(H53), 0, H53),", ""badgeId"": """,IF(ISBLANK(I53), 0, I53),""", ""timeBattle"": ",J53," }, ")</f>
-        <v>53: { "eventKey": "Lexaeus’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375973, "badgeId": "422538", "timeBattle": 0 }, </v>
+        <v>53: { "eventKey": "Lexaeus’s Absent Silhouette", "locationCode": "StationOfOblivion2", "eventId": 0x8e, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375973, "badgeId": "422538", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13007,7 +13007,7 @@
       </c>
       <c r="K54" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C54, """, ""locationCode"": """,B54,""", ""eventId"": 0x",A54,", ""score"": ",E54,", ""isBoss"": ",D54,", ""lv1"": ",F54,", ""isProper"": ",G54,", ""achId"": ",IF(ISBLANK(H54), 0, H54),", ""badgeId"": """,IF(ISBLANK(I54), 0, I54),""", ""timeBattle"": ",J54," }, ")</f>
-        <v>54: { "eventKey": "Vexen’s Absent Silhouette", "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375974, "badgeId": "422539", "timeBattle": 0 }, </v>
+        <v>54: { "eventKey": "Vexen’s Absent Silhouette", "locationCode": "StationOfOblivionMansion", "eventId": 0x73, "score": 10, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375974, "badgeId": "422539", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13037,7 +13037,7 @@
       </c>
       <c r="K55" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C55, """, ""locationCode"": """,B55,""", ""eventId"": 0x",A55,", ""score"": ",E55,", ""isBoss"": ",D55,", ""lv1"": ",F55,", ""isProper"": ",G55,", ""achId"": ",IF(ISBLANK(H55), 0, H55),", ""badgeId"": """,IF(ISBLANK(I55), 0, I55),""", ""timeBattle"": ",J55," }, ")</f>
-        <v>55: { "eventKey": "Phil’s Training – Maniac Mode", "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>55: { "eventKey": "Phil’s Training – Maniac Mode", "locationCode": "ColiseumGatesRuined2", "eventId": 0x8f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13067,7 +13067,7 @@
       </c>
       <c r="K56" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C56, """, ""locationCode"": """,B56,""", ""eventId"": 0x",A56,", ""score"": ",E56,", ""isBoss"": ",D56,", ""lv1"": ",F56,", ""isProper"": ",G56,", ""achId"": ",IF(ISBLANK(H56), 0, H56),", ""badgeId"": """,IF(ISBLANK(I56), 0, I56),""", ""timeBattle"": ",J56," }, ")</f>
-        <v>56: { "eventKey": "Skateboard Freestyle", "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>56: { "eventKey": "Skateboard Freestyle", "locationCode": "Borough", "eventId": 0x64, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13097,7 +13097,7 @@
       </c>
       <c r="K57" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C57, """, ""locationCode"": """,B57,""", ""eventId"": 0x",A57,", ""score"": ",E57,", ""isBoss"": ",D57,", ""lv1"": ",F57,", ""isProper"": ",G57,", ""achId"": ",IF(ISBLANK(H57), 0, H57),", ""badgeId"": """,IF(ISBLANK(I57), 0, I57),""", ""timeBattle"": ",J57," }, ")</f>
-        <v>57: { "eventKey": "Skateboard Time Attack", "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>57: { "eventKey": "Skateboard Time Attack", "locationCode": "PortTown", "eventId": 0x58, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13127,7 +13127,7 @@
       </c>
       <c r="K58" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C58, """, ""locationCode"": """,B58,""", ""eventId"": 0x",A58,", ""score"": ",E58,", ""isBoss"": ",D58,", ""lv1"": ",F58,", ""isProper"": ",G58,", ""achId"": ",IF(ISBLANK(H58), 0, H58),", ""badgeId"": """,IF(ISBLANK(I58), 0, I58),""", ""timeBattle"": ",J58," }, ")</f>
-        <v>58: { "eventKey": "Skateboard Sand Slider", "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>58: { "eventKey": "Skateboard Sand Slider", "locationCode": "Agrabah", "eventId": 0x6e, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13157,7 +13157,7 @@
       </c>
       <c r="K59" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C59, """, ""locationCode"": """,B59,""", ""eventId"": 0x",A59,", ""score"": ",E59,", ""isBoss"": ",D59,", ""lv1"": ",F59,", ""isProper"": ",G59,", ""achId"": ",IF(ISBLANK(H59), 0, H59),", ""badgeId"": """,IF(ISBLANK(I59), 0, I59),""", ""timeBattle"": ",J59," }, ")</f>
-        <v>59: { "eventKey": "Skateboard Workshop Rave", "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>59: { "eventKey": "Skateboard Workshop Rave", "locationCode": "HalloweenFactory", "eventId": 0x4b, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13187,7 +13187,7 @@
       </c>
       <c r="K60" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C60, """, ""locationCode"": """,B60,""", ""eventId"": 0x",A60,", ""score"": ",E60,", ""isBoss"": ",D60,", ""lv1"": ",F60,", ""isProper"": ",G60,", ""achId"": ",IF(ISBLANK(H60), 0, H60),", ""badgeId"": """,IF(ISBLANK(I60), 0, I60),""", ""timeBattle"": ",J60," }, ")</f>
-        <v>60: { "eventKey": "Light Cycle", "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>60: { "eventKey": "Light Cycle", "locationCode": "SpaceGrid", "eventId": 0x3f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13217,7 +13217,7 @@
       </c>
       <c r="K61" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C61, """, ""locationCode"": """,B61,""", ""eventId"": 0x",A61,", ""score"": ",E61,", ""isBoss"": ",D61,", ""lv1"": ",F61,", ""isProper"": ",G61,", ""achId"": ",IF(ISBLANK(H61), 0, H61),", ""badgeId"": """,IF(ISBLANK(I61), 0, I61),""", ""timeBattle"": ",J61," }, ")</f>
-        <v>61: { "eventKey": "A Blustery Rescue", "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>61: { "eventKey": "A Blustery Rescue", "locationCode": "PigletRescue", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13247,7 +13247,7 @@
       </c>
       <c r="K62" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C62, """, ""locationCode"": """,B62,""", ""eventId"": 0x",A62,", ""score"": ",E62,", ""isBoss"": ",D62,", ""lv1"": ",F62,", ""isProper"": ",G62,", ""achId"": ",IF(ISBLANK(H62), 0, H62),", ""badgeId"": """,IF(ISBLANK(I62), 0, I62),""", ""timeBattle"": ",J62," }, ")</f>
-        <v>62: { "eventKey": "Hunny Slider", "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>62: { "eventKey": "Hunny Slider", "locationCode": "HunnySlider", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13277,7 +13277,7 @@
       </c>
       <c r="K63" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C63, """, ""locationCode"": """,B63,""", ""eventId"": 0x",A63,", ""score"": ",E63,", ""isBoss"": ",D63,", ""lv1"": ",F63,", ""isProper"": ",G63,", ""achId"": ",IF(ISBLANK(H63), 0, H63),", ""badgeId"": """,IF(ISBLANK(I63), 0, I63),""", ""timeBattle"": ",J63," }, ")</f>
-        <v>63: { "eventKey": "Balloon Bounce", "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>63: { "eventKey": "Balloon Bounce", "locationCode": "BalloonBounce", "eventId": 0x47, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13307,7 +13307,7 @@
       </c>
       <c r="K64" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C64, """, ""locationCode"": """,B64,""", ""eventId"": 0x",A64,", ""score"": ",E64,", ""isBoss"": ",D64,", ""lv1"": ",F64,", ""isProper"": ",G64,", ""achId"": ",IF(ISBLANK(H64), 0, H64),", ""badgeId"": """,IF(ISBLANK(I64), 0, I64),""", ""timeBattle"": ",J64," }, ")</f>
-        <v>64: { "eventKey": "The Expotition", "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>64: { "eventKey": "The Expotition", "locationCode": "SpookyCave", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13337,7 +13337,7 @@
       </c>
       <c r="K65" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C65, """, ""locationCode"": """,B65,""", ""eventId"": 0x",A65,", ""score"": ",E65,", ""isBoss"": ",D65,", ""lv1"": ",F65,", ""isProper"": ",G65,", ""achId"": ",IF(ISBLANK(H65), 0, H65),", ""badgeId"": """,IF(ISBLANK(I65), 0, I65),""", ""timeBattle"": ",J65," }, ")</f>
-        <v>65: { "eventKey": "The Hunny Pot", "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>65: { "eventKey": "The Hunny Pot", "locationCode": "StarryHill", "eventId": 0x49, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13367,7 +13367,7 @@
       </c>
       <c r="K66" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C66, """, ""locationCode"": """,B66,""", ""eventId"": 0x",A66,", ""score"": ",E66,", ""isBoss"": ",D66,", ""lv1"": ",F66,", ""isProper"": ",G66,", ""achId"": ",IF(ISBLANK(H66), 0, H66),", ""badgeId"": """,IF(ISBLANK(I66), 0, I66),""", ""timeBattle"": ",J66," }, ")</f>
-        <v>66: { "eventKey": "Swim This Way", "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>66: { "eventKey": "Swim This Way", "locationCode": "AtlanticaOrchestra", "eventId": 0x42, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13397,7 +13397,7 @@
       </c>
       <c r="K67" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C67, """, ""locationCode"": """,B67,""", ""eventId"": 0x",A67,", ""score"": ",E67,", ""isBoss"": ",D67,", ""lv1"": ",F67,", ""isProper"": ",G67,", ""achId"": ",IF(ISBLANK(H67), 0, H67),", ""badgeId"": """,IF(ISBLANK(I67), 0, I67),""", ""timeBattle"": ",J67," }, ")</f>
-        <v>67: { "eventKey": "Part of Your World", "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>67: { "eventKey": "Part of Your World", "locationCode": "AtlanticaGrotto", "eventId": 0x43, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13427,7 +13427,7 @@
       </c>
       <c r="K68" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C68, """, ""locationCode"": """,B68,""", ""eventId"": 0x",A68,", ""score"": ",E68,", ""isBoss"": ",D68,", ""lv1"": ",F68,", ""isProper"": ",G68,", ""achId"": ",IF(ISBLANK(H68), 0, H68),", ""badgeId"": """,IF(ISBLANK(I68), 0, I68),""", ""timeBattle"": ",J68," }, ")</f>
-        <v>68: { "eventKey": "Under the Sea", "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>68: { "eventKey": "Under the Sea", "locationCode": "AtlanticaCourtyard", "eventId": 0x44, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13457,7 +13457,7 @@
       </c>
       <c r="K69" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C69, """, ""locationCode"": """,B69,""", ""eventId"": 0x",A69,", ""score"": ",E69,", ""isBoss"": ",D69,", ""lv1"": ",F69,", ""isProper"": ",G69,", ""achId"": ",IF(ISBLANK(H69), 0, H69),", ""badgeId"": """,IF(ISBLANK(I69), 0, I69),""", ""timeBattle"": ",J69," }, ")</f>
-        <v>69: { "eventKey": "Ursula’s Revenge", "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>69: { "eventKey": "Ursula’s Revenge", "locationCode": "AtlanticaWrath", "eventId": 0x45, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13487,7 +13487,7 @@
       </c>
       <c r="K70" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C70, """, ""locationCode"": """,B70,""", ""eventId"": 0x",A70,", ""score"": ",E70,", ""isBoss"": ",D70,", ""lv1"": ",F70,", ""isProper"": ",G70,", ""achId"": ",IF(ISBLANK(H70), 0, H70),", ""badgeId"": """,IF(ISBLANK(I70), 0, I70),""", ""timeBattle"": ",J70," }, ")</f>
-        <v>70: { "eventKey": "A New Day Is Dawning", "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>70: { "eventKey": "A New Day Is Dawning", "locationCode": "AtlanticaOrchestra", "eventId": 0x46, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13517,7 +13517,7 @@
       </c>
       <c r="K71" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C71, """, ""locationCode"": """,B71,""", ""eventId"": 0x",A71,", ""score"": ",E71,", ""isBoss"": ",D71,", ""lv1"": ",F71,", ""isProper"": ",G71,", ""achId"": ",IF(ISBLANK(H71), 0, H71),", ""badgeId"": """,IF(ISBLANK(I71), 0, I71),""", ""timeBattle"": ",J71," }, ")</f>
-        <v>71: { "eventKey": "Gift Wrapping", "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>71: { "eventKey": "Gift Wrapping", "locationCode": "HalloweenWrapping", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13547,7 +13547,7 @@
       </c>
       <c r="K72" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C72, """, ""locationCode"": """,B72,""", ""eventId"": 0x",A72,", ""score"": ",E72,", ""isBoss"": ",D72,", ""lv1"": ",F72,", ""isProper"": ",G72,", ""achId"": ",IF(ISBLANK(H72), 0, H72),", ""badgeId"": """,IF(ISBLANK(I72), 0, I72),""", ""timeBattle"": ",J72," }, ")</f>
-        <v>72: { "eventKey": "Xemnas Dragon", "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>72: { "eventKey": "Xemnas Dragon", "locationCode": "NeverDragon", "eventId": 0x48, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13577,7 +13577,7 @@
       </c>
       <c r="K73" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C73, """, ""locationCode"": """,B73,""", ""eventId"": 0x",A73,", ""score"": ",E73,", ""isBoss"": ",D73,", ""lv1"": ",F73,", ""isProper"": ",G73,", ""achId"": ",IF(ISBLANK(H73), 0, H73),", ""badgeId"": """,IF(ISBLANK(I73), 0, I73),""", ""timeBattle"": ",J73," }, ")</f>
-        <v>73: { "eventKey": "Magic Carpet", "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>73: { "eventKey": "Magic Carpet", "locationCode": "AgrabahSand", "eventId": 0x6f, "score": 0, "isBoss": 0, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13613,7 +13613,7 @@
       </c>
       <c r="K74" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C74, """, ""locationCode"": """,B74,""", ""eventId"": 0x",A74,", ""score"": ",E74,", ""isBoss"": ",D74,", ""lv1"": ",F74,", ""isProper"": ",G74,", ""achId"": ",IF(ISBLANK(H74), 0, H74),", ""badgeId"": """,IF(ISBLANK(I74), 0, I74),""", ""timeBattle"": ",J74," }, ")</f>
-        <v>74: { "eventKey": "Data Luxord", "locationCode": "NeverDivide", "eventId": 0x65, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375966, "badgeId": "422531", "timeBattle": 1 }, </v>
+        <v>74: { "eventKey": "Data Luxord", "locationCode": "NeverDivide", "eventId": 0x65, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375966, "badgeId": "422531", "timeBattle": 1 },</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13649,7 +13649,7 @@
       </c>
       <c r="K75" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C75, """, ""locationCode"": """,B75,""", ""eventId"": 0x",A75,", ""score"": ",E75,", ""isBoss"": ",D75,", ""lv1"": ",F75,", ""isProper"": ",G75,", ""achId"": ",IF(ISBLANK(H75), 0, H75),", ""badgeId"": """,IF(ISBLANK(I75), 0, I75),""", ""timeBattle"": ",J75," }, ")</f>
-        <v>75: { "eventKey": "Data Xemnas I", "locationCode": "NeverContortion", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422533", "timeBattle": 0 }, </v>
+        <v>75: { "eventKey": "Data Xemnas I", "locationCode": "NeverContortion", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375975, "badgeId": "422533", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13685,7 +13685,7 @@
       </c>
       <c r="K76" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C76, """, ""locationCode"": """,B76,""", ""eventId"": 0x",A76,", ""score"": ",E76,", ""isBoss"": ",D76,", ""lv1"": ",F76,", ""isProper"": ",G76,", ""achId"": ",IF(ISBLANK(H76), 0, H76),", ""badgeId"": """,IF(ISBLANK(I76), 0, I76),""", ""timeBattle"": ",J76," }, ")</f>
-        <v>76: { "eventKey": "Data Xemnas II", "locationCode": "NeverFinal", "eventId": 0x62, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375976, "badgeId": "422541", "timeBattle": 0 }, </v>
+        <v>76: { "eventKey": "Data Xemnas II", "locationCode": "NeverFinal", "eventId": 0x62, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375976, "badgeId": "422541", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13721,7 +13721,7 @@
       </c>
       <c r="K77" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C77, """, ""locationCode"": """,B77,""", ""eventId"": 0x",A77,", ""score"": ",E77,", ""isBoss"": ",D77,", ""lv1"": ",F77,", ""isProper"": ",G77,", ""achId"": ",IF(ISBLANK(H77), 0, H77),", ""badgeId"": """,IF(ISBLANK(I77), 0, I77),""", ""timeBattle"": ",J77," }, ")</f>
-        <v>77: { "eventKey": "Data Xigbar", "locationCode": "NeverHall", "eventId": 0x64, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375977, "badgeId": "422542", "timeBattle": 0 }, </v>
+        <v>77: { "eventKey": "Data Xigbar", "locationCode": "NeverHall", "eventId": 0x64, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375977, "badgeId": "422542", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13757,7 +13757,7 @@
       </c>
       <c r="K78" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C78, """, ""locationCode"": """,B78,""", ""eventId"": 0x",A78,", ""score"": ",E78,", ""isBoss"": ",D78,", ""lv1"": ",F78,", ""isProper"": ",G78,", ""achId"": ",IF(ISBLANK(H78), 0, H78),", ""badgeId"": """,IF(ISBLANK(I78), 0, I78),""", ""timeBattle"": ",J78," }, ")</f>
-        <v>78: { "eventKey": "Data Xaldin", "locationCode": "BeastBridge", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375978, "badgeId": "422543", "timeBattle": 0 }, </v>
+        <v>78: { "eventKey": "Data Xaldin", "locationCode": "BeastBridge", "eventId": 0x61, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375978, "badgeId": "422543", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13793,7 +13793,7 @@
       </c>
       <c r="K79" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C79, """, ""locationCode"": """,B79,""", ""eventId"": 0x",A79,", ""score"": ",E79,", ""isBoss"": ",D79,", ""lv1"": ",F79,", ""isProper"": ",G79,", ""achId"": ",IF(ISBLANK(H79), 0, H79),", ""badgeId"": """,IF(ISBLANK(I79), 0, I79),""", ""timeBattle"": ",J79," }, ")</f>
-        <v>79: { "eventKey": "Data Vexen", "locationCode": "StationOfOblivionMansion", "eventId": 0x92, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375979, "badgeId": "422544", "timeBattle": 0 }, </v>
+        <v>79: { "eventKey": "Data Vexen", "locationCode": "StationOfOblivionMansion", "eventId": 0x92, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375979, "badgeId": "422544", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13829,7 +13829,7 @@
       </c>
       <c r="K80" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C80, """, ""locationCode"": """,B80,""", ""eventId"": 0x",A80,", ""score"": ",E80,", ""isBoss"": ",D80,", ""lv1"": ",F80,", ""isProper"": ",G80,", ""achId"": ",IF(ISBLANK(H80), 0, H80),", ""badgeId"": """,IF(ISBLANK(I80), 0, I80),""", ""timeBattle"": ",J80," }, ")</f>
-        <v>80: { "eventKey": "Data Lexaeus", "locationCode": "StationOfOblivion2", "eventId": 0x93, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375980, "badgeId": "422545", "timeBattle": 0 }, </v>
+        <v>80: { "eventKey": "Data Lexaeus", "locationCode": "StationOfOblivion2", "eventId": 0x93, "score": 25, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375980, "badgeId": "422545", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13865,7 +13865,7 @@
       </c>
       <c r="K81" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C81, """, ""locationCode"": """,B81,""", ""eventId"": 0x",A81,", ""score"": ",E81,", ""isBoss"": ",D81,", ""lv1"": ",F81,", ""isProper"": ",G81,", ""achId"": ",IF(ISBLANK(H81), 0, H81),", ""badgeId"": """,IF(ISBLANK(I81), 0, I81),""", ""timeBattle"": ",J81," }, ")</f>
-        <v>81: { "eventKey": "Data Zexion", "locationCode": "DestinyStorm", "eventId": 0x98, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375981, "badgeId": "422546", "timeBattle": 0 }, </v>
+        <v>81: { "eventKey": "Data Zexion", "locationCode": "DestinyStorm", "eventId": 0x98, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375981, "badgeId": "422546", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="K82" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C82, """, ""locationCode"": """,B82,""", ""eventId"": 0x",A82,", ""score"": ",E82,", ""isBoss"": ",D82,", ""lv1"": ",F82,", ""isProper"": ",G82,", ""achId"": ",IF(ISBLANK(H82), 0, H82),", ""badgeId"": """,IF(ISBLANK(I82), 0, I82),""", ""timeBattle"": ",J82," }, ")</f>
-        <v>82: { "eventKey": "Data Saïx", "locationCode": "NeverImpasse", "eventId": 0x66, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375982, "badgeId": "422547", "timeBattle": 0 }, </v>
+        <v>82: { "eventKey": "Data Saïx", "locationCode": "NeverImpasse", "eventId": 0x66, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375982, "badgeId": "422547", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13937,7 +13937,7 @@
       </c>
       <c r="K83" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C83, """, ""locationCode"": """,B83,""", ""eventId"": 0x",A83,", ""score"": ",E83,", ""isBoss"": ",D83,", ""lv1"": ",F83,", ""isProper"": ",G83,", ""achId"": ",IF(ISBLANK(H83), 0, H83),", ""badgeId"": """,IF(ISBLANK(I83), 0, I83),""", ""timeBattle"": ",J83," }, ")</f>
-        <v>83: { "eventKey": "Data Axel", "locationCode": "BasementHallAxel", "eventId": 0xd5, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375983, "badgeId": "422548", "timeBattle": 0 }, </v>
+        <v>83: { "eventKey": "Data Axel", "locationCode": "BasementHallAxel", "eventId": 0xd5, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375983, "badgeId": "422548", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13973,7 +13973,7 @@
       </c>
       <c r="K84" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C84, """, ""locationCode"": """,B84,""", ""eventId"": 0x",A84,", ""score"": ",E84,", ""isBoss"": ",D84,", ""lv1"": ",F84,", ""isProper"": ",G84,", ""achId"": ",IF(ISBLANK(H84), 0, H84),", ""badgeId"": """,IF(ISBLANK(I84), 0, I84),""", ""timeBattle"": ",J84," }, ")</f>
-        <v>84: { "eventKey": "Data Demyx", "locationCode": "CastleGate", "eventId": 0x72, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375984, "badgeId": "422549", "timeBattle": 0 }, </v>
+        <v>84: { "eventKey": "Data Demyx", "locationCode": "CastleGate", "eventId": 0x72, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375984, "badgeId": "422549", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14009,7 +14009,7 @@
       </c>
       <c r="K85" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C85, """, ""locationCode"": """,B85,""", ""eventId"": 0x",A85,", ""score"": ",E85,", ""isBoss"": ",D85,", ""lv1"": ",F85,", ""isProper"": ",G85,", ""achId"": ",IF(ISBLANK(H85), 0, H85),", ""badgeId"": """,IF(ISBLANK(I85), 0, I85),""", ""timeBattle"": ",J85," }, ")</f>
-        <v>85: { "eventKey": "Data Marluxia", "locationCode": "StationOfOblivion", "eventId": 0x96, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375985, "badgeId": "422550", "timeBattle": 0 }, </v>
+        <v>85: { "eventKey": "Data Marluxia", "locationCode": "StationOfOblivion", "eventId": 0x96, "score": 100, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375985, "badgeId": "422550", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14045,7 +14045,7 @@
       </c>
       <c r="K86" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C86, """, ""locationCode"": """,B86,""", ""eventId"": 0x",A86,", ""score"": ",E86,", ""isBoss"": ",D86,", ""lv1"": ",F86,", ""isProper"": ",G86,", ""achId"": ",IF(ISBLANK(H86), 0, H86),", ""badgeId"": """,IF(ISBLANK(I86), 0, I86),""", ""timeBattle"": ",J86," }, ")</f>
-        <v>86: { "eventKey": "Data Larxene", "locationCode": "StationOfOblivion2", "eventId": 0x94, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375986, "badgeId": "422551", "timeBattle": 0 }, </v>
+        <v>86: { "eventKey": "Data Larxene", "locationCode": "StationOfOblivion2", "eventId": 0x94, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375986, "badgeId": "422551", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14081,7 +14081,7 @@
       </c>
       <c r="K87" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C87, """, ""locationCode"": """,B87,""", ""eventId"": 0x",A87,", ""score"": ",E87,", ""isBoss"": ",D87,", ""lv1"": ",F87,", ""isProper"": ",G87,", ""achId"": ",IF(ISBLANK(H87), 0, H87),", ""badgeId"": """,IF(ISBLANK(I87), 0, I87),""", ""timeBattle"": ",J87," }, ")</f>
-        <v>87: { "eventKey": "Data Roxas", "locationCode": "NeverStation", "eventId": 0x63, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375987, "badgeId": "422552", "timeBattle": 0 }, </v>
+        <v>87: { "eventKey": "Data Roxas", "locationCode": "NeverStation", "eventId": 0x63, "score": 50, "isBoss": 1, "lv1": 1, "isProper": 1, "achId": 375987, "badgeId": "422552", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14111,7 +14111,7 @@
       </c>
       <c r="K88" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C88, """, ""locationCode"": """,B88,""", ""eventId"": 0x",A88,", ""score"": ",E88,", ""isBoss"": ",D88,", ""lv1"": ",F88,", ""isProper"": ",G88,", ""achId"": ",IF(ISBLANK(H88), 0, H88),", ""badgeId"": """,IF(ISBLANK(I88), 0, I88),""", ""timeBattle"": ",J88," }, ")</f>
-        <v>88: { "eventKey": "Lingering Will", "locationCode": "GraveyardBadlands", "eventId": 0x43, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>88: { "eventKey": "Lingering Will", "locationCode": "GraveyardBadlands", "eventId": 0x43, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14141,7 +14141,7 @@
       </c>
       <c r="K89" s="1" t="str">
         <f aca="false">_xlfn.CONCAT( ,ROW(),": { ""eventKey"": """,C89, """, ""locationCode"": """,B89,""", ""eventId"": 0x",A89,", ""score"": ",E89,", ""isBoss"": ",D89,", ""lv1"": ",F89,", ""isProper"": ",G89,", ""achId"": ",IF(ISBLANK(H89), 0, H89),", ""badgeId"": """,IF(ISBLANK(I89), 0, I89),""", ""timeBattle"": ",J89," }, ")</f>
-        <v>89: { "eventKey": "Lingering Will 2", "locationCode": "GraveyardBadlands", "eventId": 0x49, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 }, </v>
+        <v>89: { "eventKey": "Lingering Will 2", "locationCode": "GraveyardBadlands", "eventId": 0x49, "score": 100, "isBoss": 1, "lv1": 0, "isProper": 0, "achId": 0, "badgeId": "0", "timeBattle": 0 },</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27309,7 +27309,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BB122571-2711-4DF9-8F19-12169166EAA1}</x14:id>
+          <x14:id>{4D69BDDD-C886-40A6-A571-F4CC4F83F8D7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27323,7 +27323,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{507693FA-7A7C-4D86-AD42-101C561A6BBC}</x14:id>
+          <x14:id>{50FB76E7-315B-4438-9AE0-00C1953B4E63}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27339,7 +27339,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BB122571-2711-4DF9-8F19-12169166EAA1}">
+          <x14:cfRule type="dataBar" id="{4D69BDDD-C886-40A6-A571-F4CC4F83F8D7}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -27350,7 +27350,7 @@
           <xm:sqref>A104:A1048576 A1:A102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{507693FA-7A7C-4D86-AD42-101C561A6BBC}">
+          <x14:cfRule type="dataBar" id="{50FB76E7-315B-4438-9AE0-00C1953B4E63}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>